<commit_message>
Add box primitives demo
</commit_message>
<xml_diff>
--- a/Leetcode-tag record.xlsx
+++ b/Leetcode-tag record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiahsing/git-repositories/workspace-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96C6395-FD52-C646-97A4-CF994E6FB2FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5782D8F8-B913-0D4B-8EF9-14FB5D5CD622}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28840" yWindow="3120" windowWidth="34420" windowHeight="24460" activeTab="1" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="777">
   <si>
     <t>Array</t>
   </si>
@@ -2354,6 +2354,9 @@
   </si>
   <si>
     <t>Largest Number At Least Twice of Others</t>
+  </si>
+  <si>
+    <t>Diagonal Traverse</t>
   </si>
 </sst>
 </file>
@@ -21781,7 +21784,7 @@
   <dimension ref="B1:AV157"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23174,8 +23177,12 @@
       <c r="O20" s="5" t="s">
         <v>752</v>
       </c>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="5"/>
+      <c r="Q20" s="100">
+        <v>498</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>776</v>
+      </c>
       <c r="T20" s="3">
         <v>209</v>
       </c>

</xml_diff>

<commit_message>
Collections framework summary: add ArrayDeque, LinkedList
</commit_message>
<xml_diff>
--- a/Leetcode-tag record.xlsx
+++ b/Leetcode-tag record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiahsing/git-repositories/workspace-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D569371-D5DF-3D4E-B729-4A6C3310BA8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD00678-4D32-5E4C-992C-897E686AE746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38660" yWindow="940" windowWidth="28180" windowHeight="26640" activeTab="2" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
+    <workbookView xWindow="29680" yWindow="500" windowWidth="29000" windowHeight="26640" activeTab="2" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="844">
   <si>
     <t>Array</t>
   </si>
@@ -2378,9 +2378,6 @@
   </si>
   <si>
     <t>ArrayList</t>
-  </si>
-  <si>
-    <t>List</t>
   </si>
   <si>
     <t>LinkedList</t>
@@ -3064,17 +3061,285 @@
     <t>Inherited Methods</t>
   </si>
   <si>
-    <t>equals(Object o)</t>
-  </si>
-  <si>
     <t>toString()</t>
+  </si>
+  <si>
+    <t>empty()</t>
+  </si>
+  <si>
+    <t>pop()</t>
+  </si>
+  <si>
+    <t>search(Object o)</t>
+  </si>
+  <si>
+    <t>addLast(E e)</t>
+  </si>
+  <si>
+    <r>
+      <t>addFirst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> e)</t>
+    </r>
+  </si>
+  <si>
+    <t>getFirst()</t>
+  </si>
+  <si>
+    <t>getLast()</t>
+  </si>
+  <si>
+    <t>offer(E e)</t>
+  </si>
+  <si>
+    <r>
+      <t>offerFirst</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> e)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>offerLast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t> e)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>peek()</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Retrieves, but does not remove, the head (first element) of this list</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>peekFirst()</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Retrieves, but does not remove, the first element of this list, or returns null if this list is empty.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>peekLast()</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Retrieves, but does not remove, the last element of this list, or returns null if this list is empty</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>poll()</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - Retrieves and removes the head (first element) of this list.</t>
+    </r>
+  </si>
+  <si>
+    <t>pollFirst()</t>
+  </si>
+  <si>
+    <t>pollLast()</t>
+  </si>
+  <si>
+    <r>
+      <t>push</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> e)</t>
+    </r>
+  </si>
+  <si>
+    <t>removeFirst()</t>
+  </si>
+  <si>
+    <t>removeLast()</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">equals(Object o) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Compares the specified object with this list for equality. Returns true if and only if the specified object is also a list, both lists have the same size, and all corresponding pairs of elements in the two lists are equal. </t>
+    </r>
+  </si>
+  <si>
+    <t>ArrayDeque</t>
+  </si>
+  <si>
+    <r>
+      <t>Queue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> - interface</t>
+    </r>
+  </si>
+  <si>
+    <t>remove() - the head</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>- interface</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3187,6 +3452,37 @@
       <color theme="1"/>
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="50">
@@ -3485,7 +3781,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -3987,6 +4283,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4293,41 +4600,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="41" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="43" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="43" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="43" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="42" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="44" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4346,7 +4627,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4475,6 +4755,39 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="49" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4827,27 +5140,27 @@
   <sheetData>
     <row r="1" spans="2:21" ht="17" thickBot="1"/>
     <row r="2" spans="2:21" ht="17" thickBot="1">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="185" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="112"/>
-      <c r="R2" s="116"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="116"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
+      <c r="J2" s="186"/>
+      <c r="K2" s="186"/>
+      <c r="L2" s="186"/>
+      <c r="M2" s="186"/>
+      <c r="N2" s="186"/>
+      <c r="O2" s="186"/>
+      <c r="P2" s="187"/>
+      <c r="R2" s="184"/>
+      <c r="S2" s="184"/>
+      <c r="T2" s="184"/>
+      <c r="U2" s="184"/>
     </row>
     <row r="3" spans="2:21" ht="17" thickBot="1">
       <c r="B3" s="25" t="s">
@@ -5219,8 +5532,8 @@
       <c r="N15" s="42"/>
       <c r="O15" s="15"/>
       <c r="P15" s="17"/>
-      <c r="R15" s="116"/>
-      <c r="S15" s="116"/>
+      <c r="R15" s="184"/>
+      <c r="S15" s="184"/>
       <c r="T15" s="102"/>
       <c r="U15" s="102"/>
     </row>
@@ -7198,23 +7511,23 @@
       <c r="P98" s="45"/>
     </row>
     <row r="99" spans="2:16" ht="17" thickBot="1">
-      <c r="B99" s="110" t="s">
+      <c r="B99" s="185" t="s">
         <v>101</v>
       </c>
-      <c r="C99" s="111"/>
-      <c r="D99" s="111"/>
-      <c r="E99" s="111"/>
-      <c r="F99" s="111"/>
-      <c r="G99" s="111"/>
-      <c r="H99" s="111"/>
-      <c r="I99" s="111"/>
-      <c r="J99" s="111"/>
-      <c r="K99" s="111"/>
-      <c r="L99" s="111"/>
-      <c r="M99" s="111"/>
-      <c r="N99" s="111"/>
-      <c r="O99" s="111"/>
-      <c r="P99" s="112"/>
+      <c r="C99" s="186"/>
+      <c r="D99" s="186"/>
+      <c r="E99" s="186"/>
+      <c r="F99" s="186"/>
+      <c r="G99" s="186"/>
+      <c r="H99" s="186"/>
+      <c r="I99" s="186"/>
+      <c r="J99" s="186"/>
+      <c r="K99" s="186"/>
+      <c r="L99" s="186"/>
+      <c r="M99" s="186"/>
+      <c r="N99" s="186"/>
+      <c r="O99" s="186"/>
+      <c r="P99" s="187"/>
     </row>
     <row r="100" spans="2:16" ht="17" thickBot="1">
       <c r="B100" s="25" t="s">
@@ -9628,23 +9941,23 @@
       <c r="P208" s="45"/>
     </row>
     <row r="209" spans="2:16" ht="17" thickBot="1">
-      <c r="B209" s="110" t="s">
+      <c r="B209" s="185" t="s">
         <v>166</v>
       </c>
-      <c r="C209" s="111"/>
-      <c r="D209" s="111"/>
-      <c r="E209" s="111"/>
-      <c r="F209" s="111"/>
-      <c r="G209" s="111"/>
-      <c r="H209" s="111"/>
-      <c r="I209" s="111"/>
-      <c r="J209" s="111"/>
-      <c r="K209" s="111"/>
-      <c r="L209" s="111"/>
-      <c r="M209" s="111"/>
-      <c r="N209" s="111"/>
-      <c r="O209" s="111"/>
-      <c r="P209" s="112"/>
+      <c r="C209" s="186"/>
+      <c r="D209" s="186"/>
+      <c r="E209" s="186"/>
+      <c r="F209" s="186"/>
+      <c r="G209" s="186"/>
+      <c r="H209" s="186"/>
+      <c r="I209" s="186"/>
+      <c r="J209" s="186"/>
+      <c r="K209" s="186"/>
+      <c r="L209" s="186"/>
+      <c r="M209" s="186"/>
+      <c r="N209" s="186"/>
+      <c r="O209" s="186"/>
+      <c r="P209" s="187"/>
     </row>
     <row r="210" spans="2:16" ht="17" thickBot="1">
       <c r="B210" s="25" t="s">
@@ -11125,23 +11438,23 @@
       <c r="P273" s="45"/>
     </row>
     <row r="274" spans="2:16" ht="17" thickBot="1">
-      <c r="B274" s="110" t="s">
+      <c r="B274" s="185" t="s">
         <v>43</v>
       </c>
-      <c r="C274" s="111"/>
-      <c r="D274" s="111"/>
-      <c r="E274" s="111"/>
-      <c r="F274" s="111"/>
-      <c r="G274" s="111"/>
-      <c r="H274" s="111"/>
-      <c r="I274" s="111"/>
-      <c r="J274" s="111"/>
-      <c r="K274" s="111"/>
-      <c r="L274" s="111"/>
-      <c r="M274" s="111"/>
-      <c r="N274" s="111"/>
-      <c r="O274" s="111"/>
-      <c r="P274" s="112"/>
+      <c r="C274" s="186"/>
+      <c r="D274" s="186"/>
+      <c r="E274" s="186"/>
+      <c r="F274" s="186"/>
+      <c r="G274" s="186"/>
+      <c r="H274" s="186"/>
+      <c r="I274" s="186"/>
+      <c r="J274" s="186"/>
+      <c r="K274" s="186"/>
+      <c r="L274" s="186"/>
+      <c r="M274" s="186"/>
+      <c r="N274" s="186"/>
+      <c r="O274" s="186"/>
+      <c r="P274" s="187"/>
     </row>
     <row r="275" spans="2:16" ht="17" thickBot="1">
       <c r="B275" s="25" t="s">
@@ -13169,23 +13482,23 @@
       <c r="P363" s="45"/>
     </row>
     <row r="364" spans="2:16" ht="17" thickBot="1">
-      <c r="B364" s="110" t="s">
+      <c r="B364" s="185" t="s">
         <v>255</v>
       </c>
-      <c r="C364" s="111"/>
-      <c r="D364" s="111"/>
-      <c r="E364" s="111"/>
-      <c r="F364" s="111"/>
-      <c r="G364" s="111"/>
-      <c r="H364" s="111"/>
-      <c r="I364" s="111"/>
-      <c r="J364" s="111"/>
-      <c r="K364" s="111"/>
-      <c r="L364" s="111"/>
-      <c r="M364" s="111"/>
-      <c r="N364" s="111"/>
-      <c r="O364" s="111"/>
-      <c r="P364" s="112"/>
+      <c r="C364" s="186"/>
+      <c r="D364" s="186"/>
+      <c r="E364" s="186"/>
+      <c r="F364" s="186"/>
+      <c r="G364" s="186"/>
+      <c r="H364" s="186"/>
+      <c r="I364" s="186"/>
+      <c r="J364" s="186"/>
+      <c r="K364" s="186"/>
+      <c r="L364" s="186"/>
+      <c r="M364" s="186"/>
+      <c r="N364" s="186"/>
+      <c r="O364" s="186"/>
+      <c r="P364" s="187"/>
     </row>
     <row r="365" spans="2:16" ht="17" thickBot="1">
       <c r="B365" s="25" t="s">
@@ -14063,23 +14376,23 @@
       <c r="P401" s="45"/>
     </row>
     <row r="402" spans="2:16" ht="17" thickBot="1">
-      <c r="B402" s="110" t="s">
+      <c r="B402" s="185" t="s">
         <v>42</v>
       </c>
-      <c r="C402" s="111"/>
-      <c r="D402" s="111"/>
-      <c r="E402" s="111"/>
-      <c r="F402" s="111"/>
-      <c r="G402" s="111"/>
-      <c r="H402" s="111"/>
-      <c r="I402" s="111"/>
-      <c r="J402" s="111"/>
-      <c r="K402" s="111"/>
-      <c r="L402" s="111"/>
-      <c r="M402" s="111"/>
-      <c r="N402" s="111"/>
-      <c r="O402" s="111"/>
-      <c r="P402" s="112"/>
+      <c r="C402" s="186"/>
+      <c r="D402" s="186"/>
+      <c r="E402" s="186"/>
+      <c r="F402" s="186"/>
+      <c r="G402" s="186"/>
+      <c r="H402" s="186"/>
+      <c r="I402" s="186"/>
+      <c r="J402" s="186"/>
+      <c r="K402" s="186"/>
+      <c r="L402" s="186"/>
+      <c r="M402" s="186"/>
+      <c r="N402" s="186"/>
+      <c r="O402" s="186"/>
+      <c r="P402" s="187"/>
     </row>
     <row r="403" spans="2:16" ht="17" thickBot="1">
       <c r="B403" s="25" t="s">
@@ -14935,23 +15248,23 @@
       <c r="P439" s="45"/>
     </row>
     <row r="440" spans="2:16" ht="17" thickBot="1">
-      <c r="B440" s="110" t="s">
+      <c r="B440" s="185" t="s">
         <v>300</v>
       </c>
-      <c r="C440" s="111"/>
-      <c r="D440" s="111"/>
-      <c r="E440" s="111"/>
-      <c r="F440" s="111"/>
-      <c r="G440" s="111"/>
-      <c r="H440" s="111"/>
-      <c r="I440" s="111"/>
-      <c r="J440" s="111"/>
-      <c r="K440" s="111"/>
-      <c r="L440" s="111"/>
-      <c r="M440" s="111"/>
-      <c r="N440" s="111"/>
-      <c r="O440" s="111"/>
-      <c r="P440" s="112"/>
+      <c r="C440" s="186"/>
+      <c r="D440" s="186"/>
+      <c r="E440" s="186"/>
+      <c r="F440" s="186"/>
+      <c r="G440" s="186"/>
+      <c r="H440" s="186"/>
+      <c r="I440" s="186"/>
+      <c r="J440" s="186"/>
+      <c r="K440" s="186"/>
+      <c r="L440" s="186"/>
+      <c r="M440" s="186"/>
+      <c r="N440" s="186"/>
+      <c r="O440" s="186"/>
+      <c r="P440" s="187"/>
     </row>
     <row r="441" spans="2:16" ht="17" thickBot="1">
       <c r="B441" s="25" t="s">
@@ -15844,23 +16157,23 @@
       <c r="P478" s="45"/>
     </row>
     <row r="479" spans="2:16" ht="17" thickBot="1">
-      <c r="B479" s="110" t="s">
+      <c r="B479" s="185" t="s">
         <v>59</v>
       </c>
-      <c r="C479" s="111"/>
-      <c r="D479" s="111"/>
-      <c r="E479" s="111"/>
-      <c r="F479" s="111"/>
-      <c r="G479" s="111"/>
-      <c r="H479" s="111"/>
-      <c r="I479" s="111"/>
-      <c r="J479" s="111"/>
-      <c r="K479" s="111"/>
-      <c r="L479" s="111"/>
-      <c r="M479" s="111"/>
-      <c r="N479" s="111"/>
-      <c r="O479" s="111"/>
-      <c r="P479" s="112"/>
+      <c r="C479" s="186"/>
+      <c r="D479" s="186"/>
+      <c r="E479" s="186"/>
+      <c r="F479" s="186"/>
+      <c r="G479" s="186"/>
+      <c r="H479" s="186"/>
+      <c r="I479" s="186"/>
+      <c r="J479" s="186"/>
+      <c r="K479" s="186"/>
+      <c r="L479" s="186"/>
+      <c r="M479" s="186"/>
+      <c r="N479" s="186"/>
+      <c r="O479" s="186"/>
+      <c r="P479" s="187"/>
     </row>
     <row r="480" spans="2:16" ht="17" thickBot="1">
       <c r="B480" s="25" t="s">
@@ -16555,23 +16868,23 @@
       <c r="P505" s="45"/>
     </row>
     <row r="506" spans="2:16" ht="17" thickBot="1">
-      <c r="B506" s="110" t="s">
+      <c r="B506" s="185" t="s">
         <v>324</v>
       </c>
-      <c r="C506" s="111"/>
-      <c r="D506" s="111"/>
-      <c r="E506" s="111"/>
-      <c r="F506" s="111"/>
-      <c r="G506" s="111"/>
-      <c r="H506" s="111"/>
-      <c r="I506" s="111"/>
-      <c r="J506" s="111"/>
-      <c r="K506" s="111"/>
-      <c r="L506" s="111"/>
-      <c r="M506" s="111"/>
-      <c r="N506" s="111"/>
-      <c r="O506" s="111"/>
-      <c r="P506" s="112"/>
+      <c r="C506" s="186"/>
+      <c r="D506" s="186"/>
+      <c r="E506" s="186"/>
+      <c r="F506" s="186"/>
+      <c r="G506" s="186"/>
+      <c r="H506" s="186"/>
+      <c r="I506" s="186"/>
+      <c r="J506" s="186"/>
+      <c r="K506" s="186"/>
+      <c r="L506" s="186"/>
+      <c r="M506" s="186"/>
+      <c r="N506" s="186"/>
+      <c r="O506" s="186"/>
+      <c r="P506" s="187"/>
     </row>
     <row r="507" spans="2:16" ht="17" thickBot="1">
       <c r="B507" s="25" t="s">
@@ -17274,23 +17587,23 @@
       <c r="P538" s="45"/>
     </row>
     <row r="539" spans="2:16" ht="17" thickBot="1">
-      <c r="B539" s="110" t="s">
+      <c r="B539" s="185" t="s">
         <v>352</v>
       </c>
-      <c r="C539" s="111"/>
-      <c r="D539" s="111"/>
-      <c r="E539" s="111"/>
-      <c r="F539" s="111"/>
-      <c r="G539" s="111"/>
-      <c r="H539" s="111"/>
-      <c r="I539" s="111"/>
-      <c r="J539" s="111"/>
-      <c r="K539" s="111"/>
-      <c r="L539" s="111"/>
-      <c r="M539" s="111"/>
-      <c r="N539" s="111"/>
-      <c r="O539" s="111"/>
-      <c r="P539" s="112"/>
+      <c r="C539" s="186"/>
+      <c r="D539" s="186"/>
+      <c r="E539" s="186"/>
+      <c r="F539" s="186"/>
+      <c r="G539" s="186"/>
+      <c r="H539" s="186"/>
+      <c r="I539" s="186"/>
+      <c r="J539" s="186"/>
+      <c r="K539" s="186"/>
+      <c r="L539" s="186"/>
+      <c r="M539" s="186"/>
+      <c r="N539" s="186"/>
+      <c r="O539" s="186"/>
+      <c r="P539" s="187"/>
     </row>
     <row r="540" spans="2:16" ht="17" thickBot="1">
       <c r="B540" s="25" t="s">
@@ -18098,23 +18411,23 @@
       <c r="P576" s="45"/>
     </row>
     <row r="577" spans="2:16" ht="17" thickBot="1">
-      <c r="B577" s="110" t="s">
+      <c r="B577" s="185" t="s">
         <v>342</v>
       </c>
-      <c r="C577" s="111"/>
-      <c r="D577" s="111"/>
-      <c r="E577" s="111"/>
-      <c r="F577" s="111"/>
-      <c r="G577" s="111"/>
-      <c r="H577" s="111"/>
-      <c r="I577" s="111"/>
-      <c r="J577" s="111"/>
-      <c r="K577" s="111"/>
-      <c r="L577" s="111"/>
-      <c r="M577" s="111"/>
-      <c r="N577" s="111"/>
-      <c r="O577" s="111"/>
-      <c r="P577" s="112"/>
+      <c r="C577" s="186"/>
+      <c r="D577" s="186"/>
+      <c r="E577" s="186"/>
+      <c r="F577" s="186"/>
+      <c r="G577" s="186"/>
+      <c r="H577" s="186"/>
+      <c r="I577" s="186"/>
+      <c r="J577" s="186"/>
+      <c r="K577" s="186"/>
+      <c r="L577" s="186"/>
+      <c r="M577" s="186"/>
+      <c r="N577" s="186"/>
+      <c r="O577" s="186"/>
+      <c r="P577" s="187"/>
     </row>
     <row r="578" spans="2:16" ht="17" thickBot="1">
       <c r="B578" s="25" t="s">
@@ -18615,23 +18928,23 @@
       <c r="P599" s="45"/>
     </row>
     <row r="600" spans="2:16" ht="17" thickBot="1">
-      <c r="B600" s="110" t="s">
+      <c r="B600" s="185" t="s">
         <v>373</v>
       </c>
-      <c r="C600" s="111"/>
-      <c r="D600" s="111"/>
-      <c r="E600" s="111"/>
-      <c r="F600" s="111"/>
-      <c r="G600" s="111"/>
-      <c r="H600" s="111"/>
-      <c r="I600" s="111"/>
-      <c r="J600" s="111"/>
-      <c r="K600" s="111"/>
-      <c r="L600" s="111"/>
-      <c r="M600" s="111"/>
-      <c r="N600" s="111"/>
-      <c r="O600" s="111"/>
-      <c r="P600" s="112"/>
+      <c r="C600" s="186"/>
+      <c r="D600" s="186"/>
+      <c r="E600" s="186"/>
+      <c r="F600" s="186"/>
+      <c r="G600" s="186"/>
+      <c r="H600" s="186"/>
+      <c r="I600" s="186"/>
+      <c r="J600" s="186"/>
+      <c r="K600" s="186"/>
+      <c r="L600" s="186"/>
+      <c r="M600" s="186"/>
+      <c r="N600" s="186"/>
+      <c r="O600" s="186"/>
+      <c r="P600" s="187"/>
     </row>
     <row r="601" spans="2:16" ht="17" thickBot="1">
       <c r="B601" s="25" t="s">
@@ -19368,23 +19681,23 @@
       <c r="P636" s="45"/>
     </row>
     <row r="637" spans="2:16" ht="17" thickBot="1">
-      <c r="B637" s="110" t="s">
+      <c r="B637" s="185" t="s">
         <v>387</v>
       </c>
-      <c r="C637" s="111"/>
-      <c r="D637" s="111"/>
-      <c r="E637" s="111"/>
-      <c r="F637" s="111"/>
-      <c r="G637" s="111"/>
-      <c r="H637" s="111"/>
-      <c r="I637" s="111"/>
-      <c r="J637" s="111"/>
-      <c r="K637" s="111"/>
-      <c r="L637" s="111"/>
-      <c r="M637" s="111"/>
-      <c r="N637" s="111"/>
-      <c r="O637" s="111"/>
-      <c r="P637" s="112"/>
+      <c r="C637" s="186"/>
+      <c r="D637" s="186"/>
+      <c r="E637" s="186"/>
+      <c r="F637" s="186"/>
+      <c r="G637" s="186"/>
+      <c r="H637" s="186"/>
+      <c r="I637" s="186"/>
+      <c r="J637" s="186"/>
+      <c r="K637" s="186"/>
+      <c r="L637" s="186"/>
+      <c r="M637" s="186"/>
+      <c r="N637" s="186"/>
+      <c r="O637" s="186"/>
+      <c r="P637" s="187"/>
     </row>
     <row r="638" spans="2:16" ht="17" thickBot="1">
       <c r="B638" s="25" t="s">
@@ -19638,23 +19951,23 @@
       <c r="P648" s="45"/>
     </row>
     <row r="649" spans="2:16" ht="17" thickBot="1">
-      <c r="B649" s="110" t="s">
+      <c r="B649" s="185" t="s">
         <v>391</v>
       </c>
-      <c r="C649" s="111"/>
-      <c r="D649" s="111"/>
-      <c r="E649" s="111"/>
-      <c r="F649" s="111"/>
-      <c r="G649" s="111"/>
-      <c r="H649" s="111"/>
-      <c r="I649" s="111"/>
-      <c r="J649" s="111"/>
-      <c r="K649" s="111"/>
-      <c r="L649" s="111"/>
-      <c r="M649" s="111"/>
-      <c r="N649" s="111"/>
-      <c r="O649" s="111"/>
-      <c r="P649" s="112"/>
+      <c r="C649" s="186"/>
+      <c r="D649" s="186"/>
+      <c r="E649" s="186"/>
+      <c r="F649" s="186"/>
+      <c r="G649" s="186"/>
+      <c r="H649" s="186"/>
+      <c r="I649" s="186"/>
+      <c r="J649" s="186"/>
+      <c r="K649" s="186"/>
+      <c r="L649" s="186"/>
+      <c r="M649" s="186"/>
+      <c r="N649" s="186"/>
+      <c r="O649" s="186"/>
+      <c r="P649" s="187"/>
     </row>
     <row r="650" spans="2:16" ht="17" thickBot="1">
       <c r="B650" s="25" t="s">
@@ -20156,23 +20469,23 @@
       <c r="P674" s="45"/>
     </row>
     <row r="675" spans="2:16" ht="17" thickBot="1">
-      <c r="B675" s="113" t="s">
+      <c r="B675" s="181" t="s">
         <v>398</v>
       </c>
-      <c r="C675" s="114"/>
-      <c r="D675" s="114"/>
-      <c r="E675" s="114"/>
-      <c r="F675" s="114"/>
-      <c r="G675" s="114"/>
-      <c r="H675" s="114"/>
-      <c r="I675" s="114"/>
-      <c r="J675" s="114"/>
-      <c r="K675" s="114"/>
-      <c r="L675" s="114"/>
-      <c r="M675" s="114"/>
-      <c r="N675" s="114"/>
-      <c r="O675" s="114"/>
-      <c r="P675" s="115"/>
+      <c r="C675" s="182"/>
+      <c r="D675" s="182"/>
+      <c r="E675" s="182"/>
+      <c r="F675" s="182"/>
+      <c r="G675" s="182"/>
+      <c r="H675" s="182"/>
+      <c r="I675" s="182"/>
+      <c r="J675" s="182"/>
+      <c r="K675" s="182"/>
+      <c r="L675" s="182"/>
+      <c r="M675" s="182"/>
+      <c r="N675" s="182"/>
+      <c r="O675" s="182"/>
+      <c r="P675" s="183"/>
     </row>
     <row r="676" spans="2:16" ht="17" thickBot="1">
       <c r="B676" s="49" t="s">
@@ -20741,23 +21054,23 @@
       <c r="P703" s="45"/>
     </row>
     <row r="704" spans="2:16" ht="17" thickBot="1">
-      <c r="B704" s="113" t="s">
+      <c r="B704" s="181" t="s">
         <v>408</v>
       </c>
-      <c r="C704" s="114"/>
-      <c r="D704" s="114"/>
-      <c r="E704" s="114"/>
-      <c r="F704" s="114"/>
-      <c r="G704" s="114"/>
-      <c r="H704" s="114"/>
-      <c r="I704" s="114"/>
-      <c r="J704" s="114"/>
-      <c r="K704" s="114"/>
-      <c r="L704" s="114"/>
-      <c r="M704" s="114"/>
-      <c r="N704" s="114"/>
-      <c r="O704" s="114"/>
-      <c r="P704" s="115"/>
+      <c r="C704" s="182"/>
+      <c r="D704" s="182"/>
+      <c r="E704" s="182"/>
+      <c r="F704" s="182"/>
+      <c r="G704" s="182"/>
+      <c r="H704" s="182"/>
+      <c r="I704" s="182"/>
+      <c r="J704" s="182"/>
+      <c r="K704" s="182"/>
+      <c r="L704" s="182"/>
+      <c r="M704" s="182"/>
+      <c r="N704" s="182"/>
+      <c r="O704" s="182"/>
+      <c r="P704" s="183"/>
     </row>
     <row r="705" spans="2:16" ht="17" thickBot="1">
       <c r="B705" s="49" t="s">
@@ -21090,23 +21403,23 @@
       <c r="P720" s="45"/>
     </row>
     <row r="721" spans="2:16" ht="17" thickBot="1">
-      <c r="B721" s="113" t="s">
+      <c r="B721" s="181" t="s">
         <v>412</v>
       </c>
-      <c r="C721" s="114"/>
-      <c r="D721" s="114"/>
-      <c r="E721" s="114"/>
-      <c r="F721" s="114"/>
-      <c r="G721" s="114"/>
-      <c r="H721" s="114"/>
-      <c r="I721" s="114"/>
-      <c r="J721" s="114"/>
-      <c r="K721" s="114"/>
-      <c r="L721" s="114"/>
-      <c r="M721" s="114"/>
-      <c r="N721" s="114"/>
-      <c r="O721" s="114"/>
-      <c r="P721" s="115"/>
+      <c r="C721" s="182"/>
+      <c r="D721" s="182"/>
+      <c r="E721" s="182"/>
+      <c r="F721" s="182"/>
+      <c r="G721" s="182"/>
+      <c r="H721" s="182"/>
+      <c r="I721" s="182"/>
+      <c r="J721" s="182"/>
+      <c r="K721" s="182"/>
+      <c r="L721" s="182"/>
+      <c r="M721" s="182"/>
+      <c r="N721" s="182"/>
+      <c r="O721" s="182"/>
+      <c r="P721" s="183"/>
     </row>
     <row r="722" spans="2:16" ht="17" thickBot="1">
       <c r="B722" s="49" t="s">
@@ -21482,23 +21795,23 @@
       <c r="P740" s="45"/>
     </row>
     <row r="741" spans="2:16" ht="17" thickBot="1">
-      <c r="B741" s="113" t="s">
+      <c r="B741" s="181" t="s">
         <v>416</v>
       </c>
-      <c r="C741" s="114"/>
-      <c r="D741" s="114"/>
-      <c r="E741" s="114"/>
-      <c r="F741" s="114"/>
-      <c r="G741" s="114"/>
-      <c r="H741" s="114"/>
-      <c r="I741" s="114"/>
-      <c r="J741" s="114"/>
-      <c r="K741" s="114"/>
-      <c r="L741" s="114"/>
-      <c r="M741" s="114"/>
-      <c r="N741" s="114"/>
-      <c r="O741" s="114"/>
-      <c r="P741" s="115"/>
+      <c r="C741" s="182"/>
+      <c r="D741" s="182"/>
+      <c r="E741" s="182"/>
+      <c r="F741" s="182"/>
+      <c r="G741" s="182"/>
+      <c r="H741" s="182"/>
+      <c r="I741" s="182"/>
+      <c r="J741" s="182"/>
+      <c r="K741" s="182"/>
+      <c r="L741" s="182"/>
+      <c r="M741" s="182"/>
+      <c r="N741" s="182"/>
+      <c r="O741" s="182"/>
+      <c r="P741" s="183"/>
     </row>
     <row r="742" spans="2:16" ht="17" thickBot="1">
       <c r="B742" s="49" t="s">
@@ -22325,23 +22638,23 @@
       <c r="P781" s="45"/>
     </row>
     <row r="782" spans="2:16" ht="17" thickBot="1">
-      <c r="B782" s="113" t="s">
+      <c r="B782" s="181" t="s">
         <v>564</v>
       </c>
-      <c r="C782" s="114"/>
-      <c r="D782" s="114"/>
-      <c r="E782" s="114"/>
-      <c r="F782" s="114"/>
-      <c r="G782" s="114"/>
-      <c r="H782" s="114"/>
-      <c r="I782" s="114"/>
-      <c r="J782" s="114"/>
-      <c r="K782" s="114"/>
-      <c r="L782" s="114"/>
-      <c r="M782" s="114"/>
-      <c r="N782" s="114"/>
-      <c r="O782" s="114"/>
-      <c r="P782" s="115"/>
+      <c r="C782" s="182"/>
+      <c r="D782" s="182"/>
+      <c r="E782" s="182"/>
+      <c r="F782" s="182"/>
+      <c r="G782" s="182"/>
+      <c r="H782" s="182"/>
+      <c r="I782" s="182"/>
+      <c r="J782" s="182"/>
+      <c r="K782" s="182"/>
+      <c r="L782" s="182"/>
+      <c r="M782" s="182"/>
+      <c r="N782" s="182"/>
+      <c r="O782" s="182"/>
+      <c r="P782" s="183"/>
     </row>
     <row r="783" spans="2:16" ht="17" thickBot="1">
       <c r="B783" s="49" t="s">
@@ -22557,6 +22870,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B649:P649"/>
+    <mergeCell ref="B506:P506"/>
+    <mergeCell ref="B539:P539"/>
+    <mergeCell ref="B577:P577"/>
+    <mergeCell ref="B600:P600"/>
+    <mergeCell ref="B637:P637"/>
     <mergeCell ref="B782:P782"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
@@ -22573,12 +22892,6 @@
     <mergeCell ref="B704:P704"/>
     <mergeCell ref="B721:P721"/>
     <mergeCell ref="B741:P741"/>
-    <mergeCell ref="B649:P649"/>
-    <mergeCell ref="B506:P506"/>
-    <mergeCell ref="B539:P539"/>
-    <mergeCell ref="B577:P577"/>
-    <mergeCell ref="B600:P600"/>
-    <mergeCell ref="B637:P637"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="https://leetcode.com/problems/remove-element/" xr:uid="{0C08439D-F97A-154E-B763-1F7C1F321813}"/>
@@ -26954,15 +27267,15 @@
       <c r="X87" s="98"/>
       <c r="Y87" s="98"/>
       <c r="Z87" s="98"/>
-      <c r="AA87" s="117"/>
-      <c r="AB87" s="117"/>
-      <c r="AC87" s="117"/>
-      <c r="AD87" s="117"/>
-      <c r="AE87" s="117"/>
-      <c r="AF87" s="117"/>
-      <c r="AG87" s="117"/>
-      <c r="AH87" s="117"/>
-      <c r="AI87" s="117"/>
+      <c r="AA87" s="188"/>
+      <c r="AB87" s="188"/>
+      <c r="AC87" s="188"/>
+      <c r="AD87" s="188"/>
+      <c r="AE87" s="188"/>
+      <c r="AF87" s="188"/>
+      <c r="AG87" s="188"/>
+      <c r="AH87" s="188"/>
+      <c r="AI87" s="188"/>
       <c r="AJ87" s="105"/>
     </row>
     <row r="88" spans="2:36" ht="17" thickBot="1">
@@ -30028,1010 +30341,1794 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C48959B-82B5-DA45-8B96-25DF2B5B4CD9}">
-  <dimension ref="C9:K85"/>
+  <dimension ref="C9:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="65.33203125" customWidth="1"/>
-    <col min="4" max="8" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="84" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:11" ht="17" thickBot="1"/>
-    <row r="10" spans="3:11" ht="20" thickBot="1">
-      <c r="C10" s="140"/>
-      <c r="D10" s="189" t="s">
+    <row r="9" spans="3:14" ht="17" thickBot="1"/>
+    <row r="10" spans="3:14" ht="20" thickBot="1">
+      <c r="C10" s="129"/>
+      <c r="D10" s="178" t="s">
+        <v>843</v>
+      </c>
+      <c r="E10" s="179" t="s">
+        <v>779</v>
+      </c>
+      <c r="F10" s="178" t="s">
         <v>780</v>
       </c>
-      <c r="E10" s="190" t="s">
-        <v>779</v>
-      </c>
-      <c r="F10" s="189" t="s">
+      <c r="G10" s="178" t="s">
+        <v>353</v>
+      </c>
+      <c r="H10" s="178" t="s">
+        <v>841</v>
+      </c>
+      <c r="I10" s="178" t="s">
+        <v>840</v>
+      </c>
+      <c r="J10" s="178" t="s">
+        <v>365</v>
+      </c>
+      <c r="K10" s="178" t="s">
         <v>781</v>
       </c>
-      <c r="G10" s="189" t="s">
-        <v>353</v>
-      </c>
-      <c r="H10" s="189" t="s">
+      <c r="L10" s="178" t="s">
+        <v>783</v>
+      </c>
+      <c r="M10" s="178" t="s">
         <v>782</v>
       </c>
-      <c r="I10" s="189" t="s">
+      <c r="N10" s="180" t="s">
         <v>784</v>
       </c>
-      <c r="J10" s="189" t="s">
-        <v>783</v>
-      </c>
-      <c r="K10" s="191" t="s">
+    </row>
+    <row r="11" spans="3:14" ht="18">
+      <c r="C11" s="111" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" ht="18">
-      <c r="C11" s="119" t="s">
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="111"/>
+    </row>
+    <row r="12" spans="3:14" ht="18">
+      <c r="C12" s="112" t="s">
+        <v>789</v>
+      </c>
+      <c r="D12" s="137"/>
+      <c r="E12" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="F12" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G12" s="137"/>
+      <c r="H12" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="I12" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J12" s="137"/>
+      <c r="K12" s="137"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="137"/>
+      <c r="N12" s="137"/>
+    </row>
+    <row r="13" spans="3:14" ht="18">
+      <c r="C13" s="112" t="s">
+        <v>790</v>
+      </c>
+      <c r="D13" s="137"/>
+      <c r="E13" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="F13" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G13" s="137"/>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="137"/>
+      <c r="N13" s="137"/>
+    </row>
+    <row r="14" spans="3:14" ht="18">
+      <c r="C14" s="112" t="s">
+        <v>791</v>
+      </c>
+      <c r="D14" s="137"/>
+      <c r="E14" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="F14" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G14" s="137"/>
+      <c r="H14" s="137"/>
+      <c r="I14" s="137"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="137"/>
+      <c r="L14" s="137"/>
+      <c r="M14" s="137"/>
+      <c r="N14" s="137"/>
+    </row>
+    <row r="15" spans="3:14" ht="18">
+      <c r="C15" s="112" t="s">
+        <v>792</v>
+      </c>
+      <c r="D15" s="137"/>
+      <c r="E15" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="F15" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G15" s="137"/>
+      <c r="H15" s="137"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="137"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="137"/>
+      <c r="N15" s="137"/>
+    </row>
+    <row r="16" spans="3:14" ht="18">
+      <c r="C16" s="112" t="s">
+        <v>824</v>
+      </c>
+      <c r="D16" s="137"/>
+      <c r="E16" s="137"/>
+      <c r="F16" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G16" s="137"/>
+      <c r="H16" s="137"/>
+      <c r="I16" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J16" s="137"/>
+      <c r="K16" s="137"/>
+      <c r="L16" s="137"/>
+      <c r="M16" s="137"/>
+      <c r="N16" s="137"/>
+    </row>
+    <row r="17" spans="3:14" ht="18">
+      <c r="C17" s="112" t="s">
+        <v>823</v>
+      </c>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G17" s="137"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J17" s="137"/>
+      <c r="K17" s="137"/>
+      <c r="L17" s="137"/>
+      <c r="M17" s="137"/>
+      <c r="N17" s="137"/>
+    </row>
+    <row r="18" spans="3:14" ht="18">
+      <c r="C18" s="112" t="s">
+        <v>827</v>
+      </c>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G18" s="137"/>
+      <c r="H18" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="I18" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J18" s="137"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="137"/>
+      <c r="N18" s="137"/>
+    </row>
+    <row r="19" spans="3:14" ht="18">
+      <c r="C19" s="112" t="s">
+        <v>828</v>
+      </c>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G19" s="137"/>
+      <c r="H19" s="137"/>
+      <c r="I19" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J19" s="137"/>
+      <c r="K19" s="137"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="137"/>
+      <c r="N19" s="137"/>
+    </row>
+    <row r="20" spans="3:14" ht="18">
+      <c r="C20" s="112" t="s">
+        <v>829</v>
+      </c>
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G20" s="137"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J20" s="137"/>
+      <c r="K20" s="137"/>
+      <c r="L20" s="137"/>
+      <c r="M20" s="137"/>
+      <c r="N20" s="137"/>
+    </row>
+    <row r="21" spans="3:14" ht="19">
+      <c r="C21" s="112" t="s">
+        <v>836</v>
+      </c>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="G21" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="H21" s="137"/>
+      <c r="I21" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="J21" s="137"/>
+      <c r="K21" s="137"/>
+      <c r="L21" s="137"/>
+      <c r="M21" s="137"/>
+      <c r="N21" s="137"/>
+    </row>
+    <row r="22" spans="3:14" ht="18">
+      <c r="C22" s="112"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="137"/>
+      <c r="H22" s="137"/>
+      <c r="I22" s="137"/>
+      <c r="J22" s="137"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="137"/>
+      <c r="M22" s="137"/>
+      <c r="N22" s="137"/>
+    </row>
+    <row r="23" spans="3:14" ht="18">
+      <c r="C23" s="112"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="137"/>
+      <c r="G23" s="137"/>
+      <c r="H23" s="137"/>
+      <c r="I23" s="137"/>
+      <c r="J23" s="137"/>
+      <c r="K23" s="137"/>
+      <c r="L23" s="137"/>
+      <c r="M23" s="137"/>
+      <c r="N23" s="137"/>
+    </row>
+    <row r="24" spans="3:14">
+      <c r="C24" s="113"/>
+      <c r="D24" s="138"/>
+      <c r="E24" s="138"/>
+      <c r="F24" s="138"/>
+      <c r="G24" s="138"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="138"/>
+      <c r="J24" s="138"/>
+      <c r="K24" s="138"/>
+      <c r="L24" s="138"/>
+      <c r="M24" s="138"/>
+      <c r="N24" s="138"/>
+    </row>
+    <row r="25" spans="3:14" ht="19" thickBot="1">
+      <c r="C25" s="112"/>
+      <c r="D25" s="137"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="137"/>
+      <c r="G25" s="137"/>
+      <c r="H25" s="137"/>
+      <c r="I25" s="137"/>
+      <c r="J25" s="189"/>
+      <c r="K25" s="139"/>
+      <c r="L25" s="139"/>
+      <c r="M25" s="139"/>
+      <c r="N25" s="139"/>
+    </row>
+    <row r="26" spans="3:14" ht="17" thickBot="1">
+      <c r="C26" s="122"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="110"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="110"/>
+      <c r="N26" s="125"/>
+    </row>
+    <row r="27" spans="3:14" ht="18">
+      <c r="C27" s="114" t="s">
         <v>786</v>
       </c>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="119"/>
-      <c r="K11" s="119"/>
-    </row>
-    <row r="12" spans="3:11" ht="18">
-      <c r="C12" s="120" t="s">
-        <v>790</v>
-      </c>
-      <c r="D12" s="148"/>
-      <c r="E12" s="148" t="s">
+      <c r="D27" s="140"/>
+      <c r="E27" s="140"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="140"/>
+      <c r="I27" s="140"/>
+      <c r="J27" s="140"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="140"/>
+    </row>
+    <row r="28" spans="3:14" ht="18">
+      <c r="C28" s="115" t="s">
         <v>788</v>
       </c>
-      <c r="F12" s="148"/>
-      <c r="G12" s="148"/>
-      <c r="H12" s="148"/>
-      <c r="I12" s="148"/>
-      <c r="J12" s="148"/>
-      <c r="K12" s="148"/>
-    </row>
-    <row r="13" spans="3:11" ht="18">
-      <c r="C13" s="120" t="s">
-        <v>791</v>
-      </c>
-      <c r="D13" s="148"/>
-      <c r="E13" s="148" t="s">
-        <v>788</v>
-      </c>
-      <c r="F13" s="148"/>
-      <c r="G13" s="148"/>
-      <c r="H13" s="148"/>
-      <c r="I13" s="148"/>
-      <c r="J13" s="148"/>
-      <c r="K13" s="148"/>
-    </row>
-    <row r="14" spans="3:11" ht="18">
-      <c r="C14" s="120" t="s">
-        <v>792</v>
-      </c>
-      <c r="D14" s="148"/>
-      <c r="E14" s="148" t="s">
-        <v>788</v>
-      </c>
-      <c r="F14" s="148"/>
-      <c r="G14" s="148"/>
-      <c r="H14" s="148"/>
-      <c r="I14" s="148"/>
-      <c r="J14" s="148"/>
-      <c r="K14" s="148"/>
-    </row>
-    <row r="15" spans="3:11" ht="18">
-      <c r="C15" s="120" t="s">
+      <c r="D28" s="141"/>
+      <c r="E28" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="F28" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="141"/>
+      <c r="L28" s="141"/>
+      <c r="M28" s="141"/>
+      <c r="N28" s="141"/>
+    </row>
+    <row r="29" spans="3:14" ht="18">
+      <c r="C29" s="115" t="s">
         <v>793</v>
       </c>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148" t="s">
-        <v>788</v>
-      </c>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
-      <c r="K15" s="148"/>
-    </row>
-    <row r="16" spans="3:11" ht="18">
-      <c r="C16" s="120"/>
-      <c r="D16" s="148"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
-      <c r="K16" s="148"/>
-    </row>
-    <row r="17" spans="3:11" ht="18">
-      <c r="C17" s="120"/>
-      <c r="D17" s="148"/>
-      <c r="E17" s="148"/>
-      <c r="F17" s="148"/>
-      <c r="G17" s="148"/>
-      <c r="H17" s="148"/>
-      <c r="I17" s="148"/>
-      <c r="J17" s="148"/>
-      <c r="K17" s="148"/>
-    </row>
-    <row r="18" spans="3:11" ht="18">
-      <c r="C18" s="120"/>
-      <c r="D18" s="148"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
-      <c r="G18" s="148"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="148"/>
-      <c r="J18" s="148"/>
-      <c r="K18" s="148"/>
-    </row>
-    <row r="19" spans="3:11">
-      <c r="C19" s="121"/>
-      <c r="D19" s="149"/>
-      <c r="E19" s="149"/>
-      <c r="F19" s="149"/>
-      <c r="G19" s="149"/>
-      <c r="H19" s="149"/>
-      <c r="I19" s="149"/>
-      <c r="J19" s="149"/>
-      <c r="K19" s="149"/>
-    </row>
-    <row r="20" spans="3:11" ht="17" thickBot="1">
-      <c r="C20" s="122"/>
-      <c r="D20" s="150"/>
-      <c r="E20" s="150"/>
-      <c r="F20" s="150"/>
-      <c r="G20" s="150"/>
-      <c r="H20" s="150"/>
-      <c r="I20" s="150"/>
-      <c r="J20" s="150"/>
-      <c r="K20" s="150"/>
-    </row>
-    <row r="21" spans="3:11" ht="17" thickBot="1">
-      <c r="C21" s="132"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
-      <c r="K21" s="135"/>
-    </row>
-    <row r="22" spans="3:11" ht="18">
-      <c r="C22" s="123" t="s">
+      <c r="D29" s="141"/>
+      <c r="E29" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="D22" s="151"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="151"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="151"/>
-      <c r="J22" s="151"/>
-      <c r="K22" s="151"/>
-    </row>
-    <row r="23" spans="3:11" ht="18">
-      <c r="C23" s="124" t="s">
-        <v>789</v>
-      </c>
-      <c r="D23" s="152"/>
-      <c r="E23" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F23" s="152"/>
-      <c r="G23" s="152"/>
-      <c r="H23" s="152"/>
-      <c r="I23" s="152"/>
-      <c r="J23" s="152"/>
-      <c r="K23" s="152"/>
-    </row>
-    <row r="24" spans="3:11" ht="18">
-      <c r="C24" s="124" t="s">
+      <c r="F29" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G29" s="141"/>
+      <c r="H29" s="141"/>
+      <c r="I29" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J29" s="141"/>
+      <c r="K29" s="141"/>
+      <c r="L29" s="141"/>
+      <c r="M29" s="141"/>
+      <c r="N29" s="141"/>
+    </row>
+    <row r="30" spans="3:14" ht="18">
+      <c r="C30" s="115" t="s">
         <v>794</v>
       </c>
-      <c r="D24" s="152"/>
-      <c r="E24" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F24" s="152"/>
-      <c r="G24" s="152"/>
-      <c r="H24" s="152"/>
-      <c r="I24" s="152"/>
-      <c r="J24" s="152"/>
-      <c r="K24" s="152"/>
-    </row>
-    <row r="25" spans="3:11" ht="18">
-      <c r="C25" s="124" t="s">
+      <c r="D30" s="141"/>
+      <c r="E30" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="F30" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G30" s="141"/>
+      <c r="H30" s="141"/>
+      <c r="I30" s="141"/>
+      <c r="J30" s="141"/>
+      <c r="K30" s="141"/>
+      <c r="L30" s="141"/>
+      <c r="M30" s="141"/>
+      <c r="N30" s="141"/>
+    </row>
+    <row r="31" spans="3:14" ht="18">
+      <c r="C31" s="115" t="s">
+        <v>799</v>
+      </c>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="F31" s="141"/>
+      <c r="G31" s="141"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="141"/>
+      <c r="J31" s="141"/>
+      <c r="K31" s="141"/>
+      <c r="L31" s="141"/>
+      <c r="M31" s="141"/>
+      <c r="N31" s="141"/>
+    </row>
+    <row r="32" spans="3:14" ht="18">
+      <c r="C32" s="115" t="s">
+        <v>800</v>
+      </c>
+      <c r="D32" s="141"/>
+      <c r="E32" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="F32" s="141"/>
+      <c r="G32" s="141"/>
+      <c r="H32" s="141"/>
+      <c r="I32" s="141"/>
+      <c r="J32" s="141"/>
+      <c r="K32" s="141"/>
+      <c r="L32" s="141"/>
+      <c r="M32" s="141"/>
+      <c r="N32" s="141"/>
+    </row>
+    <row r="33" spans="3:14" ht="18">
+      <c r="C33" s="115" t="s">
+        <v>801</v>
+      </c>
+      <c r="D33" s="141"/>
+      <c r="E33" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="F33" s="141"/>
+      <c r="G33" s="141"/>
+      <c r="H33" s="141"/>
+      <c r="I33" s="141"/>
+      <c r="J33" s="141"/>
+      <c r="K33" s="141"/>
+      <c r="L33" s="141"/>
+      <c r="M33" s="141"/>
+      <c r="N33" s="141"/>
+    </row>
+    <row r="34" spans="3:14" ht="18">
+      <c r="C34" s="115" t="s">
         <v>795</v>
       </c>
-      <c r="D25" s="152"/>
-      <c r="E25" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F25" s="152"/>
-      <c r="G25" s="152"/>
-      <c r="H25" s="152"/>
-      <c r="I25" s="152"/>
-      <c r="J25" s="152"/>
-      <c r="K25" s="152"/>
-    </row>
-    <row r="26" spans="3:11" ht="18">
-      <c r="C26" s="124" t="s">
-        <v>800</v>
-      </c>
-      <c r="D26" s="152"/>
-      <c r="E26" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F26" s="152"/>
-      <c r="G26" s="152"/>
-      <c r="H26" s="152"/>
-      <c r="I26" s="152"/>
-      <c r="J26" s="152"/>
-      <c r="K26" s="152"/>
-    </row>
-    <row r="27" spans="3:11" ht="18">
-      <c r="C27" s="124" t="s">
-        <v>801</v>
-      </c>
-      <c r="D27" s="152"/>
-      <c r="E27" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F27" s="152"/>
-      <c r="G27" s="152"/>
-      <c r="H27" s="152"/>
-      <c r="I27" s="152"/>
-      <c r="J27" s="152"/>
-      <c r="K27" s="152"/>
-    </row>
-    <row r="28" spans="3:11" ht="18">
-      <c r="C28" s="124" t="s">
+      <c r="D34" s="141"/>
+      <c r="E34" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="F34" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G34" s="141"/>
+      <c r="H34" s="141"/>
+      <c r="I34" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J34" s="141"/>
+      <c r="K34" s="141"/>
+      <c r="L34" s="141"/>
+      <c r="M34" s="141"/>
+      <c r="N34" s="141"/>
+    </row>
+    <row r="35" spans="3:14" ht="18">
+      <c r="C35" s="115" t="s">
+        <v>833</v>
+      </c>
+      <c r="D35" s="141"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G35" s="141"/>
+      <c r="H35" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="I35" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J35" s="141"/>
+      <c r="K35" s="141"/>
+      <c r="L35" s="141"/>
+      <c r="M35" s="141"/>
+      <c r="N35" s="141"/>
+    </row>
+    <row r="36" spans="3:14" ht="18">
+      <c r="C36" s="115" t="s">
+        <v>834</v>
+      </c>
+      <c r="D36" s="141"/>
+      <c r="E36" s="141"/>
+      <c r="F36" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G36" s="141"/>
+      <c r="H36" s="141"/>
+      <c r="I36" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J36" s="141"/>
+      <c r="K36" s="141"/>
+      <c r="L36" s="141"/>
+      <c r="M36" s="141"/>
+      <c r="N36" s="141"/>
+    </row>
+    <row r="37" spans="3:14" ht="18">
+      <c r="C37" s="115" t="s">
+        <v>835</v>
+      </c>
+      <c r="D37" s="141"/>
+      <c r="E37" s="141"/>
+      <c r="F37" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G37" s="141"/>
+      <c r="H37" s="141"/>
+      <c r="I37" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J37" s="141"/>
+      <c r="K37" s="141"/>
+      <c r="L37" s="141"/>
+      <c r="M37" s="141"/>
+      <c r="N37" s="141"/>
+    </row>
+    <row r="38" spans="3:14" ht="18">
+      <c r="C38" s="115" t="s">
+        <v>821</v>
+      </c>
+      <c r="D38" s="141"/>
+      <c r="E38" s="141"/>
+      <c r="F38" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G38" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="H38" s="141"/>
+      <c r="I38" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J38" s="141"/>
+      <c r="K38" s="141"/>
+      <c r="L38" s="141"/>
+      <c r="M38" s="141"/>
+      <c r="N38" s="141"/>
+    </row>
+    <row r="39" spans="3:14" ht="18">
+      <c r="C39" s="115" t="s">
+        <v>842</v>
+      </c>
+      <c r="D39" s="141"/>
+      <c r="E39" s="141"/>
+      <c r="F39" s="141"/>
+      <c r="G39" s="141"/>
+      <c r="H39" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="I39" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J39" s="141"/>
+      <c r="K39" s="141"/>
+      <c r="L39" s="141"/>
+      <c r="M39" s="141"/>
+      <c r="N39" s="141"/>
+    </row>
+    <row r="40" spans="3:14" ht="18">
+      <c r="C40" s="115" t="s">
+        <v>837</v>
+      </c>
+      <c r="D40" s="141"/>
+      <c r="E40" s="141"/>
+      <c r="F40" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G40" s="141"/>
+      <c r="H40" s="141"/>
+      <c r="I40" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J40" s="141"/>
+      <c r="K40" s="141"/>
+      <c r="L40" s="141"/>
+      <c r="M40" s="141"/>
+      <c r="N40" s="141"/>
+    </row>
+    <row r="41" spans="3:14" ht="18">
+      <c r="C41" s="115" t="s">
+        <v>838</v>
+      </c>
+      <c r="D41" s="141"/>
+      <c r="E41" s="141"/>
+      <c r="F41" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="G41" s="141"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="J41" s="141"/>
+      <c r="K41" s="141"/>
+      <c r="L41" s="141"/>
+      <c r="M41" s="141"/>
+      <c r="N41" s="141"/>
+    </row>
+    <row r="42" spans="3:14" ht="18">
+      <c r="C42" s="115"/>
+      <c r="D42" s="141"/>
+      <c r="E42" s="141"/>
+      <c r="F42" s="141"/>
+      <c r="G42" s="141"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
+      <c r="J42" s="141"/>
+      <c r="K42" s="141"/>
+      <c r="L42" s="141"/>
+      <c r="M42" s="141"/>
+      <c r="N42" s="141"/>
+    </row>
+    <row r="43" spans="3:14">
+      <c r="C43" s="116"/>
+      <c r="D43" s="142"/>
+      <c r="E43" s="142"/>
+      <c r="F43" s="142"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="142"/>
+      <c r="I43" s="142"/>
+      <c r="J43" s="142"/>
+      <c r="K43" s="142"/>
+      <c r="L43" s="142"/>
+      <c r="M43" s="142"/>
+      <c r="N43" s="142"/>
+    </row>
+    <row r="44" spans="3:14" ht="19" thickBot="1">
+      <c r="C44" s="115"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="141"/>
+      <c r="F44" s="141"/>
+      <c r="G44" s="141"/>
+      <c r="H44" s="141"/>
+      <c r="I44" s="141"/>
+      <c r="J44" s="190"/>
+      <c r="K44" s="143"/>
+      <c r="L44" s="143"/>
+      <c r="M44" s="143"/>
+      <c r="N44" s="143"/>
+    </row>
+    <row r="45" spans="3:14" ht="17" thickBot="1">
+      <c r="C45" s="122"/>
+      <c r="D45" s="110"/>
+      <c r="E45" s="110"/>
+      <c r="F45" s="110"/>
+      <c r="G45" s="110"/>
+      <c r="H45" s="110"/>
+      <c r="I45" s="110"/>
+      <c r="J45" s="110"/>
+      <c r="K45" s="110"/>
+      <c r="L45" s="110"/>
+      <c r="M45" s="110"/>
+      <c r="N45" s="125"/>
+    </row>
+    <row r="46" spans="3:14" ht="18">
+      <c r="C46" s="126" t="s">
+        <v>803</v>
+      </c>
+      <c r="D46" s="144"/>
+      <c r="E46" s="144"/>
+      <c r="F46" s="144"/>
+      <c r="G46" s="144"/>
+      <c r="H46" s="144"/>
+      <c r="I46" s="144"/>
+      <c r="J46" s="144"/>
+      <c r="K46" s="144"/>
+      <c r="L46" s="144"/>
+      <c r="M46" s="144"/>
+      <c r="N46" s="144"/>
+    </row>
+    <row r="47" spans="3:14" ht="18">
+      <c r="C47" s="127" t="s">
+        <v>797</v>
+      </c>
+      <c r="D47" s="145"/>
+      <c r="E47" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="F47" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G47" s="145"/>
+      <c r="H47" s="145"/>
+      <c r="I47" s="145"/>
+      <c r="J47" s="145"/>
+      <c r="K47" s="145"/>
+      <c r="L47" s="145"/>
+      <c r="M47" s="145"/>
+      <c r="N47" s="145"/>
+    </row>
+    <row r="48" spans="3:14" ht="18">
+      <c r="C48" s="127" t="s">
+        <v>804</v>
+      </c>
+      <c r="D48" s="145"/>
+      <c r="E48" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="F48" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G48" s="145"/>
+      <c r="H48" s="145"/>
+      <c r="I48" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J48" s="145"/>
+      <c r="K48" s="145"/>
+      <c r="L48" s="145"/>
+      <c r="M48" s="145"/>
+      <c r="N48" s="145"/>
+    </row>
+    <row r="49" spans="3:14" ht="18">
+      <c r="C49" s="127" t="s">
+        <v>805</v>
+      </c>
+      <c r="D49" s="145"/>
+      <c r="E49" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="F49" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G49" s="145"/>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="145"/>
+      <c r="K49" s="145"/>
+      <c r="L49" s="145"/>
+      <c r="M49" s="145"/>
+      <c r="N49" s="145"/>
+    </row>
+    <row r="50" spans="3:14" ht="18">
+      <c r="C50" s="127" t="s">
+        <v>806</v>
+      </c>
+      <c r="D50" s="145"/>
+      <c r="E50" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="F50" s="145"/>
+      <c r="G50" s="145"/>
+      <c r="H50" s="145"/>
+      <c r="I50" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J50" s="145"/>
+      <c r="K50" s="145"/>
+      <c r="L50" s="145"/>
+      <c r="M50" s="145"/>
+      <c r="N50" s="145"/>
+    </row>
+    <row r="51" spans="3:14" ht="19">
+      <c r="C51" s="127" t="s">
+        <v>810</v>
+      </c>
+      <c r="D51" s="145"/>
+      <c r="E51" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="F51" s="145"/>
+      <c r="G51" s="145"/>
+      <c r="H51" s="145"/>
+      <c r="I51" s="145"/>
+      <c r="J51" s="145"/>
+      <c r="K51" s="145"/>
+      <c r="L51" s="145"/>
+      <c r="M51" s="145"/>
+      <c r="N51" s="145"/>
+    </row>
+    <row r="52" spans="3:14" ht="18">
+      <c r="C52" s="127" t="s">
+        <v>825</v>
+      </c>
+      <c r="D52" s="145"/>
+      <c r="E52" s="145"/>
+      <c r="F52" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G52" s="145"/>
+      <c r="H52" s="145"/>
+      <c r="I52" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J52" s="145"/>
+      <c r="K52" s="145"/>
+      <c r="L52" s="145"/>
+      <c r="M52" s="145"/>
+      <c r="N52" s="145"/>
+    </row>
+    <row r="53" spans="3:14" ht="18">
+      <c r="C53" s="127" t="s">
+        <v>826</v>
+      </c>
+      <c r="D53" s="145"/>
+      <c r="E53" s="145"/>
+      <c r="F53" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G53" s="145"/>
+      <c r="H53" s="145"/>
+      <c r="I53" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J53" s="145"/>
+      <c r="K53" s="145"/>
+      <c r="L53" s="145"/>
+      <c r="M53" s="145"/>
+      <c r="N53" s="145"/>
+    </row>
+    <row r="54" spans="3:14" ht="18">
+      <c r="C54" s="127" t="s">
+        <v>830</v>
+      </c>
+      <c r="D54" s="127"/>
+      <c r="E54" s="127"/>
+      <c r="F54" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G54" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="H54" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="I54" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J54" s="145"/>
+      <c r="K54" s="145"/>
+      <c r="L54" s="145"/>
+      <c r="M54" s="145"/>
+      <c r="N54" s="145"/>
+    </row>
+    <row r="55" spans="3:14" ht="18">
+      <c r="C55" s="127" t="s">
+        <v>831</v>
+      </c>
+      <c r="D55" s="127"/>
+      <c r="E55" s="127"/>
+      <c r="F55" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G55" s="145"/>
+      <c r="H55" s="145"/>
+      <c r="I55" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J55" s="145"/>
+      <c r="K55" s="145"/>
+      <c r="L55" s="145"/>
+      <c r="M55" s="145"/>
+      <c r="N55" s="145"/>
+    </row>
+    <row r="56" spans="3:14" ht="18">
+      <c r="C56" s="127" t="s">
+        <v>832</v>
+      </c>
+      <c r="D56" s="127"/>
+      <c r="E56" s="127"/>
+      <c r="F56" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="G56" s="145"/>
+      <c r="H56" s="145"/>
+      <c r="I56" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="J56" s="145"/>
+      <c r="K56" s="145"/>
+      <c r="L56" s="145"/>
+      <c r="M56" s="145"/>
+      <c r="N56" s="145"/>
+    </row>
+    <row r="57" spans="3:14" ht="18">
+      <c r="C57" s="127"/>
+      <c r="D57" s="145"/>
+      <c r="E57" s="145"/>
+      <c r="F57" s="145"/>
+      <c r="G57" s="145"/>
+      <c r="H57" s="145"/>
+      <c r="I57" s="145"/>
+      <c r="J57" s="145"/>
+      <c r="K57" s="145"/>
+      <c r="L57" s="145"/>
+      <c r="M57" s="145"/>
+      <c r="N57" s="145"/>
+    </row>
+    <row r="58" spans="3:14" ht="18">
+      <c r="C58" s="127"/>
+      <c r="D58" s="145"/>
+      <c r="E58" s="145"/>
+      <c r="F58" s="145"/>
+      <c r="G58" s="145"/>
+      <c r="H58" s="145"/>
+      <c r="I58" s="145"/>
+      <c r="J58" s="145"/>
+      <c r="K58" s="145"/>
+      <c r="L58" s="145"/>
+      <c r="M58" s="145"/>
+      <c r="N58" s="145"/>
+    </row>
+    <row r="59" spans="3:14" ht="18">
+      <c r="C59" s="127"/>
+      <c r="D59" s="145"/>
+      <c r="E59" s="145"/>
+      <c r="F59" s="145"/>
+      <c r="G59" s="145"/>
+      <c r="H59" s="145"/>
+      <c r="I59" s="145"/>
+      <c r="J59" s="145"/>
+      <c r="K59" s="145"/>
+      <c r="L59" s="145"/>
+      <c r="M59" s="145"/>
+      <c r="N59" s="145"/>
+    </row>
+    <row r="60" spans="3:14">
+      <c r="C60" s="128"/>
+      <c r="D60" s="146"/>
+      <c r="E60" s="146"/>
+      <c r="F60" s="146"/>
+      <c r="G60" s="146"/>
+      <c r="H60" s="146"/>
+      <c r="I60" s="146"/>
+      <c r="J60" s="146"/>
+      <c r="K60" s="146"/>
+      <c r="L60" s="146"/>
+      <c r="M60" s="146"/>
+      <c r="N60" s="146"/>
+    </row>
+    <row r="61" spans="3:14" ht="19" thickBot="1">
+      <c r="C61" s="127"/>
+      <c r="D61" s="145"/>
+      <c r="E61" s="145"/>
+      <c r="F61" s="145"/>
+      <c r="G61" s="145"/>
+      <c r="H61" s="145"/>
+      <c r="I61" s="145"/>
+      <c r="J61" s="191"/>
+      <c r="K61" s="147"/>
+      <c r="L61" s="147"/>
+      <c r="M61" s="147"/>
+      <c r="N61" s="147"/>
+    </row>
+    <row r="62" spans="3:14" ht="17" thickBot="1">
+      <c r="C62" s="122"/>
+      <c r="D62" s="110"/>
+      <c r="E62" s="110"/>
+      <c r="F62" s="110"/>
+      <c r="G62" s="110"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="110"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="110"/>
+      <c r="L62" s="110"/>
+      <c r="M62" s="110"/>
+      <c r="N62" s="125"/>
+    </row>
+    <row r="63" spans="3:14" ht="18">
+      <c r="C63" s="117" t="s">
+        <v>808</v>
+      </c>
+      <c r="D63" s="148"/>
+      <c r="E63" s="148"/>
+      <c r="F63" s="148"/>
+      <c r="G63" s="148"/>
+      <c r="H63" s="148"/>
+      <c r="I63" s="148"/>
+      <c r="J63" s="148"/>
+      <c r="K63" s="148"/>
+      <c r="L63" s="148"/>
+      <c r="M63" s="148"/>
+      <c r="N63" s="148"/>
+    </row>
+    <row r="64" spans="3:14" ht="19">
+      <c r="C64" s="118" t="s">
+        <v>811</v>
+      </c>
+      <c r="D64" s="149"/>
+      <c r="E64" s="149" t="s">
+        <v>787</v>
+      </c>
+      <c r="F64" s="149" t="s">
+        <v>787</v>
+      </c>
+      <c r="G64" s="149"/>
+      <c r="H64" s="149"/>
+      <c r="I64" s="149"/>
+      <c r="J64" s="149"/>
+      <c r="K64" s="149"/>
+      <c r="L64" s="149"/>
+      <c r="M64" s="149"/>
+      <c r="N64" s="149"/>
+    </row>
+    <row r="65" spans="3:14" ht="19">
+      <c r="C65" s="118" t="s">
+        <v>812</v>
+      </c>
+      <c r="D65" s="149"/>
+      <c r="E65" s="149" t="s">
+        <v>787</v>
+      </c>
+      <c r="F65" s="149"/>
+      <c r="G65" s="149"/>
+      <c r="H65" s="149"/>
+      <c r="I65" s="149"/>
+      <c r="J65" s="149"/>
+      <c r="K65" s="149"/>
+      <c r="L65" s="149"/>
+      <c r="M65" s="149"/>
+      <c r="N65" s="149"/>
+    </row>
+    <row r="66" spans="3:14" ht="18">
+      <c r="C66" s="118"/>
+      <c r="D66" s="149"/>
+      <c r="E66" s="149"/>
+      <c r="F66" s="149"/>
+      <c r="G66" s="149"/>
+      <c r="H66" s="149"/>
+      <c r="I66" s="149"/>
+      <c r="J66" s="149"/>
+      <c r="K66" s="149"/>
+      <c r="L66" s="149"/>
+      <c r="M66" s="149"/>
+      <c r="N66" s="149"/>
+    </row>
+    <row r="67" spans="3:14" ht="18">
+      <c r="C67" s="118"/>
+      <c r="D67" s="149"/>
+      <c r="E67" s="149"/>
+      <c r="F67" s="149"/>
+      <c r="G67" s="149"/>
+      <c r="H67" s="149"/>
+      <c r="I67" s="149"/>
+      <c r="J67" s="149"/>
+      <c r="K67" s="149"/>
+      <c r="L67" s="149"/>
+      <c r="M67" s="149"/>
+      <c r="N67" s="149"/>
+    </row>
+    <row r="68" spans="3:14" ht="18">
+      <c r="C68" s="118"/>
+      <c r="D68" s="149"/>
+      <c r="E68" s="149"/>
+      <c r="F68" s="149"/>
+      <c r="G68" s="149"/>
+      <c r="H68" s="149"/>
+      <c r="I68" s="149"/>
+      <c r="J68" s="149"/>
+      <c r="K68" s="149"/>
+      <c r="L68" s="149"/>
+      <c r="M68" s="149"/>
+      <c r="N68" s="149"/>
+    </row>
+    <row r="69" spans="3:14" ht="18">
+      <c r="C69" s="118"/>
+      <c r="D69" s="149"/>
+      <c r="E69" s="149"/>
+      <c r="F69" s="149"/>
+      <c r="G69" s="149"/>
+      <c r="H69" s="149"/>
+      <c r="I69" s="149"/>
+      <c r="J69" s="149"/>
+      <c r="K69" s="149"/>
+      <c r="L69" s="149"/>
+      <c r="M69" s="149"/>
+      <c r="N69" s="149"/>
+    </row>
+    <row r="70" spans="3:14" ht="18">
+      <c r="C70" s="118"/>
+      <c r="D70" s="149"/>
+      <c r="E70" s="149"/>
+      <c r="F70" s="149"/>
+      <c r="G70" s="149"/>
+      <c r="H70" s="149"/>
+      <c r="I70" s="149"/>
+      <c r="J70" s="149"/>
+      <c r="K70" s="149"/>
+      <c r="L70" s="149"/>
+      <c r="M70" s="149"/>
+      <c r="N70" s="149"/>
+    </row>
+    <row r="71" spans="3:14" ht="18">
+      <c r="C71" s="118"/>
+      <c r="D71" s="149"/>
+      <c r="E71" s="149"/>
+      <c r="F71" s="149"/>
+      <c r="G71" s="149"/>
+      <c r="H71" s="149"/>
+      <c r="I71" s="149"/>
+      <c r="J71" s="149"/>
+      <c r="K71" s="149"/>
+      <c r="L71" s="149"/>
+      <c r="M71" s="149"/>
+      <c r="N71" s="149"/>
+    </row>
+    <row r="72" spans="3:14" ht="18">
+      <c r="C72" s="118"/>
+      <c r="D72" s="149"/>
+      <c r="E72" s="149"/>
+      <c r="F72" s="149"/>
+      <c r="G72" s="149"/>
+      <c r="H72" s="149"/>
+      <c r="I72" s="149"/>
+      <c r="J72" s="149"/>
+      <c r="K72" s="149"/>
+      <c r="L72" s="149"/>
+      <c r="M72" s="149"/>
+      <c r="N72" s="149"/>
+    </row>
+    <row r="73" spans="3:14">
+      <c r="C73" s="119"/>
+      <c r="D73" s="150"/>
+      <c r="E73" s="150"/>
+      <c r="F73" s="150"/>
+      <c r="G73" s="150"/>
+      <c r="H73" s="150"/>
+      <c r="I73" s="150"/>
+      <c r="J73" s="150"/>
+      <c r="K73" s="150"/>
+      <c r="L73" s="150"/>
+      <c r="M73" s="150"/>
+      <c r="N73" s="150"/>
+    </row>
+    <row r="74" spans="3:14" ht="17" thickBot="1">
+      <c r="C74" s="120"/>
+      <c r="D74" s="151"/>
+      <c r="E74" s="151"/>
+      <c r="F74" s="151"/>
+      <c r="G74" s="151"/>
+      <c r="H74" s="151"/>
+      <c r="I74" s="151"/>
+      <c r="J74" s="151"/>
+      <c r="K74" s="151"/>
+      <c r="L74" s="151"/>
+      <c r="M74" s="151"/>
+      <c r="N74" s="151"/>
+    </row>
+    <row r="75" spans="3:14" ht="17" thickBot="1">
+      <c r="C75" s="122"/>
+      <c r="D75" s="110"/>
+      <c r="E75" s="110"/>
+      <c r="F75" s="110"/>
+      <c r="G75" s="110"/>
+      <c r="H75" s="110"/>
+      <c r="I75" s="110"/>
+      <c r="J75" s="110"/>
+      <c r="K75" s="110"/>
+      <c r="L75" s="110"/>
+      <c r="M75" s="110"/>
+      <c r="N75" s="125"/>
+    </row>
+    <row r="76" spans="3:14" ht="19">
+      <c r="C76" s="132" t="s">
+        <v>796</v>
+      </c>
+      <c r="D76" s="152"/>
+      <c r="E76" s="152"/>
+      <c r="F76" s="152"/>
+      <c r="G76" s="152"/>
+      <c r="H76" s="152"/>
+      <c r="I76" s="152"/>
+      <c r="J76" s="152"/>
+      <c r="K76" s="152"/>
+      <c r="L76" s="152"/>
+      <c r="M76" s="152"/>
+      <c r="N76" s="152"/>
+    </row>
+    <row r="77" spans="3:14" ht="18">
+      <c r="C77" s="130" t="s">
+        <v>809</v>
+      </c>
+      <c r="D77" s="153"/>
+      <c r="E77" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="F77" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="G77" s="153"/>
+      <c r="H77" s="153"/>
+      <c r="I77" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="J77" s="153"/>
+      <c r="K77" s="153"/>
+      <c r="L77" s="153"/>
+      <c r="M77" s="153"/>
+      <c r="N77" s="153"/>
+    </row>
+    <row r="78" spans="3:14" ht="18">
+      <c r="C78" s="130" t="s">
+        <v>798</v>
+      </c>
+      <c r="D78" s="153"/>
+      <c r="E78" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="F78" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="G78" s="153"/>
+      <c r="H78" s="153"/>
+      <c r="I78" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="J78" s="153"/>
+      <c r="K78" s="153"/>
+      <c r="L78" s="153"/>
+      <c r="M78" s="153"/>
+      <c r="N78" s="153"/>
+    </row>
+    <row r="79" spans="3:14" ht="19">
+      <c r="C79" s="130" t="s">
+        <v>813</v>
+      </c>
+      <c r="D79" s="153"/>
+      <c r="E79" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="F79" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="G79" s="153"/>
+      <c r="H79" s="153"/>
+      <c r="I79" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="J79" s="153"/>
+      <c r="K79" s="153"/>
+      <c r="L79" s="153"/>
+      <c r="M79" s="153"/>
+      <c r="N79" s="153"/>
+    </row>
+    <row r="80" spans="3:14" ht="19">
+      <c r="C80" s="130" t="s">
+        <v>814</v>
+      </c>
+      <c r="D80" s="153"/>
+      <c r="E80" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="F80" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="G80" s="153"/>
+      <c r="H80" s="153"/>
+      <c r="I80" s="153"/>
+      <c r="J80" s="153"/>
+      <c r="K80" s="153"/>
+      <c r="L80" s="153"/>
+      <c r="M80" s="153"/>
+      <c r="N80" s="153"/>
+    </row>
+    <row r="81" spans="3:14" ht="18">
+      <c r="C81" s="130" t="s">
+        <v>815</v>
+      </c>
+      <c r="D81" s="153"/>
+      <c r="E81" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="F81" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="G81" s="153"/>
+      <c r="H81" s="153"/>
+      <c r="I81" s="153"/>
+      <c r="J81" s="153"/>
+      <c r="K81" s="153"/>
+      <c r="L81" s="153"/>
+      <c r="M81" s="153"/>
+      <c r="N81" s="153"/>
+    </row>
+    <row r="82" spans="3:14" ht="18">
+      <c r="C82" s="130" t="s">
+        <v>807</v>
+      </c>
+      <c r="D82" s="153"/>
+      <c r="E82" s="153" t="s">
+        <v>787</v>
+      </c>
+      <c r="F82" s="153"/>
+      <c r="G82" s="153"/>
+      <c r="H82" s="153"/>
+      <c r="I82" s="153"/>
+      <c r="J82" s="153"/>
+      <c r="K82" s="153"/>
+      <c r="L82" s="153"/>
+      <c r="M82" s="153"/>
+      <c r="N82" s="153"/>
+    </row>
+    <row r="83" spans="3:14" ht="18">
+      <c r="C83" s="131" t="s">
         <v>802</v>
       </c>
-      <c r="D28" s="152"/>
-      <c r="E28" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F28" s="152"/>
-      <c r="G28" s="152"/>
-      <c r="H28" s="152"/>
-      <c r="I28" s="152"/>
-      <c r="J28" s="152"/>
-      <c r="K28" s="152"/>
-    </row>
-    <row r="29" spans="3:11" ht="18">
-      <c r="C29" s="124" t="s">
-        <v>796</v>
-      </c>
-      <c r="D29" s="152"/>
-      <c r="E29" s="152" t="s">
-        <v>788</v>
-      </c>
-      <c r="F29" s="152"/>
-      <c r="G29" s="152"/>
-      <c r="H29" s="152"/>
-      <c r="I29" s="152"/>
-      <c r="J29" s="152"/>
-      <c r="K29" s="152"/>
-    </row>
-    <row r="30" spans="3:11" ht="18">
-      <c r="C30" s="124"/>
-      <c r="D30" s="152"/>
-      <c r="E30" s="152"/>
-      <c r="F30" s="152"/>
-      <c r="G30" s="152"/>
-      <c r="H30" s="152"/>
-      <c r="I30" s="152"/>
-      <c r="J30" s="152"/>
-      <c r="K30" s="152"/>
-    </row>
-    <row r="31" spans="3:11" ht="18">
-      <c r="C31" s="124"/>
-      <c r="D31" s="152"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="152"/>
-      <c r="I31" s="152"/>
-      <c r="J31" s="152"/>
-      <c r="K31" s="152"/>
-    </row>
-    <row r="32" spans="3:11" ht="18">
-      <c r="C32" s="124"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
-      <c r="H32" s="152"/>
-      <c r="I32" s="152"/>
-      <c r="J32" s="152"/>
-      <c r="K32" s="152"/>
-    </row>
-    <row r="33" spans="3:11">
-      <c r="C33" s="125"/>
-      <c r="D33" s="153"/>
-      <c r="E33" s="153"/>
-      <c r="F33" s="153"/>
-      <c r="G33" s="153"/>
-      <c r="H33" s="153"/>
-      <c r="I33" s="153"/>
-      <c r="J33" s="153"/>
-      <c r="K33" s="153"/>
-    </row>
-    <row r="34" spans="3:11" ht="17" thickBot="1">
-      <c r="C34" s="126"/>
-      <c r="D34" s="154"/>
-      <c r="E34" s="154"/>
-      <c r="F34" s="154"/>
-      <c r="G34" s="154"/>
-      <c r="H34" s="154"/>
-      <c r="I34" s="154"/>
-      <c r="J34" s="154"/>
-      <c r="K34" s="154"/>
-    </row>
-    <row r="35" spans="3:11" ht="17" thickBot="1">
-      <c r="C35" s="132"/>
-      <c r="D35" s="118"/>
-      <c r="E35" s="118"/>
-      <c r="F35" s="118"/>
-      <c r="G35" s="118"/>
-      <c r="H35" s="118"/>
-      <c r="I35" s="118"/>
-      <c r="J35" s="118"/>
-      <c r="K35" s="135"/>
-    </row>
-    <row r="36" spans="3:11" ht="18">
-      <c r="C36" s="136" t="s">
-        <v>804</v>
-      </c>
-      <c r="D36" s="155"/>
-      <c r="E36" s="155"/>
-      <c r="F36" s="155"/>
-      <c r="G36" s="155"/>
-      <c r="H36" s="155"/>
-      <c r="I36" s="155"/>
-      <c r="J36" s="155"/>
-      <c r="K36" s="155"/>
-    </row>
-    <row r="37" spans="3:11" ht="18">
-      <c r="C37" s="137" t="s">
-        <v>798</v>
-      </c>
-      <c r="D37" s="156"/>
-      <c r="E37" s="156" t="s">
-        <v>788</v>
-      </c>
-      <c r="F37" s="156"/>
-      <c r="G37" s="156"/>
-      <c r="H37" s="156"/>
-      <c r="I37" s="156"/>
-      <c r="J37" s="156"/>
-      <c r="K37" s="156"/>
-    </row>
-    <row r="38" spans="3:11" ht="18">
-      <c r="C38" s="137" t="s">
-        <v>805</v>
-      </c>
-      <c r="D38" s="156"/>
-      <c r="E38" s="156" t="s">
-        <v>788</v>
-      </c>
-      <c r="F38" s="156"/>
-      <c r="G38" s="156"/>
-      <c r="H38" s="156"/>
-      <c r="I38" s="156"/>
-      <c r="J38" s="156"/>
-      <c r="K38" s="156"/>
-    </row>
-    <row r="39" spans="3:11" ht="18">
-      <c r="C39" s="137" t="s">
-        <v>806</v>
-      </c>
-      <c r="D39" s="156"/>
-      <c r="E39" s="156" t="s">
-        <v>788</v>
-      </c>
-      <c r="F39" s="156"/>
-      <c r="G39" s="156"/>
-      <c r="H39" s="156"/>
-      <c r="I39" s="156"/>
-      <c r="J39" s="156"/>
-      <c r="K39" s="156"/>
-    </row>
-    <row r="40" spans="3:11" ht="18">
-      <c r="C40" s="137" t="s">
-        <v>807</v>
-      </c>
-      <c r="D40" s="156"/>
-      <c r="E40" s="156" t="s">
-        <v>788</v>
-      </c>
-      <c r="F40" s="156"/>
-      <c r="G40" s="156"/>
-      <c r="H40" s="156"/>
-      <c r="I40" s="156"/>
-      <c r="J40" s="156"/>
-      <c r="K40" s="156"/>
-    </row>
-    <row r="41" spans="3:11" ht="19">
-      <c r="C41" s="137" t="s">
-        <v>811</v>
-      </c>
-      <c r="D41" s="156"/>
-      <c r="E41" s="156" t="s">
-        <v>788</v>
-      </c>
-      <c r="F41" s="156"/>
-      <c r="G41" s="156"/>
-      <c r="H41" s="156"/>
-      <c r="I41" s="156"/>
-      <c r="J41" s="156"/>
-      <c r="K41" s="156"/>
-    </row>
-    <row r="42" spans="3:11" ht="18">
-      <c r="C42" s="137"/>
-      <c r="D42" s="156"/>
-      <c r="E42" s="156"/>
-      <c r="F42" s="156"/>
-      <c r="G42" s="156"/>
-      <c r="H42" s="156"/>
-      <c r="I42" s="156"/>
-      <c r="J42" s="156"/>
-      <c r="K42" s="156"/>
-    </row>
-    <row r="43" spans="3:11" ht="18">
-      <c r="C43" s="137"/>
-      <c r="D43" s="156"/>
-      <c r="E43" s="156"/>
-      <c r="F43" s="156"/>
-      <c r="G43" s="156"/>
-      <c r="H43" s="156"/>
-      <c r="I43" s="156"/>
-      <c r="J43" s="156"/>
-      <c r="K43" s="156"/>
-    </row>
-    <row r="44" spans="3:11" ht="18">
-      <c r="C44" s="137"/>
-      <c r="D44" s="156"/>
-      <c r="E44" s="156"/>
-      <c r="F44" s="156"/>
-      <c r="G44" s="156"/>
-      <c r="H44" s="156"/>
-      <c r="I44" s="156"/>
-      <c r="J44" s="156"/>
-      <c r="K44" s="156"/>
-    </row>
-    <row r="45" spans="3:11">
-      <c r="C45" s="138"/>
-      <c r="D45" s="157"/>
-      <c r="E45" s="157"/>
-      <c r="F45" s="157"/>
-      <c r="G45" s="157"/>
-      <c r="H45" s="157"/>
-      <c r="I45" s="157"/>
-      <c r="J45" s="157"/>
-      <c r="K45" s="157"/>
-    </row>
-    <row r="46" spans="3:11" ht="17" thickBot="1">
-      <c r="C46" s="139"/>
-      <c r="D46" s="158"/>
-      <c r="E46" s="158"/>
-      <c r="F46" s="158"/>
-      <c r="G46" s="158"/>
-      <c r="H46" s="158"/>
-      <c r="I46" s="158"/>
-      <c r="J46" s="158"/>
-      <c r="K46" s="158"/>
-    </row>
-    <row r="47" spans="3:11" ht="17" thickBot="1">
-      <c r="C47" s="132"/>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="118"/>
-      <c r="I47" s="118"/>
-      <c r="J47" s="118"/>
-      <c r="K47" s="135"/>
-    </row>
-    <row r="48" spans="3:11" ht="18">
-      <c r="C48" s="127" t="s">
-        <v>809</v>
-      </c>
-      <c r="D48" s="159"/>
-      <c r="E48" s="159"/>
-      <c r="F48" s="159"/>
-      <c r="G48" s="159"/>
-      <c r="H48" s="159"/>
-      <c r="I48" s="159"/>
-      <c r="J48" s="159"/>
-      <c r="K48" s="159"/>
-    </row>
-    <row r="49" spans="3:11" ht="19">
-      <c r="C49" s="128" t="s">
-        <v>812</v>
-      </c>
-      <c r="D49" s="160"/>
-      <c r="E49" s="160" t="s">
-        <v>788</v>
-      </c>
-      <c r="F49" s="160"/>
-      <c r="G49" s="160"/>
-      <c r="H49" s="160"/>
-      <c r="I49" s="160"/>
-      <c r="J49" s="160"/>
-      <c r="K49" s="160"/>
-    </row>
-    <row r="50" spans="3:11" ht="19">
-      <c r="C50" s="128" t="s">
-        <v>813</v>
-      </c>
-      <c r="D50" s="160"/>
-      <c r="E50" s="160" t="s">
-        <v>788</v>
-      </c>
-      <c r="F50" s="160"/>
-      <c r="G50" s="160"/>
-      <c r="H50" s="160"/>
-      <c r="I50" s="160"/>
-      <c r="J50" s="160"/>
-      <c r="K50" s="160"/>
-    </row>
-    <row r="51" spans="3:11" ht="18">
-      <c r="C51" s="128"/>
-      <c r="D51" s="160"/>
-      <c r="E51" s="160"/>
-      <c r="F51" s="160"/>
-      <c r="G51" s="160"/>
-      <c r="H51" s="160"/>
-      <c r="I51" s="160"/>
-      <c r="J51" s="160"/>
-      <c r="K51" s="160"/>
-    </row>
-    <row r="52" spans="3:11" ht="18">
-      <c r="C52" s="128"/>
-      <c r="D52" s="160"/>
-      <c r="E52" s="160"/>
-      <c r="F52" s="160"/>
-      <c r="G52" s="160"/>
-      <c r="H52" s="160"/>
-      <c r="I52" s="160"/>
-      <c r="J52" s="160"/>
-      <c r="K52" s="160"/>
-    </row>
-    <row r="53" spans="3:11" ht="18">
-      <c r="C53" s="128"/>
-      <c r="D53" s="160"/>
-      <c r="E53" s="160"/>
-      <c r="F53" s="160"/>
-      <c r="G53" s="160"/>
-      <c r="H53" s="160"/>
-      <c r="I53" s="160"/>
-      <c r="J53" s="160"/>
-      <c r="K53" s="160"/>
-    </row>
-    <row r="54" spans="3:11">
-      <c r="C54" s="129"/>
-      <c r="D54" s="161"/>
-      <c r="E54" s="161"/>
-      <c r="F54" s="161"/>
-      <c r="G54" s="161"/>
-      <c r="H54" s="161"/>
-      <c r="I54" s="161"/>
-      <c r="J54" s="161"/>
-      <c r="K54" s="161"/>
-    </row>
-    <row r="55" spans="3:11" ht="17" thickBot="1">
-      <c r="C55" s="130"/>
-      <c r="D55" s="162"/>
-      <c r="E55" s="162"/>
-      <c r="F55" s="162"/>
-      <c r="G55" s="162"/>
-      <c r="H55" s="162"/>
-      <c r="I55" s="162"/>
-      <c r="J55" s="162"/>
-      <c r="K55" s="162"/>
-    </row>
-    <row r="56" spans="3:11" ht="17" thickBot="1">
-      <c r="C56" s="132"/>
-      <c r="D56" s="118"/>
-      <c r="E56" s="118"/>
-      <c r="F56" s="118"/>
-      <c r="G56" s="118"/>
-      <c r="H56" s="118"/>
-      <c r="I56" s="118"/>
-      <c r="J56" s="118"/>
-      <c r="K56" s="135"/>
-    </row>
-    <row r="57" spans="3:11" ht="19">
-      <c r="C57" s="143" t="s">
-        <v>797</v>
-      </c>
-      <c r="D57" s="163"/>
-      <c r="E57" s="163"/>
-      <c r="F57" s="163"/>
-      <c r="G57" s="163"/>
-      <c r="H57" s="163"/>
-      <c r="I57" s="163"/>
-      <c r="J57" s="163"/>
-      <c r="K57" s="163"/>
-    </row>
-    <row r="58" spans="3:11" ht="18">
-      <c r="C58" s="141" t="s">
-        <v>810</v>
-      </c>
-      <c r="D58" s="164"/>
-      <c r="E58" s="164" t="s">
-        <v>788</v>
-      </c>
-      <c r="F58" s="164"/>
-      <c r="G58" s="164"/>
-      <c r="H58" s="164"/>
-      <c r="I58" s="164"/>
-      <c r="J58" s="164"/>
-      <c r="K58" s="164"/>
-    </row>
-    <row r="59" spans="3:11" ht="18">
-      <c r="C59" s="141" t="s">
-        <v>799</v>
-      </c>
-      <c r="D59" s="164"/>
-      <c r="E59" s="164" t="s">
-        <v>788</v>
-      </c>
-      <c r="F59" s="164"/>
-      <c r="G59" s="164"/>
-      <c r="H59" s="164"/>
-      <c r="I59" s="164"/>
-      <c r="J59" s="164"/>
-      <c r="K59" s="164"/>
-    </row>
-    <row r="60" spans="3:11" ht="19">
-      <c r="C60" s="141" t="s">
-        <v>814</v>
-      </c>
-      <c r="D60" s="164"/>
-      <c r="E60" s="164" t="s">
-        <v>788</v>
-      </c>
-      <c r="F60" s="164"/>
-      <c r="G60" s="164"/>
-      <c r="H60" s="164"/>
-      <c r="I60" s="164"/>
-      <c r="J60" s="164"/>
-      <c r="K60" s="164"/>
-    </row>
-    <row r="61" spans="3:11" ht="19">
-      <c r="C61" s="141" t="s">
-        <v>815</v>
-      </c>
-      <c r="D61" s="164"/>
-      <c r="E61" s="164" t="s">
-        <v>788</v>
-      </c>
-      <c r="F61" s="164"/>
-      <c r="G61" s="164"/>
-      <c r="H61" s="164"/>
-      <c r="I61" s="164"/>
-      <c r="J61" s="164"/>
-      <c r="K61" s="164"/>
-    </row>
-    <row r="62" spans="3:11" ht="18">
-      <c r="C62" s="141" t="s">
+      <c r="D83" s="154"/>
+      <c r="E83" s="154" t="s">
+        <v>787</v>
+      </c>
+      <c r="F83" s="154" t="s">
+        <v>787</v>
+      </c>
+      <c r="G83" s="154"/>
+      <c r="H83" s="154"/>
+      <c r="I83" s="154"/>
+      <c r="J83" s="154"/>
+      <c r="K83" s="154"/>
+      <c r="L83" s="154"/>
+      <c r="M83" s="154"/>
+      <c r="N83" s="154"/>
+    </row>
+    <row r="84" spans="3:14" ht="18">
+      <c r="C84" s="131" t="s">
+        <v>820</v>
+      </c>
+      <c r="D84" s="154"/>
+      <c r="E84" s="154"/>
+      <c r="F84" s="154"/>
+      <c r="G84" s="154" t="s">
+        <v>787</v>
+      </c>
+      <c r="H84" s="154"/>
+      <c r="I84" s="154"/>
+      <c r="J84" s="154"/>
+      <c r="K84" s="154"/>
+      <c r="L84" s="154"/>
+      <c r="M84" s="154"/>
+      <c r="N84" s="154"/>
+    </row>
+    <row r="85" spans="3:14" ht="18">
+      <c r="C85" s="131" t="s">
+        <v>822</v>
+      </c>
+      <c r="D85" s="154"/>
+      <c r="E85" s="154"/>
+      <c r="F85" s="154"/>
+      <c r="G85" s="154" t="s">
+        <v>787</v>
+      </c>
+      <c r="H85" s="154"/>
+      <c r="I85" s="154"/>
+      <c r="J85" s="154"/>
+      <c r="K85" s="154"/>
+      <c r="L85" s="154"/>
+      <c r="M85" s="154"/>
+      <c r="N85" s="154"/>
+    </row>
+    <row r="86" spans="3:14" ht="18">
+      <c r="C86" s="131"/>
+      <c r="D86" s="154"/>
+      <c r="E86" s="154"/>
+      <c r="F86" s="154"/>
+      <c r="G86" s="154"/>
+      <c r="H86" s="154"/>
+      <c r="I86" s="154"/>
+      <c r="J86" s="154"/>
+      <c r="K86" s="154"/>
+      <c r="L86" s="154"/>
+      <c r="M86" s="154"/>
+      <c r="N86" s="154"/>
+    </row>
+    <row r="87" spans="3:14" ht="18">
+      <c r="C87" s="131"/>
+      <c r="D87" s="154"/>
+      <c r="E87" s="154"/>
+      <c r="F87" s="154"/>
+      <c r="G87" s="154"/>
+      <c r="H87" s="154"/>
+      <c r="I87" s="154"/>
+      <c r="J87" s="154"/>
+      <c r="K87" s="154"/>
+      <c r="L87" s="154"/>
+      <c r="M87" s="154"/>
+      <c r="N87" s="154"/>
+    </row>
+    <row r="88" spans="3:14" ht="18">
+      <c r="C88" s="131"/>
+      <c r="D88" s="154"/>
+      <c r="E88" s="154"/>
+      <c r="F88" s="154"/>
+      <c r="G88" s="154"/>
+      <c r="H88" s="154"/>
+      <c r="I88" s="154"/>
+      <c r="J88" s="154"/>
+      <c r="K88" s="154"/>
+      <c r="L88" s="154"/>
+      <c r="M88" s="154"/>
+      <c r="N88" s="154"/>
+    </row>
+    <row r="89" spans="3:14" ht="18">
+      <c r="C89" s="131"/>
+      <c r="D89" s="154"/>
+      <c r="E89" s="154"/>
+      <c r="F89" s="154"/>
+      <c r="G89" s="154"/>
+      <c r="H89" s="154"/>
+      <c r="I89" s="154"/>
+      <c r="J89" s="154"/>
+      <c r="K89" s="154"/>
+      <c r="L89" s="154"/>
+      <c r="M89" s="154"/>
+      <c r="N89" s="154"/>
+    </row>
+    <row r="90" spans="3:14" ht="18">
+      <c r="C90" s="131"/>
+      <c r="D90" s="154"/>
+      <c r="E90" s="154"/>
+      <c r="F90" s="154"/>
+      <c r="G90" s="154"/>
+      <c r="H90" s="154"/>
+      <c r="I90" s="154"/>
+      <c r="J90" s="154"/>
+      <c r="K90" s="154"/>
+      <c r="L90" s="154"/>
+      <c r="M90" s="154"/>
+      <c r="N90" s="154"/>
+    </row>
+    <row r="91" spans="3:14" ht="18">
+      <c r="C91" s="131"/>
+      <c r="D91" s="154"/>
+      <c r="E91" s="154"/>
+      <c r="F91" s="154"/>
+      <c r="G91" s="154"/>
+      <c r="H91" s="154"/>
+      <c r="I91" s="154"/>
+      <c r="J91" s="154"/>
+      <c r="K91" s="154"/>
+      <c r="L91" s="154"/>
+      <c r="M91" s="154"/>
+      <c r="N91" s="154"/>
+    </row>
+    <row r="92" spans="3:14" ht="18">
+      <c r="C92" s="131"/>
+      <c r="D92" s="154"/>
+      <c r="E92" s="154"/>
+      <c r="F92" s="154"/>
+      <c r="G92" s="154"/>
+      <c r="H92" s="154"/>
+      <c r="I92" s="154"/>
+      <c r="J92" s="154"/>
+      <c r="K92" s="154"/>
+      <c r="L92" s="154"/>
+      <c r="M92" s="154"/>
+      <c r="N92" s="154"/>
+    </row>
+    <row r="93" spans="3:14" ht="19" thickBot="1">
+      <c r="C93" s="131"/>
+      <c r="D93" s="154"/>
+      <c r="E93" s="154"/>
+      <c r="F93" s="154"/>
+      <c r="G93" s="154"/>
+      <c r="H93" s="154"/>
+      <c r="I93" s="154"/>
+      <c r="J93" s="154"/>
+      <c r="K93" s="154"/>
+      <c r="L93" s="154"/>
+      <c r="M93" s="154"/>
+      <c r="N93" s="154"/>
+    </row>
+    <row r="94" spans="3:14" ht="17" thickBot="1">
+      <c r="C94" s="121"/>
+      <c r="D94" s="123"/>
+      <c r="E94" s="123"/>
+      <c r="F94" s="123"/>
+      <c r="G94" s="123"/>
+      <c r="H94" s="123"/>
+      <c r="I94" s="123"/>
+      <c r="J94" s="123"/>
+      <c r="K94" s="123"/>
+      <c r="L94" s="123"/>
+      <c r="M94" s="123"/>
+      <c r="N94" s="124"/>
+    </row>
+    <row r="95" spans="3:14" ht="18">
+      <c r="C95" s="136" t="s">
         <v>816</v>
       </c>
-      <c r="D62" s="164"/>
-      <c r="E62" s="164" t="s">
-        <v>788</v>
-      </c>
-      <c r="F62" s="164"/>
-      <c r="G62" s="164"/>
-      <c r="H62" s="164"/>
-      <c r="I62" s="164"/>
-      <c r="J62" s="164"/>
-      <c r="K62" s="164"/>
-    </row>
-    <row r="63" spans="3:11" ht="18">
-      <c r="C63" s="141" t="s">
-        <v>808</v>
-      </c>
-      <c r="D63" s="164"/>
-      <c r="E63" s="164" t="s">
-        <v>788</v>
-      </c>
-      <c r="F63" s="164"/>
-      <c r="G63" s="164"/>
-      <c r="H63" s="164"/>
-      <c r="I63" s="164"/>
-      <c r="J63" s="164"/>
-      <c r="K63" s="164"/>
-    </row>
-    <row r="64" spans="3:11" ht="18">
-      <c r="C64" s="142" t="s">
-        <v>803</v>
-      </c>
-      <c r="D64" s="165"/>
-      <c r="E64" s="165" t="s">
-        <v>788</v>
-      </c>
-      <c r="F64" s="165"/>
-      <c r="G64" s="165"/>
-      <c r="H64" s="165"/>
-      <c r="I64" s="165"/>
-      <c r="J64" s="165"/>
-      <c r="K64" s="165"/>
-    </row>
-    <row r="65" spans="3:11" ht="18">
-      <c r="C65" s="142"/>
-      <c r="D65" s="165"/>
-      <c r="E65" s="165"/>
-      <c r="F65" s="165"/>
-      <c r="G65" s="165"/>
-      <c r="H65" s="165"/>
-      <c r="I65" s="165"/>
-      <c r="J65" s="165"/>
-      <c r="K65" s="165"/>
-    </row>
-    <row r="66" spans="3:11" ht="18">
-      <c r="C66" s="142"/>
-      <c r="D66" s="165"/>
-      <c r="E66" s="165"/>
-      <c r="F66" s="165"/>
-      <c r="G66" s="165"/>
-      <c r="H66" s="165"/>
-      <c r="I66" s="165"/>
-      <c r="J66" s="165"/>
-      <c r="K66" s="165"/>
-    </row>
-    <row r="67" spans="3:11" ht="18">
-      <c r="C67" s="142"/>
-      <c r="D67" s="165"/>
-      <c r="E67" s="165"/>
-      <c r="F67" s="165"/>
-      <c r="G67" s="165"/>
-      <c r="H67" s="165"/>
-      <c r="I67" s="165"/>
-      <c r="J67" s="165"/>
-      <c r="K67" s="165"/>
-    </row>
-    <row r="68" spans="3:11" ht="19" thickBot="1">
-      <c r="C68" s="142"/>
-      <c r="D68" s="165"/>
-      <c r="E68" s="165"/>
-      <c r="F68" s="165"/>
-      <c r="G68" s="165"/>
-      <c r="H68" s="165"/>
-      <c r="I68" s="165"/>
-      <c r="J68" s="165"/>
-      <c r="K68" s="165"/>
-    </row>
-    <row r="69" spans="3:11" ht="17" thickBot="1">
-      <c r="C69" s="131"/>
-      <c r="D69" s="133"/>
-      <c r="E69" s="133"/>
-      <c r="F69" s="133"/>
-      <c r="G69" s="133"/>
-      <c r="H69" s="133"/>
-      <c r="I69" s="133"/>
-      <c r="J69" s="133"/>
-      <c r="K69" s="134"/>
-    </row>
-    <row r="70" spans="3:11" ht="18">
-      <c r="C70" s="147" t="s">
+      <c r="D95" s="155"/>
+      <c r="E95" s="155"/>
+      <c r="F95" s="155"/>
+      <c r="G95" s="155"/>
+      <c r="H95" s="155"/>
+      <c r="I95" s="155"/>
+      <c r="J95" s="155"/>
+      <c r="K95" s="155"/>
+      <c r="L95" s="155"/>
+      <c r="M95" s="155"/>
+      <c r="N95" s="155"/>
+    </row>
+    <row r="96" spans="3:14" ht="19">
+      <c r="C96" s="133" t="s">
         <v>817</v>
       </c>
-      <c r="D70" s="166"/>
-      <c r="E70" s="166"/>
-      <c r="F70" s="166"/>
-      <c r="G70" s="166"/>
-      <c r="H70" s="166"/>
-      <c r="I70" s="166"/>
-      <c r="J70" s="166"/>
-      <c r="K70" s="166"/>
-    </row>
-    <row r="71" spans="3:11" ht="19">
-      <c r="C71" s="144" t="s">
+      <c r="D96" s="156"/>
+      <c r="E96" s="156" t="s">
+        <v>787</v>
+      </c>
+      <c r="F96" s="156"/>
+      <c r="G96" s="156"/>
+      <c r="H96" s="156"/>
+      <c r="I96" s="156"/>
+      <c r="J96" s="156"/>
+      <c r="K96" s="156"/>
+      <c r="L96" s="156"/>
+      <c r="M96" s="156"/>
+      <c r="N96" s="156"/>
+    </row>
+    <row r="97" spans="3:14" ht="18">
+      <c r="C97" s="133"/>
+      <c r="D97" s="156"/>
+      <c r="E97" s="156"/>
+      <c r="F97" s="156"/>
+      <c r="G97" s="156"/>
+      <c r="H97" s="156"/>
+      <c r="I97" s="156"/>
+      <c r="J97" s="156"/>
+      <c r="K97" s="156"/>
+      <c r="L97" s="156"/>
+      <c r="M97" s="156"/>
+      <c r="N97" s="156"/>
+    </row>
+    <row r="98" spans="3:14" ht="18">
+      <c r="C98" s="133"/>
+      <c r="D98" s="156"/>
+      <c r="E98" s="156"/>
+      <c r="F98" s="156"/>
+      <c r="G98" s="156"/>
+      <c r="H98" s="156"/>
+      <c r="I98" s="156"/>
+      <c r="J98" s="156"/>
+      <c r="K98" s="156"/>
+      <c r="L98" s="156"/>
+      <c r="M98" s="156"/>
+      <c r="N98" s="156"/>
+    </row>
+    <row r="99" spans="3:14" ht="18">
+      <c r="C99" s="133"/>
+      <c r="D99" s="156"/>
+      <c r="E99" s="156"/>
+      <c r="F99" s="156"/>
+      <c r="G99" s="156"/>
+      <c r="H99" s="156"/>
+      <c r="I99" s="156"/>
+      <c r="J99" s="156"/>
+      <c r="K99" s="156"/>
+      <c r="L99" s="156"/>
+      <c r="M99" s="156"/>
+      <c r="N99" s="156"/>
+    </row>
+    <row r="100" spans="3:14">
+      <c r="C100" s="134"/>
+      <c r="D100" s="157"/>
+      <c r="E100" s="157"/>
+      <c r="F100" s="157"/>
+      <c r="G100" s="157"/>
+      <c r="H100" s="157"/>
+      <c r="I100" s="157"/>
+      <c r="J100" s="157"/>
+      <c r="K100" s="157"/>
+      <c r="L100" s="157"/>
+      <c r="M100" s="157"/>
+      <c r="N100" s="157"/>
+    </row>
+    <row r="101" spans="3:14" ht="17" thickBot="1">
+      <c r="C101" s="135"/>
+      <c r="D101" s="158"/>
+      <c r="E101" s="158"/>
+      <c r="F101" s="158"/>
+      <c r="G101" s="158"/>
+      <c r="H101" s="158"/>
+      <c r="I101" s="158"/>
+      <c r="J101" s="158"/>
+      <c r="K101" s="158"/>
+      <c r="L101" s="158"/>
+      <c r="M101" s="158"/>
+      <c r="N101" s="158"/>
+    </row>
+    <row r="102" spans="3:14" ht="17" thickBot="1">
+      <c r="C102" s="170"/>
+      <c r="D102" s="175"/>
+      <c r="E102" s="174"/>
+      <c r="F102" s="110"/>
+      <c r="G102" s="110"/>
+      <c r="H102" s="110"/>
+      <c r="I102" s="110"/>
+      <c r="J102" s="110"/>
+      <c r="K102" s="110"/>
+      <c r="L102" s="110"/>
+      <c r="M102" s="110"/>
+      <c r="N102" s="125"/>
+    </row>
+    <row r="103" spans="3:14" ht="18">
+      <c r="C103" s="171" t="s">
         <v>818</v>
       </c>
-      <c r="D71" s="167"/>
-      <c r="E71" s="167" t="s">
-        <v>788</v>
-      </c>
-      <c r="F71" s="167"/>
-      <c r="G71" s="167"/>
-      <c r="H71" s="167"/>
-      <c r="I71" s="167"/>
-      <c r="J71" s="167"/>
-      <c r="K71" s="167"/>
-    </row>
-    <row r="72" spans="3:11" ht="18">
-      <c r="C72" s="144"/>
-      <c r="D72" s="167"/>
-      <c r="E72" s="167"/>
-      <c r="F72" s="167"/>
-      <c r="G72" s="167"/>
-      <c r="H72" s="167"/>
-      <c r="I72" s="167"/>
-      <c r="J72" s="167"/>
-      <c r="K72" s="167"/>
-    </row>
-    <row r="73" spans="3:11" ht="18">
-      <c r="C73" s="144"/>
-      <c r="D73" s="167"/>
-      <c r="E73" s="167"/>
-      <c r="F73" s="167"/>
-      <c r="G73" s="167"/>
-      <c r="H73" s="167"/>
-      <c r="I73" s="167"/>
-      <c r="J73" s="167"/>
-      <c r="K73" s="167"/>
-    </row>
-    <row r="74" spans="3:11" ht="18">
-      <c r="C74" s="144"/>
-      <c r="D74" s="167"/>
-      <c r="E74" s="167"/>
-      <c r="F74" s="167"/>
-      <c r="G74" s="167"/>
-      <c r="H74" s="167"/>
-      <c r="I74" s="167"/>
-      <c r="J74" s="167"/>
-      <c r="K74" s="167"/>
-    </row>
-    <row r="75" spans="3:11">
-      <c r="C75" s="145"/>
-      <c r="D75" s="168"/>
-      <c r="E75" s="168"/>
-      <c r="F75" s="168"/>
-      <c r="G75" s="168"/>
-      <c r="H75" s="168"/>
-      <c r="I75" s="168"/>
-      <c r="J75" s="168"/>
-      <c r="K75" s="168"/>
-    </row>
-    <row r="76" spans="3:11" ht="17" thickBot="1">
-      <c r="C76" s="146"/>
-      <c r="D76" s="169"/>
-      <c r="E76" s="169"/>
-      <c r="F76" s="169"/>
-      <c r="G76" s="169"/>
-      <c r="H76" s="169"/>
-      <c r="I76" s="169"/>
-      <c r="J76" s="169"/>
-      <c r="K76" s="169"/>
-    </row>
-    <row r="77" spans="3:11" ht="17" thickBot="1">
-      <c r="C77" s="181"/>
-      <c r="D77" s="186"/>
-      <c r="E77" s="185"/>
-      <c r="F77" s="118"/>
-      <c r="G77" s="118"/>
-      <c r="H77" s="118"/>
-      <c r="I77" s="118"/>
-      <c r="J77" s="118"/>
-      <c r="K77" s="135"/>
-    </row>
-    <row r="78" spans="3:11" ht="18">
-      <c r="C78" s="182" t="s">
+      <c r="D103" s="159"/>
+      <c r="E103" s="159"/>
+      <c r="F103" s="159"/>
+      <c r="G103" s="159"/>
+      <c r="H103" s="159"/>
+      <c r="I103" s="159"/>
+      <c r="J103" s="159"/>
+      <c r="K103" s="159"/>
+      <c r="L103" s="159"/>
+      <c r="M103" s="162"/>
+      <c r="N103" s="159"/>
+    </row>
+    <row r="104" spans="3:14" ht="18">
+      <c r="C104" s="172" t="s">
+        <v>839</v>
+      </c>
+      <c r="D104" s="176"/>
+      <c r="E104" s="177" t="s">
+        <v>787</v>
+      </c>
+      <c r="F104" s="177" t="s">
+        <v>787</v>
+      </c>
+      <c r="G104" s="176"/>
+      <c r="H104" s="177"/>
+      <c r="I104" s="176"/>
+      <c r="J104" s="176"/>
+      <c r="K104" s="176"/>
+      <c r="L104" s="176"/>
+      <c r="M104" s="168"/>
+      <c r="N104" s="166"/>
+    </row>
+    <row r="105" spans="3:14" ht="18">
+      <c r="C105" s="172" t="s">
         <v>819</v>
       </c>
-      <c r="D78" s="170"/>
-      <c r="E78" s="170"/>
-      <c r="F78" s="170"/>
-      <c r="G78" s="170"/>
-      <c r="H78" s="170"/>
-      <c r="I78" s="170"/>
-      <c r="J78" s="173"/>
-      <c r="K78" s="170"/>
-    </row>
-    <row r="79" spans="3:11" ht="18">
-      <c r="C79" s="183" t="s">
-        <v>820</v>
-      </c>
-      <c r="D79" s="187"/>
-      <c r="E79" s="188" t="s">
-        <v>788</v>
-      </c>
-      <c r="F79" s="187"/>
-      <c r="G79" s="187"/>
-      <c r="H79" s="187"/>
-      <c r="I79" s="187"/>
-      <c r="J79" s="179"/>
-      <c r="K79" s="177"/>
-    </row>
-    <row r="80" spans="3:11" ht="18">
-      <c r="C80" s="183" t="s">
-        <v>821</v>
-      </c>
-      <c r="D80" s="188"/>
-      <c r="E80" s="188" t="s">
-        <v>788</v>
-      </c>
-      <c r="F80" s="188"/>
-      <c r="G80" s="188"/>
-      <c r="H80" s="188"/>
-      <c r="I80" s="188"/>
-      <c r="J80" s="180"/>
-      <c r="K80" s="178"/>
-    </row>
-    <row r="81" spans="3:11" ht="18">
-      <c r="C81" s="176"/>
-      <c r="D81" s="188"/>
-      <c r="E81" s="188"/>
-      <c r="F81" s="188"/>
-      <c r="G81" s="188"/>
-      <c r="H81" s="188"/>
-      <c r="I81" s="188"/>
-      <c r="J81" s="180"/>
-      <c r="K81" s="178"/>
-    </row>
-    <row r="82" spans="3:11" ht="18">
-      <c r="C82" s="176"/>
-      <c r="D82" s="188"/>
-      <c r="E82" s="188"/>
-      <c r="F82" s="188"/>
-      <c r="G82" s="188"/>
-      <c r="H82" s="188"/>
-      <c r="I82" s="188"/>
-      <c r="J82" s="180"/>
-      <c r="K82" s="178"/>
-    </row>
-    <row r="83" spans="3:11" ht="18">
-      <c r="C83" s="176"/>
-      <c r="D83" s="188"/>
-      <c r="E83" s="188"/>
-      <c r="F83" s="188"/>
-      <c r="G83" s="188"/>
-      <c r="H83" s="188"/>
-      <c r="I83" s="188"/>
-      <c r="J83" s="180"/>
-      <c r="K83" s="178"/>
-    </row>
-    <row r="84" spans="3:11" ht="18">
-      <c r="C84" s="183"/>
-      <c r="D84" s="171"/>
-      <c r="E84" s="171"/>
-      <c r="F84" s="171"/>
-      <c r="G84" s="171"/>
-      <c r="H84" s="171"/>
-      <c r="I84" s="171"/>
-      <c r="J84" s="174"/>
-      <c r="K84" s="171"/>
-    </row>
-    <row r="85" spans="3:11" ht="19" thickBot="1">
-      <c r="C85" s="184"/>
-      <c r="D85" s="172"/>
-      <c r="E85" s="172"/>
-      <c r="F85" s="172"/>
-      <c r="G85" s="172"/>
-      <c r="H85" s="172"/>
-      <c r="I85" s="172"/>
-      <c r="J85" s="175"/>
-      <c r="K85" s="172"/>
+      <c r="D105" s="177"/>
+      <c r="E105" s="177" t="s">
+        <v>787</v>
+      </c>
+      <c r="F105" s="177" t="s">
+        <v>787</v>
+      </c>
+      <c r="G105" s="177"/>
+      <c r="H105" s="177"/>
+      <c r="I105" s="177"/>
+      <c r="J105" s="177"/>
+      <c r="K105" s="177"/>
+      <c r="L105" s="177"/>
+      <c r="M105" s="169"/>
+      <c r="N105" s="167"/>
+    </row>
+    <row r="106" spans="3:14" ht="18">
+      <c r="C106" s="165"/>
+      <c r="D106" s="177"/>
+      <c r="E106" s="177"/>
+      <c r="F106" s="177"/>
+      <c r="G106" s="177"/>
+      <c r="H106" s="177"/>
+      <c r="I106" s="177"/>
+      <c r="J106" s="177"/>
+      <c r="K106" s="177"/>
+      <c r="L106" s="177"/>
+      <c r="M106" s="169"/>
+      <c r="N106" s="167"/>
+    </row>
+    <row r="107" spans="3:14" ht="18">
+      <c r="C107" s="165"/>
+      <c r="D107" s="177"/>
+      <c r="E107" s="177"/>
+      <c r="F107" s="177"/>
+      <c r="G107" s="177"/>
+      <c r="H107" s="177"/>
+      <c r="I107" s="177"/>
+      <c r="J107" s="177"/>
+      <c r="K107" s="177"/>
+      <c r="L107" s="177"/>
+      <c r="M107" s="169"/>
+      <c r="N107" s="167"/>
+    </row>
+    <row r="108" spans="3:14" ht="18">
+      <c r="C108" s="165"/>
+      <c r="D108" s="177"/>
+      <c r="E108" s="177"/>
+      <c r="F108" s="177"/>
+      <c r="G108" s="177"/>
+      <c r="H108" s="177"/>
+      <c r="I108" s="177"/>
+      <c r="J108" s="177"/>
+      <c r="K108" s="177"/>
+      <c r="L108" s="177"/>
+      <c r="M108" s="169"/>
+      <c r="N108" s="167"/>
+    </row>
+    <row r="109" spans="3:14" ht="18">
+      <c r="C109" s="172"/>
+      <c r="D109" s="160"/>
+      <c r="E109" s="160"/>
+      <c r="F109" s="160"/>
+      <c r="G109" s="160"/>
+      <c r="H109" s="160"/>
+      <c r="I109" s="160"/>
+      <c r="J109" s="160"/>
+      <c r="K109" s="160"/>
+      <c r="L109" s="160"/>
+      <c r="M109" s="163"/>
+      <c r="N109" s="160"/>
+    </row>
+    <row r="110" spans="3:14" ht="19" thickBot="1">
+      <c r="C110" s="173"/>
+      <c r="D110" s="161"/>
+      <c r="E110" s="161"/>
+      <c r="F110" s="161"/>
+      <c r="G110" s="161"/>
+      <c r="H110" s="161"/>
+      <c r="I110" s="161"/>
+      <c r="J110" s="161"/>
+      <c r="K110" s="161"/>
+      <c r="L110" s="161"/>
+      <c r="M110" s="164"/>
+      <c r="N110" s="161"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C23" r:id="rId1" location="remove-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - remove-int-" xr:uid="{A3DFFAF1-3C93-B04D-A4B1-EA2A39FBEC91}"/>
-    <hyperlink ref="C59" r:id="rId2" location="isEmpty--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - isEmpty--" xr:uid="{F593362D-789B-7049-A3AA-7B6E2682E976}"/>
-    <hyperlink ref="C26" r:id="rId3" location="removeRange-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - removeRange-int-int-" xr:uid="{D0BFE38E-2B8B-CE41-967A-C3C9EA93BE4E}"/>
-    <hyperlink ref="C29" r:id="rId4" location="clear--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - clear--" xr:uid="{2FFA909C-C109-B14D-8F33-325805174D8D}"/>
-    <hyperlink ref="C37" r:id="rId5" location="get-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - get-int-" xr:uid="{FBBAAF6B-E143-864D-A6C3-F1E24E50E661}"/>
-    <hyperlink ref="C38" r:id="rId6" location="iterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - iterator--" xr:uid="{A075F592-CC84-B840-8050-836C5620A000}"/>
-    <hyperlink ref="C39" r:id="rId7" location="listIterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - listIterator--" xr:uid="{F4F1EE1C-1937-BB49-B4F9-158A67374360}"/>
-    <hyperlink ref="C40" r:id="rId8" location="spliterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - spliterator--" xr:uid="{ECABA72C-AD77-1C4F-B3FC-B32A74B26EC8}"/>
-    <hyperlink ref="C63" r:id="rId9" location="subList-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - subList-int-int-" xr:uid="{1EB080CA-5D98-3844-A4A2-E79CA8CD8EBB}"/>
-    <hyperlink ref="C58" r:id="rId10" location="size--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - size--" xr:uid="{D71DFD34-DFF3-DA45-BA53-9457F025CBE6}"/>
-    <hyperlink ref="C79" r:id="rId11" tooltip="class in java.lang" display="https://docs.oracle.com/javase/8/docs/api/java/lang/Object.html" xr:uid="{80E00372-253A-5E46-B2A9-FAFBDA183C46}"/>
+    <hyperlink ref="C28" r:id="rId1" location="remove-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - remove-int-" xr:uid="{A3DFFAF1-3C93-B04D-A4B1-EA2A39FBEC91}"/>
+    <hyperlink ref="C78" r:id="rId2" location="isEmpty--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - isEmpty--" xr:uid="{F593362D-789B-7049-A3AA-7B6E2682E976}"/>
+    <hyperlink ref="C31" r:id="rId3" location="removeRange-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - removeRange-int-int-" xr:uid="{D0BFE38E-2B8B-CE41-967A-C3C9EA93BE4E}"/>
+    <hyperlink ref="C34" r:id="rId4" location="clear--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - clear--" xr:uid="{2FFA909C-C109-B14D-8F33-325805174D8D}"/>
+    <hyperlink ref="C47" r:id="rId5" location="get-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - get-int-" xr:uid="{FBBAAF6B-E143-864D-A6C3-F1E24E50E661}"/>
+    <hyperlink ref="C48" r:id="rId6" location="iterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - iterator--" xr:uid="{A075F592-CC84-B840-8050-836C5620A000}"/>
+    <hyperlink ref="C49" r:id="rId7" location="listIterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - listIterator--" xr:uid="{F4F1EE1C-1937-BB49-B4F9-158A67374360}"/>
+    <hyperlink ref="C50" r:id="rId8" location="spliterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - spliterator--" xr:uid="{ECABA72C-AD77-1C4F-B3FC-B32A74B26EC8}"/>
+    <hyperlink ref="C82" r:id="rId9" location="subList-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - subList-int-int-" xr:uid="{1EB080CA-5D98-3844-A4A2-E79CA8CD8EBB}"/>
+    <hyperlink ref="C77" r:id="rId10" location="size--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - size--" xr:uid="{D71DFD34-DFF3-DA45-BA53-9457F025CBE6}"/>
+    <hyperlink ref="C104" r:id="rId11" tooltip="class in java.lang" display="https://docs.oracle.com/javase/8/docs/api/java/lang/Object.html" xr:uid="{80E00372-253A-5E46-B2A9-FAFBDA183C46}"/>
+    <hyperlink ref="C52" r:id="rId12" location="getFirst()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - getFirst()" xr:uid="{8BDAB115-0121-3940-B451-BF302CE8770F}"/>
+    <hyperlink ref="C53" r:id="rId13" location="getLast()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - getLast()" xr:uid="{8393D593-5133-A241-BE7A-9F172C52B66B}"/>
+    <hyperlink ref="C54" r:id="rId14" location="peek()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - peek()" xr:uid="{0CEF2AF3-6D6C-9046-BE93-019C40035281}"/>
+    <hyperlink ref="C55" r:id="rId15" location="peekFirst()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - peekFirst()" xr:uid="{C7D7CFAE-8875-9348-94AD-F5F108408698}"/>
+    <hyperlink ref="C56" r:id="rId16" location="peekLast()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - peekLast()" xr:uid="{83BC5C8D-C1F5-FE46-A065-ECB050A6ECD0}"/>
+    <hyperlink ref="C35" r:id="rId17" location="poll()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - poll()" xr:uid="{8242EE68-D381-0941-87E8-C08B2EFCDCE1}"/>
+    <hyperlink ref="C40" r:id="rId18" location="removeFirst()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - removeFirst()" xr:uid="{59C4D3D0-5891-744A-BA52-0FE35B2643B4}"/>
+    <hyperlink ref="C41" r:id="rId19" location="removeLast()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - removeLast()" xr:uid="{DC2BE068-F09F-2443-B88D-91E77B963F1D}"/>
+    <hyperlink ref="C85" r:id="rId20" tooltip="class in java.lang" display="https://docs.oracle.com/javase/7/docs/api/java/lang/Object.html" xr:uid="{AFDBA6F5-E5D2-A442-8152-52E12532F525}"/>
+    <hyperlink ref="C38" r:id="rId21" location="pop()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - pop()" xr:uid="{ECBDC240-CEB4-A74E-8A39-3B4C3D4E658E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add methods summary of priority queue
</commit_message>
<xml_diff>
--- a/Leetcode-tag record.xlsx
+++ b/Leetcode-tag record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiahsing/git-repositories/workspace-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD00678-4D32-5E4C-992C-897E686AE746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDBCC0E-58D5-AC40-A3AA-AB4DD87C9A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29680" yWindow="500" windowWidth="29000" windowHeight="26640" activeTab="2" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
+    <workbookView xWindow="26320" yWindow="960" windowWidth="29000" windowHeight="26640" activeTab="2" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="845">
   <si>
     <t>Array</t>
   </si>
@@ -3333,6 +3333,9 @@
       </rPr>
       <t>- interface</t>
     </r>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -4757,6 +4760,24 @@
     <xf numFmtId="0" fontId="11" fillId="49" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4769,25 +4790,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="43" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="44" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5140,27 +5143,27 @@
   <sheetData>
     <row r="1" spans="2:21" ht="17" thickBot="1"/>
     <row r="2" spans="2:21" ht="17" thickBot="1">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="186"/>
-      <c r="I2" s="186"/>
-      <c r="J2" s="186"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="186"/>
-      <c r="M2" s="186"/>
-      <c r="N2" s="186"/>
-      <c r="O2" s="186"/>
-      <c r="P2" s="187"/>
-      <c r="R2" s="184"/>
-      <c r="S2" s="184"/>
-      <c r="T2" s="184"/>
-      <c r="U2" s="184"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="185"/>
+      <c r="M2" s="185"/>
+      <c r="N2" s="185"/>
+      <c r="O2" s="185"/>
+      <c r="P2" s="186"/>
+      <c r="R2" s="190"/>
+      <c r="S2" s="190"/>
+      <c r="T2" s="190"/>
+      <c r="U2" s="190"/>
     </row>
     <row r="3" spans="2:21" ht="17" thickBot="1">
       <c r="B3" s="25" t="s">
@@ -5532,8 +5535,8 @@
       <c r="N15" s="42"/>
       <c r="O15" s="15"/>
       <c r="P15" s="17"/>
-      <c r="R15" s="184"/>
-      <c r="S15" s="184"/>
+      <c r="R15" s="190"/>
+      <c r="S15" s="190"/>
       <c r="T15" s="102"/>
       <c r="U15" s="102"/>
     </row>
@@ -7511,23 +7514,23 @@
       <c r="P98" s="45"/>
     </row>
     <row r="99" spans="2:16" ht="17" thickBot="1">
-      <c r="B99" s="185" t="s">
+      <c r="B99" s="184" t="s">
         <v>101</v>
       </c>
-      <c r="C99" s="186"/>
-      <c r="D99" s="186"/>
-      <c r="E99" s="186"/>
-      <c r="F99" s="186"/>
-      <c r="G99" s="186"/>
-      <c r="H99" s="186"/>
-      <c r="I99" s="186"/>
-      <c r="J99" s="186"/>
-      <c r="K99" s="186"/>
-      <c r="L99" s="186"/>
-      <c r="M99" s="186"/>
-      <c r="N99" s="186"/>
-      <c r="O99" s="186"/>
-      <c r="P99" s="187"/>
+      <c r="C99" s="185"/>
+      <c r="D99" s="185"/>
+      <c r="E99" s="185"/>
+      <c r="F99" s="185"/>
+      <c r="G99" s="185"/>
+      <c r="H99" s="185"/>
+      <c r="I99" s="185"/>
+      <c r="J99" s="185"/>
+      <c r="K99" s="185"/>
+      <c r="L99" s="185"/>
+      <c r="M99" s="185"/>
+      <c r="N99" s="185"/>
+      <c r="O99" s="185"/>
+      <c r="P99" s="186"/>
     </row>
     <row r="100" spans="2:16" ht="17" thickBot="1">
       <c r="B100" s="25" t="s">
@@ -9941,23 +9944,23 @@
       <c r="P208" s="45"/>
     </row>
     <row r="209" spans="2:16" ht="17" thickBot="1">
-      <c r="B209" s="185" t="s">
+      <c r="B209" s="184" t="s">
         <v>166</v>
       </c>
-      <c r="C209" s="186"/>
-      <c r="D209" s="186"/>
-      <c r="E209" s="186"/>
-      <c r="F209" s="186"/>
-      <c r="G209" s="186"/>
-      <c r="H209" s="186"/>
-      <c r="I209" s="186"/>
-      <c r="J209" s="186"/>
-      <c r="K209" s="186"/>
-      <c r="L209" s="186"/>
-      <c r="M209" s="186"/>
-      <c r="N209" s="186"/>
-      <c r="O209" s="186"/>
-      <c r="P209" s="187"/>
+      <c r="C209" s="185"/>
+      <c r="D209" s="185"/>
+      <c r="E209" s="185"/>
+      <c r="F209" s="185"/>
+      <c r="G209" s="185"/>
+      <c r="H209" s="185"/>
+      <c r="I209" s="185"/>
+      <c r="J209" s="185"/>
+      <c r="K209" s="185"/>
+      <c r="L209" s="185"/>
+      <c r="M209" s="185"/>
+      <c r="N209" s="185"/>
+      <c r="O209" s="185"/>
+      <c r="P209" s="186"/>
     </row>
     <row r="210" spans="2:16" ht="17" thickBot="1">
       <c r="B210" s="25" t="s">
@@ -11438,23 +11441,23 @@
       <c r="P273" s="45"/>
     </row>
     <row r="274" spans="2:16" ht="17" thickBot="1">
-      <c r="B274" s="185" t="s">
+      <c r="B274" s="184" t="s">
         <v>43</v>
       </c>
-      <c r="C274" s="186"/>
-      <c r="D274" s="186"/>
-      <c r="E274" s="186"/>
-      <c r="F274" s="186"/>
-      <c r="G274" s="186"/>
-      <c r="H274" s="186"/>
-      <c r="I274" s="186"/>
-      <c r="J274" s="186"/>
-      <c r="K274" s="186"/>
-      <c r="L274" s="186"/>
-      <c r="M274" s="186"/>
-      <c r="N274" s="186"/>
-      <c r="O274" s="186"/>
-      <c r="P274" s="187"/>
+      <c r="C274" s="185"/>
+      <c r="D274" s="185"/>
+      <c r="E274" s="185"/>
+      <c r="F274" s="185"/>
+      <c r="G274" s="185"/>
+      <c r="H274" s="185"/>
+      <c r="I274" s="185"/>
+      <c r="J274" s="185"/>
+      <c r="K274" s="185"/>
+      <c r="L274" s="185"/>
+      <c r="M274" s="185"/>
+      <c r="N274" s="185"/>
+      <c r="O274" s="185"/>
+      <c r="P274" s="186"/>
     </row>
     <row r="275" spans="2:16" ht="17" thickBot="1">
       <c r="B275" s="25" t="s">
@@ -13482,23 +13485,23 @@
       <c r="P363" s="45"/>
     </row>
     <row r="364" spans="2:16" ht="17" thickBot="1">
-      <c r="B364" s="185" t="s">
+      <c r="B364" s="184" t="s">
         <v>255</v>
       </c>
-      <c r="C364" s="186"/>
-      <c r="D364" s="186"/>
-      <c r="E364" s="186"/>
-      <c r="F364" s="186"/>
-      <c r="G364" s="186"/>
-      <c r="H364" s="186"/>
-      <c r="I364" s="186"/>
-      <c r="J364" s="186"/>
-      <c r="K364" s="186"/>
-      <c r="L364" s="186"/>
-      <c r="M364" s="186"/>
-      <c r="N364" s="186"/>
-      <c r="O364" s="186"/>
-      <c r="P364" s="187"/>
+      <c r="C364" s="185"/>
+      <c r="D364" s="185"/>
+      <c r="E364" s="185"/>
+      <c r="F364" s="185"/>
+      <c r="G364" s="185"/>
+      <c r="H364" s="185"/>
+      <c r="I364" s="185"/>
+      <c r="J364" s="185"/>
+      <c r="K364" s="185"/>
+      <c r="L364" s="185"/>
+      <c r="M364" s="185"/>
+      <c r="N364" s="185"/>
+      <c r="O364" s="185"/>
+      <c r="P364" s="186"/>
     </row>
     <row r="365" spans="2:16" ht="17" thickBot="1">
       <c r="B365" s="25" t="s">
@@ -14376,23 +14379,23 @@
       <c r="P401" s="45"/>
     </row>
     <row r="402" spans="2:16" ht="17" thickBot="1">
-      <c r="B402" s="185" t="s">
+      <c r="B402" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C402" s="186"/>
-      <c r="D402" s="186"/>
-      <c r="E402" s="186"/>
-      <c r="F402" s="186"/>
-      <c r="G402" s="186"/>
-      <c r="H402" s="186"/>
-      <c r="I402" s="186"/>
-      <c r="J402" s="186"/>
-      <c r="K402" s="186"/>
-      <c r="L402" s="186"/>
-      <c r="M402" s="186"/>
-      <c r="N402" s="186"/>
-      <c r="O402" s="186"/>
-      <c r="P402" s="187"/>
+      <c r="C402" s="185"/>
+      <c r="D402" s="185"/>
+      <c r="E402" s="185"/>
+      <c r="F402" s="185"/>
+      <c r="G402" s="185"/>
+      <c r="H402" s="185"/>
+      <c r="I402" s="185"/>
+      <c r="J402" s="185"/>
+      <c r="K402" s="185"/>
+      <c r="L402" s="185"/>
+      <c r="M402" s="185"/>
+      <c r="N402" s="185"/>
+      <c r="O402" s="185"/>
+      <c r="P402" s="186"/>
     </row>
     <row r="403" spans="2:16" ht="17" thickBot="1">
       <c r="B403" s="25" t="s">
@@ -15248,23 +15251,23 @@
       <c r="P439" s="45"/>
     </row>
     <row r="440" spans="2:16" ht="17" thickBot="1">
-      <c r="B440" s="185" t="s">
+      <c r="B440" s="184" t="s">
         <v>300</v>
       </c>
-      <c r="C440" s="186"/>
-      <c r="D440" s="186"/>
-      <c r="E440" s="186"/>
-      <c r="F440" s="186"/>
-      <c r="G440" s="186"/>
-      <c r="H440" s="186"/>
-      <c r="I440" s="186"/>
-      <c r="J440" s="186"/>
-      <c r="K440" s="186"/>
-      <c r="L440" s="186"/>
-      <c r="M440" s="186"/>
-      <c r="N440" s="186"/>
-      <c r="O440" s="186"/>
-      <c r="P440" s="187"/>
+      <c r="C440" s="185"/>
+      <c r="D440" s="185"/>
+      <c r="E440" s="185"/>
+      <c r="F440" s="185"/>
+      <c r="G440" s="185"/>
+      <c r="H440" s="185"/>
+      <c r="I440" s="185"/>
+      <c r="J440" s="185"/>
+      <c r="K440" s="185"/>
+      <c r="L440" s="185"/>
+      <c r="M440" s="185"/>
+      <c r="N440" s="185"/>
+      <c r="O440" s="185"/>
+      <c r="P440" s="186"/>
     </row>
     <row r="441" spans="2:16" ht="17" thickBot="1">
       <c r="B441" s="25" t="s">
@@ -16157,23 +16160,23 @@
       <c r="P478" s="45"/>
     </row>
     <row r="479" spans="2:16" ht="17" thickBot="1">
-      <c r="B479" s="185" t="s">
+      <c r="B479" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="C479" s="186"/>
-      <c r="D479" s="186"/>
-      <c r="E479" s="186"/>
-      <c r="F479" s="186"/>
-      <c r="G479" s="186"/>
-      <c r="H479" s="186"/>
-      <c r="I479" s="186"/>
-      <c r="J479" s="186"/>
-      <c r="K479" s="186"/>
-      <c r="L479" s="186"/>
-      <c r="M479" s="186"/>
-      <c r="N479" s="186"/>
-      <c r="O479" s="186"/>
-      <c r="P479" s="187"/>
+      <c r="C479" s="185"/>
+      <c r="D479" s="185"/>
+      <c r="E479" s="185"/>
+      <c r="F479" s="185"/>
+      <c r="G479" s="185"/>
+      <c r="H479" s="185"/>
+      <c r="I479" s="185"/>
+      <c r="J479" s="185"/>
+      <c r="K479" s="185"/>
+      <c r="L479" s="185"/>
+      <c r="M479" s="185"/>
+      <c r="N479" s="185"/>
+      <c r="O479" s="185"/>
+      <c r="P479" s="186"/>
     </row>
     <row r="480" spans="2:16" ht="17" thickBot="1">
       <c r="B480" s="25" t="s">
@@ -16868,23 +16871,23 @@
       <c r="P505" s="45"/>
     </row>
     <row r="506" spans="2:16" ht="17" thickBot="1">
-      <c r="B506" s="185" t="s">
+      <c r="B506" s="184" t="s">
         <v>324</v>
       </c>
-      <c r="C506" s="186"/>
-      <c r="D506" s="186"/>
-      <c r="E506" s="186"/>
-      <c r="F506" s="186"/>
-      <c r="G506" s="186"/>
-      <c r="H506" s="186"/>
-      <c r="I506" s="186"/>
-      <c r="J506" s="186"/>
-      <c r="K506" s="186"/>
-      <c r="L506" s="186"/>
-      <c r="M506" s="186"/>
-      <c r="N506" s="186"/>
-      <c r="O506" s="186"/>
-      <c r="P506" s="187"/>
+      <c r="C506" s="185"/>
+      <c r="D506" s="185"/>
+      <c r="E506" s="185"/>
+      <c r="F506" s="185"/>
+      <c r="G506" s="185"/>
+      <c r="H506" s="185"/>
+      <c r="I506" s="185"/>
+      <c r="J506" s="185"/>
+      <c r="K506" s="185"/>
+      <c r="L506" s="185"/>
+      <c r="M506" s="185"/>
+      <c r="N506" s="185"/>
+      <c r="O506" s="185"/>
+      <c r="P506" s="186"/>
     </row>
     <row r="507" spans="2:16" ht="17" thickBot="1">
       <c r="B507" s="25" t="s">
@@ -17587,23 +17590,23 @@
       <c r="P538" s="45"/>
     </row>
     <row r="539" spans="2:16" ht="17" thickBot="1">
-      <c r="B539" s="185" t="s">
+      <c r="B539" s="184" t="s">
         <v>352</v>
       </c>
-      <c r="C539" s="186"/>
-      <c r="D539" s="186"/>
-      <c r="E539" s="186"/>
-      <c r="F539" s="186"/>
-      <c r="G539" s="186"/>
-      <c r="H539" s="186"/>
-      <c r="I539" s="186"/>
-      <c r="J539" s="186"/>
-      <c r="K539" s="186"/>
-      <c r="L539" s="186"/>
-      <c r="M539" s="186"/>
-      <c r="N539" s="186"/>
-      <c r="O539" s="186"/>
-      <c r="P539" s="187"/>
+      <c r="C539" s="185"/>
+      <c r="D539" s="185"/>
+      <c r="E539" s="185"/>
+      <c r="F539" s="185"/>
+      <c r="G539" s="185"/>
+      <c r="H539" s="185"/>
+      <c r="I539" s="185"/>
+      <c r="J539" s="185"/>
+      <c r="K539" s="185"/>
+      <c r="L539" s="185"/>
+      <c r="M539" s="185"/>
+      <c r="N539" s="185"/>
+      <c r="O539" s="185"/>
+      <c r="P539" s="186"/>
     </row>
     <row r="540" spans="2:16" ht="17" thickBot="1">
       <c r="B540" s="25" t="s">
@@ -18411,23 +18414,23 @@
       <c r="P576" s="45"/>
     </row>
     <row r="577" spans="2:16" ht="17" thickBot="1">
-      <c r="B577" s="185" t="s">
+      <c r="B577" s="184" t="s">
         <v>342</v>
       </c>
-      <c r="C577" s="186"/>
-      <c r="D577" s="186"/>
-      <c r="E577" s="186"/>
-      <c r="F577" s="186"/>
-      <c r="G577" s="186"/>
-      <c r="H577" s="186"/>
-      <c r="I577" s="186"/>
-      <c r="J577" s="186"/>
-      <c r="K577" s="186"/>
-      <c r="L577" s="186"/>
-      <c r="M577" s="186"/>
-      <c r="N577" s="186"/>
-      <c r="O577" s="186"/>
-      <c r="P577" s="187"/>
+      <c r="C577" s="185"/>
+      <c r="D577" s="185"/>
+      <c r="E577" s="185"/>
+      <c r="F577" s="185"/>
+      <c r="G577" s="185"/>
+      <c r="H577" s="185"/>
+      <c r="I577" s="185"/>
+      <c r="J577" s="185"/>
+      <c r="K577" s="185"/>
+      <c r="L577" s="185"/>
+      <c r="M577" s="185"/>
+      <c r="N577" s="185"/>
+      <c r="O577" s="185"/>
+      <c r="P577" s="186"/>
     </row>
     <row r="578" spans="2:16" ht="17" thickBot="1">
       <c r="B578" s="25" t="s">
@@ -18928,23 +18931,23 @@
       <c r="P599" s="45"/>
     </row>
     <row r="600" spans="2:16" ht="17" thickBot="1">
-      <c r="B600" s="185" t="s">
+      <c r="B600" s="184" t="s">
         <v>373</v>
       </c>
-      <c r="C600" s="186"/>
-      <c r="D600" s="186"/>
-      <c r="E600" s="186"/>
-      <c r="F600" s="186"/>
-      <c r="G600" s="186"/>
-      <c r="H600" s="186"/>
-      <c r="I600" s="186"/>
-      <c r="J600" s="186"/>
-      <c r="K600" s="186"/>
-      <c r="L600" s="186"/>
-      <c r="M600" s="186"/>
-      <c r="N600" s="186"/>
-      <c r="O600" s="186"/>
-      <c r="P600" s="187"/>
+      <c r="C600" s="185"/>
+      <c r="D600" s="185"/>
+      <c r="E600" s="185"/>
+      <c r="F600" s="185"/>
+      <c r="G600" s="185"/>
+      <c r="H600" s="185"/>
+      <c r="I600" s="185"/>
+      <c r="J600" s="185"/>
+      <c r="K600" s="185"/>
+      <c r="L600" s="185"/>
+      <c r="M600" s="185"/>
+      <c r="N600" s="185"/>
+      <c r="O600" s="185"/>
+      <c r="P600" s="186"/>
     </row>
     <row r="601" spans="2:16" ht="17" thickBot="1">
       <c r="B601" s="25" t="s">
@@ -19681,23 +19684,23 @@
       <c r="P636" s="45"/>
     </row>
     <row r="637" spans="2:16" ht="17" thickBot="1">
-      <c r="B637" s="185" t="s">
+      <c r="B637" s="184" t="s">
         <v>387</v>
       </c>
-      <c r="C637" s="186"/>
-      <c r="D637" s="186"/>
-      <c r="E637" s="186"/>
-      <c r="F637" s="186"/>
-      <c r="G637" s="186"/>
-      <c r="H637" s="186"/>
-      <c r="I637" s="186"/>
-      <c r="J637" s="186"/>
-      <c r="K637" s="186"/>
-      <c r="L637" s="186"/>
-      <c r="M637" s="186"/>
-      <c r="N637" s="186"/>
-      <c r="O637" s="186"/>
-      <c r="P637" s="187"/>
+      <c r="C637" s="185"/>
+      <c r="D637" s="185"/>
+      <c r="E637" s="185"/>
+      <c r="F637" s="185"/>
+      <c r="G637" s="185"/>
+      <c r="H637" s="185"/>
+      <c r="I637" s="185"/>
+      <c r="J637" s="185"/>
+      <c r="K637" s="185"/>
+      <c r="L637" s="185"/>
+      <c r="M637" s="185"/>
+      <c r="N637" s="185"/>
+      <c r="O637" s="185"/>
+      <c r="P637" s="186"/>
     </row>
     <row r="638" spans="2:16" ht="17" thickBot="1">
       <c r="B638" s="25" t="s">
@@ -19951,23 +19954,23 @@
       <c r="P648" s="45"/>
     </row>
     <row r="649" spans="2:16" ht="17" thickBot="1">
-      <c r="B649" s="185" t="s">
+      <c r="B649" s="184" t="s">
         <v>391</v>
       </c>
-      <c r="C649" s="186"/>
-      <c r="D649" s="186"/>
-      <c r="E649" s="186"/>
-      <c r="F649" s="186"/>
-      <c r="G649" s="186"/>
-      <c r="H649" s="186"/>
-      <c r="I649" s="186"/>
-      <c r="J649" s="186"/>
-      <c r="K649" s="186"/>
-      <c r="L649" s="186"/>
-      <c r="M649" s="186"/>
-      <c r="N649" s="186"/>
-      <c r="O649" s="186"/>
-      <c r="P649" s="187"/>
+      <c r="C649" s="185"/>
+      <c r="D649" s="185"/>
+      <c r="E649" s="185"/>
+      <c r="F649" s="185"/>
+      <c r="G649" s="185"/>
+      <c r="H649" s="185"/>
+      <c r="I649" s="185"/>
+      <c r="J649" s="185"/>
+      <c r="K649" s="185"/>
+      <c r="L649" s="185"/>
+      <c r="M649" s="185"/>
+      <c r="N649" s="185"/>
+      <c r="O649" s="185"/>
+      <c r="P649" s="186"/>
     </row>
     <row r="650" spans="2:16" ht="17" thickBot="1">
       <c r="B650" s="25" t="s">
@@ -20469,23 +20472,23 @@
       <c r="P674" s="45"/>
     </row>
     <row r="675" spans="2:16" ht="17" thickBot="1">
-      <c r="B675" s="181" t="s">
+      <c r="B675" s="187" t="s">
         <v>398</v>
       </c>
-      <c r="C675" s="182"/>
-      <c r="D675" s="182"/>
-      <c r="E675" s="182"/>
-      <c r="F675" s="182"/>
-      <c r="G675" s="182"/>
-      <c r="H675" s="182"/>
-      <c r="I675" s="182"/>
-      <c r="J675" s="182"/>
-      <c r="K675" s="182"/>
-      <c r="L675" s="182"/>
-      <c r="M675" s="182"/>
-      <c r="N675" s="182"/>
-      <c r="O675" s="182"/>
-      <c r="P675" s="183"/>
+      <c r="C675" s="188"/>
+      <c r="D675" s="188"/>
+      <c r="E675" s="188"/>
+      <c r="F675" s="188"/>
+      <c r="G675" s="188"/>
+      <c r="H675" s="188"/>
+      <c r="I675" s="188"/>
+      <c r="J675" s="188"/>
+      <c r="K675" s="188"/>
+      <c r="L675" s="188"/>
+      <c r="M675" s="188"/>
+      <c r="N675" s="188"/>
+      <c r="O675" s="188"/>
+      <c r="P675" s="189"/>
     </row>
     <row r="676" spans="2:16" ht="17" thickBot="1">
       <c r="B676" s="49" t="s">
@@ -21054,23 +21057,23 @@
       <c r="P703" s="45"/>
     </row>
     <row r="704" spans="2:16" ht="17" thickBot="1">
-      <c r="B704" s="181" t="s">
+      <c r="B704" s="187" t="s">
         <v>408</v>
       </c>
-      <c r="C704" s="182"/>
-      <c r="D704" s="182"/>
-      <c r="E704" s="182"/>
-      <c r="F704" s="182"/>
-      <c r="G704" s="182"/>
-      <c r="H704" s="182"/>
-      <c r="I704" s="182"/>
-      <c r="J704" s="182"/>
-      <c r="K704" s="182"/>
-      <c r="L704" s="182"/>
-      <c r="M704" s="182"/>
-      <c r="N704" s="182"/>
-      <c r="O704" s="182"/>
-      <c r="P704" s="183"/>
+      <c r="C704" s="188"/>
+      <c r="D704" s="188"/>
+      <c r="E704" s="188"/>
+      <c r="F704" s="188"/>
+      <c r="G704" s="188"/>
+      <c r="H704" s="188"/>
+      <c r="I704" s="188"/>
+      <c r="J704" s="188"/>
+      <c r="K704" s="188"/>
+      <c r="L704" s="188"/>
+      <c r="M704" s="188"/>
+      <c r="N704" s="188"/>
+      <c r="O704" s="188"/>
+      <c r="P704" s="189"/>
     </row>
     <row r="705" spans="2:16" ht="17" thickBot="1">
       <c r="B705" s="49" t="s">
@@ -21403,23 +21406,23 @@
       <c r="P720" s="45"/>
     </row>
     <row r="721" spans="2:16" ht="17" thickBot="1">
-      <c r="B721" s="181" t="s">
+      <c r="B721" s="187" t="s">
         <v>412</v>
       </c>
-      <c r="C721" s="182"/>
-      <c r="D721" s="182"/>
-      <c r="E721" s="182"/>
-      <c r="F721" s="182"/>
-      <c r="G721" s="182"/>
-      <c r="H721" s="182"/>
-      <c r="I721" s="182"/>
-      <c r="J721" s="182"/>
-      <c r="K721" s="182"/>
-      <c r="L721" s="182"/>
-      <c r="M721" s="182"/>
-      <c r="N721" s="182"/>
-      <c r="O721" s="182"/>
-      <c r="P721" s="183"/>
+      <c r="C721" s="188"/>
+      <c r="D721" s="188"/>
+      <c r="E721" s="188"/>
+      <c r="F721" s="188"/>
+      <c r="G721" s="188"/>
+      <c r="H721" s="188"/>
+      <c r="I721" s="188"/>
+      <c r="J721" s="188"/>
+      <c r="K721" s="188"/>
+      <c r="L721" s="188"/>
+      <c r="M721" s="188"/>
+      <c r="N721" s="188"/>
+      <c r="O721" s="188"/>
+      <c r="P721" s="189"/>
     </row>
     <row r="722" spans="2:16" ht="17" thickBot="1">
       <c r="B722" s="49" t="s">
@@ -21795,23 +21798,23 @@
       <c r="P740" s="45"/>
     </row>
     <row r="741" spans="2:16" ht="17" thickBot="1">
-      <c r="B741" s="181" t="s">
+      <c r="B741" s="187" t="s">
         <v>416</v>
       </c>
-      <c r="C741" s="182"/>
-      <c r="D741" s="182"/>
-      <c r="E741" s="182"/>
-      <c r="F741" s="182"/>
-      <c r="G741" s="182"/>
-      <c r="H741" s="182"/>
-      <c r="I741" s="182"/>
-      <c r="J741" s="182"/>
-      <c r="K741" s="182"/>
-      <c r="L741" s="182"/>
-      <c r="M741" s="182"/>
-      <c r="N741" s="182"/>
-      <c r="O741" s="182"/>
-      <c r="P741" s="183"/>
+      <c r="C741" s="188"/>
+      <c r="D741" s="188"/>
+      <c r="E741" s="188"/>
+      <c r="F741" s="188"/>
+      <c r="G741" s="188"/>
+      <c r="H741" s="188"/>
+      <c r="I741" s="188"/>
+      <c r="J741" s="188"/>
+      <c r="K741" s="188"/>
+      <c r="L741" s="188"/>
+      <c r="M741" s="188"/>
+      <c r="N741" s="188"/>
+      <c r="O741" s="188"/>
+      <c r="P741" s="189"/>
     </row>
     <row r="742" spans="2:16" ht="17" thickBot="1">
       <c r="B742" s="49" t="s">
@@ -22638,23 +22641,23 @@
       <c r="P781" s="45"/>
     </row>
     <row r="782" spans="2:16" ht="17" thickBot="1">
-      <c r="B782" s="181" t="s">
+      <c r="B782" s="187" t="s">
         <v>564</v>
       </c>
-      <c r="C782" s="182"/>
-      <c r="D782" s="182"/>
-      <c r="E782" s="182"/>
-      <c r="F782" s="182"/>
-      <c r="G782" s="182"/>
-      <c r="H782" s="182"/>
-      <c r="I782" s="182"/>
-      <c r="J782" s="182"/>
-      <c r="K782" s="182"/>
-      <c r="L782" s="182"/>
-      <c r="M782" s="182"/>
-      <c r="N782" s="182"/>
-      <c r="O782" s="182"/>
-      <c r="P782" s="183"/>
+      <c r="C782" s="188"/>
+      <c r="D782" s="188"/>
+      <c r="E782" s="188"/>
+      <c r="F782" s="188"/>
+      <c r="G782" s="188"/>
+      <c r="H782" s="188"/>
+      <c r="I782" s="188"/>
+      <c r="J782" s="188"/>
+      <c r="K782" s="188"/>
+      <c r="L782" s="188"/>
+      <c r="M782" s="188"/>
+      <c r="N782" s="188"/>
+      <c r="O782" s="188"/>
+      <c r="P782" s="189"/>
     </row>
     <row r="783" spans="2:16" ht="17" thickBot="1">
       <c r="B783" s="49" t="s">
@@ -22870,12 +22873,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B649:P649"/>
-    <mergeCell ref="B506:P506"/>
-    <mergeCell ref="B539:P539"/>
-    <mergeCell ref="B577:P577"/>
-    <mergeCell ref="B600:P600"/>
-    <mergeCell ref="B637:P637"/>
     <mergeCell ref="B782:P782"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T2:U2"/>
@@ -22892,6 +22889,12 @@
     <mergeCell ref="B704:P704"/>
     <mergeCell ref="B721:P721"/>
     <mergeCell ref="B741:P741"/>
+    <mergeCell ref="B649:P649"/>
+    <mergeCell ref="B506:P506"/>
+    <mergeCell ref="B539:P539"/>
+    <mergeCell ref="B577:P577"/>
+    <mergeCell ref="B600:P600"/>
+    <mergeCell ref="B637:P637"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" display="https://leetcode.com/problems/remove-element/" xr:uid="{0C08439D-F97A-154E-B763-1F7C1F321813}"/>
@@ -27267,15 +27270,15 @@
       <c r="X87" s="98"/>
       <c r="Y87" s="98"/>
       <c r="Z87" s="98"/>
-      <c r="AA87" s="188"/>
-      <c r="AB87" s="188"/>
-      <c r="AC87" s="188"/>
-      <c r="AD87" s="188"/>
-      <c r="AE87" s="188"/>
-      <c r="AF87" s="188"/>
-      <c r="AG87" s="188"/>
-      <c r="AH87" s="188"/>
-      <c r="AI87" s="188"/>
+      <c r="AA87" s="191"/>
+      <c r="AB87" s="191"/>
+      <c r="AC87" s="191"/>
+      <c r="AD87" s="191"/>
+      <c r="AE87" s="191"/>
+      <c r="AF87" s="191"/>
+      <c r="AG87" s="191"/>
+      <c r="AH87" s="191"/>
+      <c r="AI87" s="191"/>
       <c r="AJ87" s="105"/>
     </row>
     <row r="88" spans="2:36" ht="17" thickBot="1">
@@ -30343,8 +30346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C48959B-82B5-DA45-8B96-25DF2B5B4CD9}">
   <dimension ref="C9:N110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30428,7 +30431,9 @@
       <c r="I12" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J12" s="137"/>
+      <c r="J12" s="137" t="s">
+        <v>787</v>
+      </c>
       <c r="K12" s="137"/>
       <c r="L12" s="137"/>
       <c r="M12" s="137"/>
@@ -30550,7 +30555,9 @@
       <c r="I18" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J18" s="137"/>
+      <c r="J18" s="137" t="s">
+        <v>787</v>
+      </c>
       <c r="K18" s="137"/>
       <c r="L18" s="137"/>
       <c r="M18" s="137"/>
@@ -30668,7 +30675,7 @@
       <c r="G25" s="137"/>
       <c r="H25" s="137"/>
       <c r="I25" s="137"/>
-      <c r="J25" s="189"/>
+      <c r="J25" s="181"/>
       <c r="K25" s="139"/>
       <c r="L25" s="139"/>
       <c r="M25" s="139"/>
@@ -30740,7 +30747,9 @@
       <c r="I29" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="J29" s="141"/>
+      <c r="J29" s="141" t="s">
+        <v>787</v>
+      </c>
       <c r="K29" s="141"/>
       <c r="L29" s="141"/>
       <c r="M29" s="141"/>
@@ -30836,7 +30845,9 @@
       <c r="I34" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="J34" s="141"/>
+      <c r="J34" s="141" t="s">
+        <v>787</v>
+      </c>
       <c r="K34" s="141"/>
       <c r="L34" s="141"/>
       <c r="M34" s="141"/>
@@ -30858,7 +30869,9 @@
       <c r="I35" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="J35" s="141"/>
+      <c r="J35" s="141" t="s">
+        <v>787</v>
+      </c>
       <c r="K35" s="141"/>
       <c r="L35" s="141"/>
       <c r="M35" s="141"/>
@@ -31022,7 +31035,7 @@
       <c r="G44" s="141"/>
       <c r="H44" s="141"/>
       <c r="I44" s="141"/>
-      <c r="J44" s="190"/>
+      <c r="J44" s="182"/>
       <c r="K44" s="143"/>
       <c r="L44" s="143"/>
       <c r="M44" s="143"/>
@@ -31094,7 +31107,9 @@
       <c r="I48" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="J48" s="145"/>
+      <c r="J48" s="145" t="s">
+        <v>787</v>
+      </c>
       <c r="K48" s="145"/>
       <c r="L48" s="145"/>
       <c r="M48" s="145"/>
@@ -31216,7 +31231,9 @@
       <c r="I54" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="J54" s="145"/>
+      <c r="J54" s="145" t="s">
+        <v>787</v>
+      </c>
       <c r="K54" s="145"/>
       <c r="L54" s="145"/>
       <c r="M54" s="145"/>
@@ -31326,7 +31343,7 @@
       <c r="G61" s="145"/>
       <c r="H61" s="145"/>
       <c r="I61" s="145"/>
-      <c r="J61" s="191"/>
+      <c r="J61" s="183"/>
       <c r="K61" s="147"/>
       <c r="L61" s="147"/>
       <c r="M61" s="147"/>
@@ -31567,12 +31584,16 @@
       <c r="F77" s="153" t="s">
         <v>787</v>
       </c>
-      <c r="G77" s="153"/>
+      <c r="G77" s="153" t="s">
+        <v>844</v>
+      </c>
       <c r="H77" s="153"/>
       <c r="I77" s="153" t="s">
         <v>787</v>
       </c>
-      <c r="J77" s="153"/>
+      <c r="J77" s="153" t="s">
+        <v>787</v>
+      </c>
       <c r="K77" s="153"/>
       <c r="L77" s="153"/>
       <c r="M77" s="153"/>
@@ -31616,7 +31637,9 @@
       <c r="I79" s="153" t="s">
         <v>787</v>
       </c>
-      <c r="J79" s="153"/>
+      <c r="J79" s="153" t="s">
+        <v>787</v>
+      </c>
       <c r="K79" s="153"/>
       <c r="L79" s="153"/>
       <c r="M79" s="153"/>

</xml_diff>

<commit_message>
Update Collection framework methods summary form
</commit_message>
<xml_diff>
--- a/Leetcode-tag record.xlsx
+++ b/Leetcode-tag record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiahsing/git-repositories/workspace-algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDBCC0E-58D5-AC40-A3AA-AB4DD87C9A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02841379-6322-2C4B-9EE5-6025832E59CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26320" yWindow="960" windowWidth="29000" windowHeight="26640" activeTab="2" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
+    <workbookView xWindow="31480" yWindow="500" windowWidth="35040" windowHeight="26640" activeTab="2" xr2:uid="{073527F3-3865-0D40-BFED-DB63B5BC01C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="868">
   <si>
     <t>Array</t>
   </si>
@@ -3336,6 +3336,576 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>Implementation of Data Structures</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Deque</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>LinkedHashSet</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>LinkedHashMap</t>
+  </si>
+  <si>
+    <t>entrySet()</t>
+  </si>
+  <si>
+    <t>keySet()</t>
+  </si>
+  <si>
+    <r>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>getOrDefault</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> defaultValue)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>put</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> value)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>putAll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Map</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;? extends </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>,? extends </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt; m)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>putIfAbsent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> value)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t> key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t> value)</t>
+    </r>
+  </si>
+  <si>
+    <t>values()</t>
+  </si>
+  <si>
+    <r>
+      <t>replace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> value)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>replace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t> key, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t> oldValue, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="DejaVu Sans Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t> newValue)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>containsKey</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> key)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>containsValue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t> value)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3488,7 +4058,7 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="50">
+  <fills count="51">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3783,8 +4353,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -4297,12 +4873,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4609,9 +5264,7 @@
     <xf numFmtId="0" fontId="8" fillId="41" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="43" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="43" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="44" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -4629,7 +5282,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4647,9 +5299,6 @@
     <xf numFmtId="0" fontId="1" fillId="43" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="44" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4657,18 +5306,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4760,15 +5397,6 @@
     <xf numFmtId="0" fontId="11" fillId="49" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="43" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="44" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4793,6 +5421,81 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4803,6 +5506,7 @@
   <colors>
     <mruColors>
       <color rgb="FFDCC0FF"/>
+      <color rgb="FFA3EBCC"/>
       <color rgb="FF73FEFF"/>
       <color rgb="FFFF85E8"/>
       <color rgb="FFF4BAFF"/>
@@ -4811,7 +5515,6 @@
       <color rgb="FFFFADA7"/>
       <color rgb="FFFF7E79"/>
       <color rgb="FFFFDBF7"/>
-      <color rgb="FFFFA7A1"/>
     </mruColors>
   </colors>
   <extLst>
@@ -5143,27 +5846,27 @@
   <sheetData>
     <row r="1" spans="2:21" ht="17" thickBot="1"/>
     <row r="2" spans="2:21" ht="17" thickBot="1">
-      <c r="B2" s="184" t="s">
+      <c r="B2" s="173" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
-      <c r="G2" s="185"/>
-      <c r="H2" s="185"/>
-      <c r="I2" s="185"/>
-      <c r="J2" s="185"/>
-      <c r="K2" s="185"/>
-      <c r="L2" s="185"/>
-      <c r="M2" s="185"/>
-      <c r="N2" s="185"/>
-      <c r="O2" s="185"/>
-      <c r="P2" s="186"/>
-      <c r="R2" s="190"/>
-      <c r="S2" s="190"/>
-      <c r="T2" s="190"/>
-      <c r="U2" s="190"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
+      <c r="J2" s="174"/>
+      <c r="K2" s="174"/>
+      <c r="L2" s="174"/>
+      <c r="M2" s="174"/>
+      <c r="N2" s="174"/>
+      <c r="O2" s="174"/>
+      <c r="P2" s="175"/>
+      <c r="R2" s="179"/>
+      <c r="S2" s="179"/>
+      <c r="T2" s="179"/>
+      <c r="U2" s="179"/>
     </row>
     <row r="3" spans="2:21" ht="17" thickBot="1">
       <c r="B3" s="25" t="s">
@@ -5535,8 +6238,8 @@
       <c r="N15" s="42"/>
       <c r="O15" s="15"/>
       <c r="P15" s="17"/>
-      <c r="R15" s="190"/>
-      <c r="S15" s="190"/>
+      <c r="R15" s="179"/>
+      <c r="S15" s="179"/>
       <c r="T15" s="102"/>
       <c r="U15" s="102"/>
     </row>
@@ -7514,23 +8217,23 @@
       <c r="P98" s="45"/>
     </row>
     <row r="99" spans="2:16" ht="17" thickBot="1">
-      <c r="B99" s="184" t="s">
+      <c r="B99" s="173" t="s">
         <v>101</v>
       </c>
-      <c r="C99" s="185"/>
-      <c r="D99" s="185"/>
-      <c r="E99" s="185"/>
-      <c r="F99" s="185"/>
-      <c r="G99" s="185"/>
-      <c r="H99" s="185"/>
-      <c r="I99" s="185"/>
-      <c r="J99" s="185"/>
-      <c r="K99" s="185"/>
-      <c r="L99" s="185"/>
-      <c r="M99" s="185"/>
-      <c r="N99" s="185"/>
-      <c r="O99" s="185"/>
-      <c r="P99" s="186"/>
+      <c r="C99" s="174"/>
+      <c r="D99" s="174"/>
+      <c r="E99" s="174"/>
+      <c r="F99" s="174"/>
+      <c r="G99" s="174"/>
+      <c r="H99" s="174"/>
+      <c r="I99" s="174"/>
+      <c r="J99" s="174"/>
+      <c r="K99" s="174"/>
+      <c r="L99" s="174"/>
+      <c r="M99" s="174"/>
+      <c r="N99" s="174"/>
+      <c r="O99" s="174"/>
+      <c r="P99" s="175"/>
     </row>
     <row r="100" spans="2:16" ht="17" thickBot="1">
       <c r="B100" s="25" t="s">
@@ -9944,23 +10647,23 @@
       <c r="P208" s="45"/>
     </row>
     <row r="209" spans="2:16" ht="17" thickBot="1">
-      <c r="B209" s="184" t="s">
+      <c r="B209" s="173" t="s">
         <v>166</v>
       </c>
-      <c r="C209" s="185"/>
-      <c r="D209" s="185"/>
-      <c r="E209" s="185"/>
-      <c r="F209" s="185"/>
-      <c r="G209" s="185"/>
-      <c r="H209" s="185"/>
-      <c r="I209" s="185"/>
-      <c r="J209" s="185"/>
-      <c r="K209" s="185"/>
-      <c r="L209" s="185"/>
-      <c r="M209" s="185"/>
-      <c r="N209" s="185"/>
-      <c r="O209" s="185"/>
-      <c r="P209" s="186"/>
+      <c r="C209" s="174"/>
+      <c r="D209" s="174"/>
+      <c r="E209" s="174"/>
+      <c r="F209" s="174"/>
+      <c r="G209" s="174"/>
+      <c r="H209" s="174"/>
+      <c r="I209" s="174"/>
+      <c r="J209" s="174"/>
+      <c r="K209" s="174"/>
+      <c r="L209" s="174"/>
+      <c r="M209" s="174"/>
+      <c r="N209" s="174"/>
+      <c r="O209" s="174"/>
+      <c r="P209" s="175"/>
     </row>
     <row r="210" spans="2:16" ht="17" thickBot="1">
       <c r="B210" s="25" t="s">
@@ -11441,23 +12144,23 @@
       <c r="P273" s="45"/>
     </row>
     <row r="274" spans="2:16" ht="17" thickBot="1">
-      <c r="B274" s="184" t="s">
+      <c r="B274" s="173" t="s">
         <v>43</v>
       </c>
-      <c r="C274" s="185"/>
-      <c r="D274" s="185"/>
-      <c r="E274" s="185"/>
-      <c r="F274" s="185"/>
-      <c r="G274" s="185"/>
-      <c r="H274" s="185"/>
-      <c r="I274" s="185"/>
-      <c r="J274" s="185"/>
-      <c r="K274" s="185"/>
-      <c r="L274" s="185"/>
-      <c r="M274" s="185"/>
-      <c r="N274" s="185"/>
-      <c r="O274" s="185"/>
-      <c r="P274" s="186"/>
+      <c r="C274" s="174"/>
+      <c r="D274" s="174"/>
+      <c r="E274" s="174"/>
+      <c r="F274" s="174"/>
+      <c r="G274" s="174"/>
+      <c r="H274" s="174"/>
+      <c r="I274" s="174"/>
+      <c r="J274" s="174"/>
+      <c r="K274" s="174"/>
+      <c r="L274" s="174"/>
+      <c r="M274" s="174"/>
+      <c r="N274" s="174"/>
+      <c r="O274" s="174"/>
+      <c r="P274" s="175"/>
     </row>
     <row r="275" spans="2:16" ht="17" thickBot="1">
       <c r="B275" s="25" t="s">
@@ -13485,23 +14188,23 @@
       <c r="P363" s="45"/>
     </row>
     <row r="364" spans="2:16" ht="17" thickBot="1">
-      <c r="B364" s="184" t="s">
+      <c r="B364" s="173" t="s">
         <v>255</v>
       </c>
-      <c r="C364" s="185"/>
-      <c r="D364" s="185"/>
-      <c r="E364" s="185"/>
-      <c r="F364" s="185"/>
-      <c r="G364" s="185"/>
-      <c r="H364" s="185"/>
-      <c r="I364" s="185"/>
-      <c r="J364" s="185"/>
-      <c r="K364" s="185"/>
-      <c r="L364" s="185"/>
-      <c r="M364" s="185"/>
-      <c r="N364" s="185"/>
-      <c r="O364" s="185"/>
-      <c r="P364" s="186"/>
+      <c r="C364" s="174"/>
+      <c r="D364" s="174"/>
+      <c r="E364" s="174"/>
+      <c r="F364" s="174"/>
+      <c r="G364" s="174"/>
+      <c r="H364" s="174"/>
+      <c r="I364" s="174"/>
+      <c r="J364" s="174"/>
+      <c r="K364" s="174"/>
+      <c r="L364" s="174"/>
+      <c r="M364" s="174"/>
+      <c r="N364" s="174"/>
+      <c r="O364" s="174"/>
+      <c r="P364" s="175"/>
     </row>
     <row r="365" spans="2:16" ht="17" thickBot="1">
       <c r="B365" s="25" t="s">
@@ -14379,23 +15082,23 @@
       <c r="P401" s="45"/>
     </row>
     <row r="402" spans="2:16" ht="17" thickBot="1">
-      <c r="B402" s="184" t="s">
+      <c r="B402" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="C402" s="185"/>
-      <c r="D402" s="185"/>
-      <c r="E402" s="185"/>
-      <c r="F402" s="185"/>
-      <c r="G402" s="185"/>
-      <c r="H402" s="185"/>
-      <c r="I402" s="185"/>
-      <c r="J402" s="185"/>
-      <c r="K402" s="185"/>
-      <c r="L402" s="185"/>
-      <c r="M402" s="185"/>
-      <c r="N402" s="185"/>
-      <c r="O402" s="185"/>
-      <c r="P402" s="186"/>
+      <c r="C402" s="174"/>
+      <c r="D402" s="174"/>
+      <c r="E402" s="174"/>
+      <c r="F402" s="174"/>
+      <c r="G402" s="174"/>
+      <c r="H402" s="174"/>
+      <c r="I402" s="174"/>
+      <c r="J402" s="174"/>
+      <c r="K402" s="174"/>
+      <c r="L402" s="174"/>
+      <c r="M402" s="174"/>
+      <c r="N402" s="174"/>
+      <c r="O402" s="174"/>
+      <c r="P402" s="175"/>
     </row>
     <row r="403" spans="2:16" ht="17" thickBot="1">
       <c r="B403" s="25" t="s">
@@ -15251,23 +15954,23 @@
       <c r="P439" s="45"/>
     </row>
     <row r="440" spans="2:16" ht="17" thickBot="1">
-      <c r="B440" s="184" t="s">
+      <c r="B440" s="173" t="s">
         <v>300</v>
       </c>
-      <c r="C440" s="185"/>
-      <c r="D440" s="185"/>
-      <c r="E440" s="185"/>
-      <c r="F440" s="185"/>
-      <c r="G440" s="185"/>
-      <c r="H440" s="185"/>
-      <c r="I440" s="185"/>
-      <c r="J440" s="185"/>
-      <c r="K440" s="185"/>
-      <c r="L440" s="185"/>
-      <c r="M440" s="185"/>
-      <c r="N440" s="185"/>
-      <c r="O440" s="185"/>
-      <c r="P440" s="186"/>
+      <c r="C440" s="174"/>
+      <c r="D440" s="174"/>
+      <c r="E440" s="174"/>
+      <c r="F440" s="174"/>
+      <c r="G440" s="174"/>
+      <c r="H440" s="174"/>
+      <c r="I440" s="174"/>
+      <c r="J440" s="174"/>
+      <c r="K440" s="174"/>
+      <c r="L440" s="174"/>
+      <c r="M440" s="174"/>
+      <c r="N440" s="174"/>
+      <c r="O440" s="174"/>
+      <c r="P440" s="175"/>
     </row>
     <row r="441" spans="2:16" ht="17" thickBot="1">
       <c r="B441" s="25" t="s">
@@ -16160,23 +16863,23 @@
       <c r="P478" s="45"/>
     </row>
     <row r="479" spans="2:16" ht="17" thickBot="1">
-      <c r="B479" s="184" t="s">
+      <c r="B479" s="173" t="s">
         <v>59</v>
       </c>
-      <c r="C479" s="185"/>
-      <c r="D479" s="185"/>
-      <c r="E479" s="185"/>
-      <c r="F479" s="185"/>
-      <c r="G479" s="185"/>
-      <c r="H479" s="185"/>
-      <c r="I479" s="185"/>
-      <c r="J479" s="185"/>
-      <c r="K479" s="185"/>
-      <c r="L479" s="185"/>
-      <c r="M479" s="185"/>
-      <c r="N479" s="185"/>
-      <c r="O479" s="185"/>
-      <c r="P479" s="186"/>
+      <c r="C479" s="174"/>
+      <c r="D479" s="174"/>
+      <c r="E479" s="174"/>
+      <c r="F479" s="174"/>
+      <c r="G479" s="174"/>
+      <c r="H479" s="174"/>
+      <c r="I479" s="174"/>
+      <c r="J479" s="174"/>
+      <c r="K479" s="174"/>
+      <c r="L479" s="174"/>
+      <c r="M479" s="174"/>
+      <c r="N479" s="174"/>
+      <c r="O479" s="174"/>
+      <c r="P479" s="175"/>
     </row>
     <row r="480" spans="2:16" ht="17" thickBot="1">
       <c r="B480" s="25" t="s">
@@ -16871,23 +17574,23 @@
       <c r="P505" s="45"/>
     </row>
     <row r="506" spans="2:16" ht="17" thickBot="1">
-      <c r="B506" s="184" t="s">
+      <c r="B506" s="173" t="s">
         <v>324</v>
       </c>
-      <c r="C506" s="185"/>
-      <c r="D506" s="185"/>
-      <c r="E506" s="185"/>
-      <c r="F506" s="185"/>
-      <c r="G506" s="185"/>
-      <c r="H506" s="185"/>
-      <c r="I506" s="185"/>
-      <c r="J506" s="185"/>
-      <c r="K506" s="185"/>
-      <c r="L506" s="185"/>
-      <c r="M506" s="185"/>
-      <c r="N506" s="185"/>
-      <c r="O506" s="185"/>
-      <c r="P506" s="186"/>
+      <c r="C506" s="174"/>
+      <c r="D506" s="174"/>
+      <c r="E506" s="174"/>
+      <c r="F506" s="174"/>
+      <c r="G506" s="174"/>
+      <c r="H506" s="174"/>
+      <c r="I506" s="174"/>
+      <c r="J506" s="174"/>
+      <c r="K506" s="174"/>
+      <c r="L506" s="174"/>
+      <c r="M506" s="174"/>
+      <c r="N506" s="174"/>
+      <c r="O506" s="174"/>
+      <c r="P506" s="175"/>
     </row>
     <row r="507" spans="2:16" ht="17" thickBot="1">
       <c r="B507" s="25" t="s">
@@ -17590,23 +18293,23 @@
       <c r="P538" s="45"/>
     </row>
     <row r="539" spans="2:16" ht="17" thickBot="1">
-      <c r="B539" s="184" t="s">
+      <c r="B539" s="173" t="s">
         <v>352</v>
       </c>
-      <c r="C539" s="185"/>
-      <c r="D539" s="185"/>
-      <c r="E539" s="185"/>
-      <c r="F539" s="185"/>
-      <c r="G539" s="185"/>
-      <c r="H539" s="185"/>
-      <c r="I539" s="185"/>
-      <c r="J539" s="185"/>
-      <c r="K539" s="185"/>
-      <c r="L539" s="185"/>
-      <c r="M539" s="185"/>
-      <c r="N539" s="185"/>
-      <c r="O539" s="185"/>
-      <c r="P539" s="186"/>
+      <c r="C539" s="174"/>
+      <c r="D539" s="174"/>
+      <c r="E539" s="174"/>
+      <c r="F539" s="174"/>
+      <c r="G539" s="174"/>
+      <c r="H539" s="174"/>
+      <c r="I539" s="174"/>
+      <c r="J539" s="174"/>
+      <c r="K539" s="174"/>
+      <c r="L539" s="174"/>
+      <c r="M539" s="174"/>
+      <c r="N539" s="174"/>
+      <c r="O539" s="174"/>
+      <c r="P539" s="175"/>
     </row>
     <row r="540" spans="2:16" ht="17" thickBot="1">
       <c r="B540" s="25" t="s">
@@ -18414,23 +19117,23 @@
       <c r="P576" s="45"/>
     </row>
     <row r="577" spans="2:16" ht="17" thickBot="1">
-      <c r="B577" s="184" t="s">
+      <c r="B577" s="173" t="s">
         <v>342</v>
       </c>
-      <c r="C577" s="185"/>
-      <c r="D577" s="185"/>
-      <c r="E577" s="185"/>
-      <c r="F577" s="185"/>
-      <c r="G577" s="185"/>
-      <c r="H577" s="185"/>
-      <c r="I577" s="185"/>
-      <c r="J577" s="185"/>
-      <c r="K577" s="185"/>
-      <c r="L577" s="185"/>
-      <c r="M577" s="185"/>
-      <c r="N577" s="185"/>
-      <c r="O577" s="185"/>
-      <c r="P577" s="186"/>
+      <c r="C577" s="174"/>
+      <c r="D577" s="174"/>
+      <c r="E577" s="174"/>
+      <c r="F577" s="174"/>
+      <c r="G577" s="174"/>
+      <c r="H577" s="174"/>
+      <c r="I577" s="174"/>
+      <c r="J577" s="174"/>
+      <c r="K577" s="174"/>
+      <c r="L577" s="174"/>
+      <c r="M577" s="174"/>
+      <c r="N577" s="174"/>
+      <c r="O577" s="174"/>
+      <c r="P577" s="175"/>
     </row>
     <row r="578" spans="2:16" ht="17" thickBot="1">
       <c r="B578" s="25" t="s">
@@ -18931,23 +19634,23 @@
       <c r="P599" s="45"/>
     </row>
     <row r="600" spans="2:16" ht="17" thickBot="1">
-      <c r="B600" s="184" t="s">
+      <c r="B600" s="173" t="s">
         <v>373</v>
       </c>
-      <c r="C600" s="185"/>
-      <c r="D600" s="185"/>
-      <c r="E600" s="185"/>
-      <c r="F600" s="185"/>
-      <c r="G600" s="185"/>
-      <c r="H600" s="185"/>
-      <c r="I600" s="185"/>
-      <c r="J600" s="185"/>
-      <c r="K600" s="185"/>
-      <c r="L600" s="185"/>
-      <c r="M600" s="185"/>
-      <c r="N600" s="185"/>
-      <c r="O600" s="185"/>
-      <c r="P600" s="186"/>
+      <c r="C600" s="174"/>
+      <c r="D600" s="174"/>
+      <c r="E600" s="174"/>
+      <c r="F600" s="174"/>
+      <c r="G600" s="174"/>
+      <c r="H600" s="174"/>
+      <c r="I600" s="174"/>
+      <c r="J600" s="174"/>
+      <c r="K600" s="174"/>
+      <c r="L600" s="174"/>
+      <c r="M600" s="174"/>
+      <c r="N600" s="174"/>
+      <c r="O600" s="174"/>
+      <c r="P600" s="175"/>
     </row>
     <row r="601" spans="2:16" ht="17" thickBot="1">
       <c r="B601" s="25" t="s">
@@ -19684,23 +20387,23 @@
       <c r="P636" s="45"/>
     </row>
     <row r="637" spans="2:16" ht="17" thickBot="1">
-      <c r="B637" s="184" t="s">
+      <c r="B637" s="173" t="s">
         <v>387</v>
       </c>
-      <c r="C637" s="185"/>
-      <c r="D637" s="185"/>
-      <c r="E637" s="185"/>
-      <c r="F637" s="185"/>
-      <c r="G637" s="185"/>
-      <c r="H637" s="185"/>
-      <c r="I637" s="185"/>
-      <c r="J637" s="185"/>
-      <c r="K637" s="185"/>
-      <c r="L637" s="185"/>
-      <c r="M637" s="185"/>
-      <c r="N637" s="185"/>
-      <c r="O637" s="185"/>
-      <c r="P637" s="186"/>
+      <c r="C637" s="174"/>
+      <c r="D637" s="174"/>
+      <c r="E637" s="174"/>
+      <c r="F637" s="174"/>
+      <c r="G637" s="174"/>
+      <c r="H637" s="174"/>
+      <c r="I637" s="174"/>
+      <c r="J637" s="174"/>
+      <c r="K637" s="174"/>
+      <c r="L637" s="174"/>
+      <c r="M637" s="174"/>
+      <c r="N637" s="174"/>
+      <c r="O637" s="174"/>
+      <c r="P637" s="175"/>
     </row>
     <row r="638" spans="2:16" ht="17" thickBot="1">
       <c r="B638" s="25" t="s">
@@ -19954,23 +20657,23 @@
       <c r="P648" s="45"/>
     </row>
     <row r="649" spans="2:16" ht="17" thickBot="1">
-      <c r="B649" s="184" t="s">
+      <c r="B649" s="173" t="s">
         <v>391</v>
       </c>
-      <c r="C649" s="185"/>
-      <c r="D649" s="185"/>
-      <c r="E649" s="185"/>
-      <c r="F649" s="185"/>
-      <c r="G649" s="185"/>
-      <c r="H649" s="185"/>
-      <c r="I649" s="185"/>
-      <c r="J649" s="185"/>
-      <c r="K649" s="185"/>
-      <c r="L649" s="185"/>
-      <c r="M649" s="185"/>
-      <c r="N649" s="185"/>
-      <c r="O649" s="185"/>
-      <c r="P649" s="186"/>
+      <c r="C649" s="174"/>
+      <c r="D649" s="174"/>
+      <c r="E649" s="174"/>
+      <c r="F649" s="174"/>
+      <c r="G649" s="174"/>
+      <c r="H649" s="174"/>
+      <c r="I649" s="174"/>
+      <c r="J649" s="174"/>
+      <c r="K649" s="174"/>
+      <c r="L649" s="174"/>
+      <c r="M649" s="174"/>
+      <c r="N649" s="174"/>
+      <c r="O649" s="174"/>
+      <c r="P649" s="175"/>
     </row>
     <row r="650" spans="2:16" ht="17" thickBot="1">
       <c r="B650" s="25" t="s">
@@ -20472,23 +21175,23 @@
       <c r="P674" s="45"/>
     </row>
     <row r="675" spans="2:16" ht="17" thickBot="1">
-      <c r="B675" s="187" t="s">
+      <c r="B675" s="176" t="s">
         <v>398</v>
       </c>
-      <c r="C675" s="188"/>
-      <c r="D675" s="188"/>
-      <c r="E675" s="188"/>
-      <c r="F675" s="188"/>
-      <c r="G675" s="188"/>
-      <c r="H675" s="188"/>
-      <c r="I675" s="188"/>
-      <c r="J675" s="188"/>
-      <c r="K675" s="188"/>
-      <c r="L675" s="188"/>
-      <c r="M675" s="188"/>
-      <c r="N675" s="188"/>
-      <c r="O675" s="188"/>
-      <c r="P675" s="189"/>
+      <c r="C675" s="177"/>
+      <c r="D675" s="177"/>
+      <c r="E675" s="177"/>
+      <c r="F675" s="177"/>
+      <c r="G675" s="177"/>
+      <c r="H675" s="177"/>
+      <c r="I675" s="177"/>
+      <c r="J675" s="177"/>
+      <c r="K675" s="177"/>
+      <c r="L675" s="177"/>
+      <c r="M675" s="177"/>
+      <c r="N675" s="177"/>
+      <c r="O675" s="177"/>
+      <c r="P675" s="178"/>
     </row>
     <row r="676" spans="2:16" ht="17" thickBot="1">
       <c r="B676" s="49" t="s">
@@ -21057,23 +21760,23 @@
       <c r="P703" s="45"/>
     </row>
     <row r="704" spans="2:16" ht="17" thickBot="1">
-      <c r="B704" s="187" t="s">
+      <c r="B704" s="176" t="s">
         <v>408</v>
       </c>
-      <c r="C704" s="188"/>
-      <c r="D704" s="188"/>
-      <c r="E704" s="188"/>
-      <c r="F704" s="188"/>
-      <c r="G704" s="188"/>
-      <c r="H704" s="188"/>
-      <c r="I704" s="188"/>
-      <c r="J704" s="188"/>
-      <c r="K704" s="188"/>
-      <c r="L704" s="188"/>
-      <c r="M704" s="188"/>
-      <c r="N704" s="188"/>
-      <c r="O704" s="188"/>
-      <c r="P704" s="189"/>
+      <c r="C704" s="177"/>
+      <c r="D704" s="177"/>
+      <c r="E704" s="177"/>
+      <c r="F704" s="177"/>
+      <c r="G704" s="177"/>
+      <c r="H704" s="177"/>
+      <c r="I704" s="177"/>
+      <c r="J704" s="177"/>
+      <c r="K704" s="177"/>
+      <c r="L704" s="177"/>
+      <c r="M704" s="177"/>
+      <c r="N704" s="177"/>
+      <c r="O704" s="177"/>
+      <c r="P704" s="178"/>
     </row>
     <row r="705" spans="2:16" ht="17" thickBot="1">
       <c r="B705" s="49" t="s">
@@ -21406,23 +22109,23 @@
       <c r="P720" s="45"/>
     </row>
     <row r="721" spans="2:16" ht="17" thickBot="1">
-      <c r="B721" s="187" t="s">
+      <c r="B721" s="176" t="s">
         <v>412</v>
       </c>
-      <c r="C721" s="188"/>
-      <c r="D721" s="188"/>
-      <c r="E721" s="188"/>
-      <c r="F721" s="188"/>
-      <c r="G721" s="188"/>
-      <c r="H721" s="188"/>
-      <c r="I721" s="188"/>
-      <c r="J721" s="188"/>
-      <c r="K721" s="188"/>
-      <c r="L721" s="188"/>
-      <c r="M721" s="188"/>
-      <c r="N721" s="188"/>
-      <c r="O721" s="188"/>
-      <c r="P721" s="189"/>
+      <c r="C721" s="177"/>
+      <c r="D721" s="177"/>
+      <c r="E721" s="177"/>
+      <c r="F721" s="177"/>
+      <c r="G721" s="177"/>
+      <c r="H721" s="177"/>
+      <c r="I721" s="177"/>
+      <c r="J721" s="177"/>
+      <c r="K721" s="177"/>
+      <c r="L721" s="177"/>
+      <c r="M721" s="177"/>
+      <c r="N721" s="177"/>
+      <c r="O721" s="177"/>
+      <c r="P721" s="178"/>
     </row>
     <row r="722" spans="2:16" ht="17" thickBot="1">
       <c r="B722" s="49" t="s">
@@ -21798,23 +22501,23 @@
       <c r="P740" s="45"/>
     </row>
     <row r="741" spans="2:16" ht="17" thickBot="1">
-      <c r="B741" s="187" t="s">
+      <c r="B741" s="176" t="s">
         <v>416</v>
       </c>
-      <c r="C741" s="188"/>
-      <c r="D741" s="188"/>
-      <c r="E741" s="188"/>
-      <c r="F741" s="188"/>
-      <c r="G741" s="188"/>
-      <c r="H741" s="188"/>
-      <c r="I741" s="188"/>
-      <c r="J741" s="188"/>
-      <c r="K741" s="188"/>
-      <c r="L741" s="188"/>
-      <c r="M741" s="188"/>
-      <c r="N741" s="188"/>
-      <c r="O741" s="188"/>
-      <c r="P741" s="189"/>
+      <c r="C741" s="177"/>
+      <c r="D741" s="177"/>
+      <c r="E741" s="177"/>
+      <c r="F741" s="177"/>
+      <c r="G741" s="177"/>
+      <c r="H741" s="177"/>
+      <c r="I741" s="177"/>
+      <c r="J741" s="177"/>
+      <c r="K741" s="177"/>
+      <c r="L741" s="177"/>
+      <c r="M741" s="177"/>
+      <c r="N741" s="177"/>
+      <c r="O741" s="177"/>
+      <c r="P741" s="178"/>
     </row>
     <row r="742" spans="2:16" ht="17" thickBot="1">
       <c r="B742" s="49" t="s">
@@ -22641,23 +23344,23 @@
       <c r="P781" s="45"/>
     </row>
     <row r="782" spans="2:16" ht="17" thickBot="1">
-      <c r="B782" s="187" t="s">
+      <c r="B782" s="176" t="s">
         <v>564</v>
       </c>
-      <c r="C782" s="188"/>
-      <c r="D782" s="188"/>
-      <c r="E782" s="188"/>
-      <c r="F782" s="188"/>
-      <c r="G782" s="188"/>
-      <c r="H782" s="188"/>
-      <c r="I782" s="188"/>
-      <c r="J782" s="188"/>
-      <c r="K782" s="188"/>
-      <c r="L782" s="188"/>
-      <c r="M782" s="188"/>
-      <c r="N782" s="188"/>
-      <c r="O782" s="188"/>
-      <c r="P782" s="189"/>
+      <c r="C782" s="177"/>
+      <c r="D782" s="177"/>
+      <c r="E782" s="177"/>
+      <c r="F782" s="177"/>
+      <c r="G782" s="177"/>
+      <c r="H782" s="177"/>
+      <c r="I782" s="177"/>
+      <c r="J782" s="177"/>
+      <c r="K782" s="177"/>
+      <c r="L782" s="177"/>
+      <c r="M782" s="177"/>
+      <c r="N782" s="177"/>
+      <c r="O782" s="177"/>
+      <c r="P782" s="178"/>
     </row>
     <row r="783" spans="2:16" ht="17" thickBot="1">
       <c r="B783" s="49" t="s">
@@ -27270,15 +27973,15 @@
       <c r="X87" s="98"/>
       <c r="Y87" s="98"/>
       <c r="Z87" s="98"/>
-      <c r="AA87" s="191"/>
-      <c r="AB87" s="191"/>
-      <c r="AC87" s="191"/>
-      <c r="AD87" s="191"/>
-      <c r="AE87" s="191"/>
-      <c r="AF87" s="191"/>
-      <c r="AG87" s="191"/>
-      <c r="AH87" s="191"/>
-      <c r="AI87" s="191"/>
+      <c r="AA87" s="180"/>
+      <c r="AB87" s="180"/>
+      <c r="AC87" s="180"/>
+      <c r="AD87" s="180"/>
+      <c r="AE87" s="180"/>
+      <c r="AF87" s="180"/>
+      <c r="AG87" s="180"/>
+      <c r="AH87" s="180"/>
+      <c r="AI87" s="180"/>
       <c r="AJ87" s="105"/>
     </row>
     <row r="88" spans="2:36" ht="17" thickBot="1">
@@ -30344,56 +31047,148 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C48959B-82B5-DA45-8B96-25DF2B5B4CD9}">
-  <dimension ref="C9:N110"/>
+  <dimension ref="C1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="M82" sqref="M82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="84" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="7" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="20.6640625" customWidth="1"/>
     <col min="10" max="10" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="19.5" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="3:14" ht="17" thickBot="1"/>
+    <row r="2" spans="3:14" ht="17" thickBot="1">
+      <c r="C2" s="184" t="s">
+        <v>845</v>
+      </c>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="182"/>
+    </row>
+    <row r="3" spans="3:14" ht="17" thickBot="1">
+      <c r="C3" s="92" t="s">
+        <v>846</v>
+      </c>
+      <c r="D3" s="185" t="s">
+        <v>779</v>
+      </c>
+      <c r="E3" s="184" t="s">
+        <v>780</v>
+      </c>
+      <c r="F3" s="185" t="s">
+        <v>852</v>
+      </c>
+      <c r="G3" s="184" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" ht="17" thickBot="1">
+      <c r="C4" s="186" t="s">
+        <v>847</v>
+      </c>
+      <c r="D4" s="106" t="s">
+        <v>782</v>
+      </c>
+      <c r="E4" s="183" t="s">
+        <v>784</v>
+      </c>
+      <c r="F4" s="106" t="s">
+        <v>851</v>
+      </c>
+      <c r="G4" s="183"/>
+    </row>
+    <row r="5" spans="3:14" ht="17" thickBot="1">
+      <c r="C5" s="187" t="s">
+        <v>848</v>
+      </c>
+      <c r="D5" s="185" t="s">
+        <v>780</v>
+      </c>
+      <c r="E5" s="184" t="s">
+        <v>840</v>
+      </c>
+      <c r="F5" s="185" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" s="184"/>
+    </row>
+    <row r="6" spans="3:14" ht="17" thickBot="1">
+      <c r="C6" s="189" t="s">
+        <v>849</v>
+      </c>
+      <c r="D6" s="185" t="s">
+        <v>780</v>
+      </c>
+      <c r="E6" s="184" t="s">
+        <v>840</v>
+      </c>
+      <c r="F6" s="185"/>
+      <c r="G6" s="184"/>
+    </row>
+    <row r="7" spans="3:14" ht="17" thickBot="1">
+      <c r="C7" s="188" t="s">
+        <v>850</v>
+      </c>
+      <c r="D7" s="185" t="s">
+        <v>781</v>
+      </c>
+      <c r="E7" s="184" t="s">
+        <v>783</v>
+      </c>
+      <c r="F7" s="185" t="s">
+        <v>853</v>
+      </c>
+      <c r="G7" s="184"/>
+    </row>
     <row r="9" spans="3:14" ht="17" thickBot="1"/>
     <row r="10" spans="3:14" ht="20" thickBot="1">
-      <c r="C10" s="129"/>
-      <c r="D10" s="178" t="s">
+      <c r="C10" s="126"/>
+      <c r="D10" s="170" t="s">
         <v>843</v>
       </c>
-      <c r="E10" s="179" t="s">
+      <c r="E10" s="171" t="s">
         <v>779</v>
       </c>
-      <c r="F10" s="178" t="s">
+      <c r="F10" s="170" t="s">
         <v>780</v>
       </c>
-      <c r="G10" s="178" t="s">
+      <c r="G10" s="170" t="s">
         <v>353</v>
       </c>
-      <c r="H10" s="178" t="s">
+      <c r="H10" s="170" t="s">
         <v>841</v>
       </c>
-      <c r="I10" s="178" t="s">
+      <c r="I10" s="170" t="s">
         <v>840</v>
       </c>
-      <c r="J10" s="178" t="s">
+      <c r="J10" s="170" t="s">
         <v>365</v>
       </c>
-      <c r="K10" s="178" t="s">
+      <c r="K10" s="170" t="s">
         <v>781</v>
       </c>
-      <c r="L10" s="178" t="s">
+      <c r="L10" s="170" t="s">
         <v>783</v>
       </c>
-      <c r="M10" s="178" t="s">
+      <c r="M10" s="170" t="s">
         <v>782</v>
       </c>
-      <c r="N10" s="180" t="s">
+      <c r="N10" s="172" t="s">
         <v>784</v>
       </c>
     </row>
@@ -30417,272 +31212,274 @@
       <c r="C12" s="112" t="s">
         <v>789</v>
       </c>
-      <c r="D12" s="137"/>
-      <c r="E12" s="137" t="s">
+      <c r="D12" s="134"/>
+      <c r="E12" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="F12" s="137" t="s">
+      <c r="F12" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G12" s="137"/>
-      <c r="H12" s="137" t="s">
+      <c r="G12" s="134"/>
+      <c r="H12" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="I12" s="137" t="s">
+      <c r="I12" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J12" s="137" t="s">
+      <c r="J12" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="K12" s="137"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="137"/>
-      <c r="N12" s="137"/>
+      <c r="K12" s="134"/>
+      <c r="L12" s="134"/>
+      <c r="M12" s="134" t="s">
+        <v>787</v>
+      </c>
+      <c r="N12" s="134"/>
     </row>
     <row r="13" spans="3:14" ht="18">
       <c r="C13" s="112" t="s">
         <v>790</v>
       </c>
-      <c r="D13" s="137"/>
-      <c r="E13" s="137" t="s">
+      <c r="D13" s="134"/>
+      <c r="E13" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="F13" s="137" t="s">
+      <c r="F13" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G13" s="137"/>
-      <c r="H13" s="137"/>
-      <c r="I13" s="137"/>
-      <c r="J13" s="137"/>
-      <c r="K13" s="137"/>
-      <c r="L13" s="137"/>
-      <c r="M13" s="137"/>
-      <c r="N13" s="137"/>
+      <c r="G13" s="134"/>
+      <c r="H13" s="134"/>
+      <c r="I13" s="134"/>
+      <c r="J13" s="134"/>
+      <c r="K13" s="134"/>
+      <c r="L13" s="134"/>
+      <c r="M13" s="134"/>
+      <c r="N13" s="134"/>
     </row>
     <row r="14" spans="3:14" ht="18">
       <c r="C14" s="112" t="s">
         <v>791</v>
       </c>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137" t="s">
+      <c r="D14" s="134"/>
+      <c r="E14" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="F14" s="137" t="s">
+      <c r="F14" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G14" s="137"/>
-      <c r="H14" s="137"/>
-      <c r="I14" s="137"/>
-      <c r="J14" s="137"/>
-      <c r="K14" s="137"/>
-      <c r="L14" s="137"/>
-      <c r="M14" s="137"/>
-      <c r="N14" s="137"/>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="134"/>
+      <c r="J14" s="134"/>
+      <c r="K14" s="134"/>
+      <c r="L14" s="134"/>
+      <c r="M14" s="134"/>
+      <c r="N14" s="134"/>
     </row>
     <row r="15" spans="3:14" ht="18">
       <c r="C15" s="112" t="s">
         <v>792</v>
       </c>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137" t="s">
+      <c r="D15" s="134"/>
+      <c r="E15" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="F15" s="137" t="s">
+      <c r="F15" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G15" s="137"/>
-      <c r="H15" s="137"/>
-      <c r="I15" s="137"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="137"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="137"/>
-      <c r="N15" s="137"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="134"/>
+      <c r="K15" s="134"/>
+      <c r="L15" s="134"/>
+      <c r="M15" s="134"/>
+      <c r="N15" s="134"/>
     </row>
     <row r="16" spans="3:14" ht="18">
       <c r="C16" s="112" t="s">
         <v>824</v>
       </c>
-      <c r="D16" s="137"/>
-      <c r="E16" s="137"/>
-      <c r="F16" s="137" t="s">
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G16" s="137"/>
-      <c r="H16" s="137"/>
-      <c r="I16" s="137" t="s">
+      <c r="G16" s="134"/>
+      <c r="H16" s="134"/>
+      <c r="I16" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J16" s="137"/>
-      <c r="K16" s="137"/>
-      <c r="L16" s="137"/>
-      <c r="M16" s="137"/>
-      <c r="N16" s="137"/>
+      <c r="J16" s="134"/>
+      <c r="K16" s="134"/>
+      <c r="L16" s="134"/>
+      <c r="M16" s="134"/>
+      <c r="N16" s="134"/>
     </row>
     <row r="17" spans="3:14" ht="18">
       <c r="C17" s="112" t="s">
         <v>823</v>
       </c>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137" t="s">
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
+      <c r="F17" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G17" s="137"/>
-      <c r="H17" s="137"/>
-      <c r="I17" s="137" t="s">
+      <c r="G17" s="134"/>
+      <c r="H17" s="134"/>
+      <c r="I17" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J17" s="137"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="137"/>
-      <c r="M17" s="137"/>
-      <c r="N17" s="137"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="134"/>
+      <c r="L17" s="134"/>
+      <c r="M17" s="134"/>
+      <c r="N17" s="134"/>
     </row>
     <row r="18" spans="3:14" ht="18">
       <c r="C18" s="112" t="s">
         <v>827</v>
       </c>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137" t="s">
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G18" s="137"/>
-      <c r="H18" s="137" t="s">
+      <c r="G18" s="134"/>
+      <c r="H18" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="I18" s="137" t="s">
+      <c r="I18" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J18" s="137" t="s">
+      <c r="J18" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="K18" s="137"/>
-      <c r="L18" s="137"/>
-      <c r="M18" s="137"/>
-      <c r="N18" s="137"/>
+      <c r="K18" s="134"/>
+      <c r="L18" s="134"/>
+      <c r="M18" s="134"/>
+      <c r="N18" s="134"/>
     </row>
     <row r="19" spans="3:14" ht="18">
       <c r="C19" s="112" t="s">
         <v>828</v>
       </c>
-      <c r="D19" s="137"/>
-      <c r="E19" s="137"/>
-      <c r="F19" s="137" t="s">
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G19" s="137"/>
-      <c r="H19" s="137"/>
-      <c r="I19" s="137" t="s">
+      <c r="G19" s="134"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J19" s="137"/>
-      <c r="K19" s="137"/>
-      <c r="L19" s="137"/>
-      <c r="M19" s="137"/>
-      <c r="N19" s="137"/>
+      <c r="J19" s="134"/>
+      <c r="K19" s="134"/>
+      <c r="L19" s="134"/>
+      <c r="M19" s="134"/>
+      <c r="N19" s="134"/>
     </row>
     <row r="20" spans="3:14" ht="18">
       <c r="C20" s="112" t="s">
         <v>829</v>
       </c>
-      <c r="D20" s="137"/>
-      <c r="E20" s="137"/>
-      <c r="F20" s="137" t="s">
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G20" s="137"/>
-      <c r="H20" s="137"/>
-      <c r="I20" s="137" t="s">
+      <c r="G20" s="134"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J20" s="137"/>
-      <c r="K20" s="137"/>
-      <c r="L20" s="137"/>
-      <c r="M20" s="137"/>
-      <c r="N20" s="137"/>
+      <c r="J20" s="134"/>
+      <c r="K20" s="134"/>
+      <c r="L20" s="134"/>
+      <c r="M20" s="134"/>
+      <c r="N20" s="134"/>
     </row>
     <row r="21" spans="3:14" ht="19">
       <c r="C21" s="112" t="s">
         <v>836</v>
       </c>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137" t="s">
+      <c r="D21" s="134"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="G21" s="137" t="s">
+      <c r="G21" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="H21" s="137"/>
-      <c r="I21" s="137" t="s">
+      <c r="H21" s="134"/>
+      <c r="I21" s="134" t="s">
         <v>787</v>
       </c>
-      <c r="J21" s="137"/>
-      <c r="K21" s="137"/>
-      <c r="L21" s="137"/>
-      <c r="M21" s="137"/>
-      <c r="N21" s="137"/>
+      <c r="J21" s="134"/>
+      <c r="K21" s="134"/>
+      <c r="L21" s="134"/>
+      <c r="M21" s="134"/>
+      <c r="N21" s="134"/>
     </row>
     <row r="22" spans="3:14" ht="18">
       <c r="C22" s="112"/>
-      <c r="D22" s="137"/>
-      <c r="E22" s="137"/>
-      <c r="F22" s="137"/>
-      <c r="G22" s="137"/>
-      <c r="H22" s="137"/>
-      <c r="I22" s="137"/>
-      <c r="J22" s="137"/>
-      <c r="K22" s="137"/>
-      <c r="L22" s="137"/>
-      <c r="M22" s="137"/>
-      <c r="N22" s="137"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
+      <c r="G22" s="134"/>
+      <c r="H22" s="134"/>
+      <c r="I22" s="134"/>
+      <c r="J22" s="134"/>
+      <c r="K22" s="134"/>
+      <c r="L22" s="134"/>
+      <c r="M22" s="134"/>
+      <c r="N22" s="134"/>
     </row>
     <row r="23" spans="3:14" ht="18">
       <c r="C23" s="112"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="137"/>
-      <c r="F23" s="137"/>
-      <c r="G23" s="137"/>
-      <c r="H23" s="137"/>
-      <c r="I23" s="137"/>
-      <c r="J23" s="137"/>
-      <c r="K23" s="137"/>
-      <c r="L23" s="137"/>
-      <c r="M23" s="137"/>
-      <c r="N23" s="137"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
+      <c r="G23" s="134"/>
+      <c r="H23" s="134"/>
+      <c r="I23" s="134"/>
+      <c r="J23" s="134"/>
+      <c r="K23" s="134"/>
+      <c r="L23" s="134"/>
+      <c r="M23" s="134"/>
+      <c r="N23" s="134"/>
     </row>
     <row r="24" spans="3:14">
       <c r="C24" s="113"/>
-      <c r="D24" s="138"/>
-      <c r="E24" s="138"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="138"/>
-      <c r="H24" s="138"/>
-      <c r="I24" s="138"/>
-      <c r="J24" s="138"/>
-      <c r="K24" s="138"/>
-      <c r="L24" s="138"/>
-      <c r="M24" s="138"/>
-      <c r="N24" s="138"/>
+      <c r="D24" s="135"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="135"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="135"/>
+      <c r="I24" s="135"/>
+      <c r="J24" s="135"/>
+      <c r="K24" s="135"/>
+      <c r="L24" s="135"/>
+      <c r="M24" s="135"/>
+      <c r="N24" s="135"/>
     </row>
     <row r="25" spans="3:14" ht="19" thickBot="1">
-      <c r="C25" s="112"/>
-      <c r="D25" s="137"/>
-      <c r="E25" s="137"/>
-      <c r="F25" s="137"/>
-      <c r="G25" s="137"/>
-      <c r="H25" s="137"/>
-      <c r="I25" s="137"/>
-      <c r="J25" s="181"/>
-      <c r="K25" s="139"/>
-      <c r="L25" s="139"/>
-      <c r="M25" s="139"/>
-      <c r="N25" s="139"/>
+      <c r="C25" s="203"/>
+      <c r="D25" s="202"/>
+      <c r="E25" s="202"/>
+      <c r="F25" s="202"/>
+      <c r="G25" s="202"/>
+      <c r="H25" s="202"/>
+      <c r="I25" s="202"/>
+      <c r="J25" s="202"/>
+      <c r="K25" s="136"/>
+      <c r="L25" s="136"/>
+      <c r="M25" s="136"/>
+      <c r="N25" s="136"/>
     </row>
     <row r="26" spans="3:14" ht="17" thickBot="1">
-      <c r="C26" s="122"/>
+      <c r="C26" s="120"/>
       <c r="D26" s="110"/>
       <c r="E26" s="110"/>
       <c r="F26" s="110"/>
@@ -30693,1455 +31490,1605 @@
       <c r="K26" s="110"/>
       <c r="L26" s="110"/>
       <c r="M26" s="110"/>
-      <c r="N26" s="125"/>
-    </row>
-    <row r="27" spans="3:14" ht="18">
-      <c r="C27" s="114" t="s">
+      <c r="N26" s="123"/>
+    </row>
+    <row r="27" spans="3:14" ht="19" thickBot="1">
+      <c r="C27" s="207" t="s">
         <v>786</v>
       </c>
-      <c r="D27" s="140"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="140"/>
-      <c r="G27" s="140"/>
-      <c r="H27" s="140"/>
-      <c r="I27" s="140"/>
-      <c r="J27" s="140"/>
-      <c r="K27" s="140"/>
-      <c r="L27" s="140"/>
-      <c r="M27" s="140"/>
-      <c r="N27" s="140"/>
+      <c r="D27" s="208"/>
+      <c r="E27" s="208"/>
+      <c r="F27" s="208"/>
+      <c r="G27" s="208"/>
+      <c r="H27" s="208"/>
+      <c r="I27" s="208"/>
+      <c r="J27" s="208"/>
+      <c r="K27" s="208"/>
+      <c r="L27" s="208"/>
+      <c r="M27" s="208"/>
+      <c r="N27" s="208"/>
     </row>
     <row r="28" spans="3:14" ht="18">
-      <c r="C28" s="115" t="s">
+      <c r="C28" s="209" t="s">
         <v>788</v>
       </c>
-      <c r="D28" s="141"/>
-      <c r="E28" s="141" t="s">
+      <c r="D28" s="210"/>
+      <c r="E28" s="210" t="s">
         <v>787</v>
       </c>
-      <c r="F28" s="141" t="s">
+      <c r="F28" s="210" t="s">
         <v>787</v>
       </c>
-      <c r="G28" s="141"/>
-      <c r="H28" s="141"/>
-      <c r="I28" s="141"/>
-      <c r="J28" s="141"/>
-      <c r="K28" s="141"/>
-      <c r="L28" s="141"/>
-      <c r="M28" s="141"/>
-      <c r="N28" s="141"/>
+      <c r="G28" s="210"/>
+      <c r="H28" s="210"/>
+      <c r="I28" s="210"/>
+      <c r="J28" s="210"/>
+      <c r="K28" s="210"/>
+      <c r="L28" s="210"/>
+      <c r="M28" s="210"/>
+      <c r="N28" s="210"/>
     </row>
     <row r="29" spans="3:14" ht="18">
-      <c r="C29" s="115" t="s">
+      <c r="C29" s="114" t="s">
         <v>793</v>
       </c>
-      <c r="D29" s="141"/>
-      <c r="E29" s="141" t="s">
+      <c r="D29" s="137"/>
+      <c r="E29" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="F29" s="141" t="s">
+      <c r="F29" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G29" s="141"/>
-      <c r="H29" s="141"/>
-      <c r="I29" s="141" t="s">
+      <c r="G29" s="137"/>
+      <c r="H29" s="137"/>
+      <c r="I29" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J29" s="141" t="s">
+      <c r="J29" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="K29" s="141"/>
-      <c r="L29" s="141"/>
-      <c r="M29" s="141"/>
-      <c r="N29" s="141"/>
+      <c r="K29" s="137"/>
+      <c r="L29" s="137"/>
+      <c r="M29" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="N29" s="137"/>
     </row>
     <row r="30" spans="3:14" ht="18">
-      <c r="C30" s="115" t="s">
+      <c r="C30" s="114" t="s">
         <v>794</v>
       </c>
-      <c r="D30" s="141"/>
-      <c r="E30" s="141" t="s">
+      <c r="D30" s="137"/>
+      <c r="E30" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="F30" s="141" t="s">
+      <c r="F30" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G30" s="141"/>
-      <c r="H30" s="141"/>
-      <c r="I30" s="141"/>
-      <c r="J30" s="141"/>
-      <c r="K30" s="141"/>
-      <c r="L30" s="141"/>
-      <c r="M30" s="141"/>
-      <c r="N30" s="141"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="137"/>
+      <c r="I30" s="137"/>
+      <c r="J30" s="137"/>
+      <c r="K30" s="137"/>
+      <c r="L30" s="137"/>
+      <c r="M30" s="137"/>
+      <c r="N30" s="137"/>
     </row>
     <row r="31" spans="3:14" ht="18">
-      <c r="C31" s="115" t="s">
+      <c r="C31" s="114" t="s">
         <v>799</v>
       </c>
-      <c r="D31" s="141"/>
-      <c r="E31" s="141" t="s">
+      <c r="D31" s="137"/>
+      <c r="E31" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="F31" s="141"/>
-      <c r="G31" s="141"/>
-      <c r="H31" s="141"/>
-      <c r="I31" s="141"/>
-      <c r="J31" s="141"/>
-      <c r="K31" s="141"/>
-      <c r="L31" s="141"/>
-      <c r="M31" s="141"/>
-      <c r="N31" s="141"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="137"/>
+      <c r="J31" s="137"/>
+      <c r="K31" s="137"/>
+      <c r="L31" s="137"/>
+      <c r="M31" s="137"/>
+      <c r="N31" s="137"/>
     </row>
     <row r="32" spans="3:14" ht="18">
-      <c r="C32" s="115" t="s">
+      <c r="C32" s="114" t="s">
         <v>800</v>
       </c>
-      <c r="D32" s="141"/>
-      <c r="E32" s="141" t="s">
+      <c r="D32" s="137"/>
+      <c r="E32" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="F32" s="141"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="141"/>
-      <c r="I32" s="141"/>
-      <c r="J32" s="141"/>
-      <c r="K32" s="141"/>
-      <c r="L32" s="141"/>
-      <c r="M32" s="141"/>
-      <c r="N32" s="141"/>
+      <c r="F32" s="137"/>
+      <c r="G32" s="137"/>
+      <c r="H32" s="137"/>
+      <c r="I32" s="137"/>
+      <c r="J32" s="137"/>
+      <c r="K32" s="137"/>
+      <c r="L32" s="137"/>
+      <c r="M32" s="137"/>
+      <c r="N32" s="137"/>
     </row>
     <row r="33" spans="3:14" ht="18">
-      <c r="C33" s="115" t="s">
+      <c r="C33" s="114" t="s">
         <v>801</v>
       </c>
-      <c r="D33" s="141"/>
-      <c r="E33" s="141" t="s">
+      <c r="D33" s="137"/>
+      <c r="E33" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="F33" s="141"/>
-      <c r="G33" s="141"/>
-      <c r="H33" s="141"/>
-      <c r="I33" s="141"/>
-      <c r="J33" s="141"/>
-      <c r="K33" s="141"/>
-      <c r="L33" s="141"/>
-      <c r="M33" s="141"/>
-      <c r="N33" s="141"/>
+      <c r="F33" s="137"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="137"/>
+      <c r="I33" s="137"/>
+      <c r="J33" s="137"/>
+      <c r="K33" s="137"/>
+      <c r="L33" s="137"/>
+      <c r="M33" s="137"/>
+      <c r="N33" s="137"/>
     </row>
     <row r="34" spans="3:14" ht="18">
-      <c r="C34" s="115" t="s">
+      <c r="C34" s="114" t="s">
         <v>795</v>
       </c>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141" t="s">
+      <c r="D34" s="137"/>
+      <c r="E34" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="F34" s="141" t="s">
+      <c r="F34" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G34" s="141"/>
-      <c r="H34" s="141"/>
-      <c r="I34" s="141" t="s">
+      <c r="G34" s="137"/>
+      <c r="H34" s="137"/>
+      <c r="I34" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J34" s="141" t="s">
+      <c r="J34" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="K34" s="141"/>
-      <c r="L34" s="141"/>
-      <c r="M34" s="141"/>
-      <c r="N34" s="141"/>
+      <c r="K34" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="L34" s="137"/>
+      <c r="M34" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="N34" s="137"/>
     </row>
     <row r="35" spans="3:14" ht="18">
-      <c r="C35" s="115" t="s">
+      <c r="C35" s="114" t="s">
         <v>833</v>
       </c>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="141" t="s">
+      <c r="D35" s="137"/>
+      <c r="E35" s="137"/>
+      <c r="F35" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141" t="s">
+      <c r="G35" s="137"/>
+      <c r="H35" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="I35" s="141" t="s">
+      <c r="I35" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J35" s="141" t="s">
+      <c r="J35" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="K35" s="141"/>
-      <c r="L35" s="141"/>
-      <c r="M35" s="141"/>
-      <c r="N35" s="141"/>
+      <c r="K35" s="137"/>
+      <c r="L35" s="137"/>
+      <c r="M35" s="137"/>
+      <c r="N35" s="137"/>
     </row>
     <row r="36" spans="3:14" ht="18">
-      <c r="C36" s="115" t="s">
+      <c r="C36" s="114" t="s">
         <v>834</v>
       </c>
-      <c r="D36" s="141"/>
-      <c r="E36" s="141"/>
-      <c r="F36" s="141" t="s">
+      <c r="D36" s="137"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G36" s="141"/>
-      <c r="H36" s="141"/>
-      <c r="I36" s="141" t="s">
+      <c r="G36" s="137"/>
+      <c r="H36" s="137"/>
+      <c r="I36" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J36" s="141"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="141"/>
-      <c r="M36" s="141"/>
-      <c r="N36" s="141"/>
+      <c r="J36" s="137"/>
+      <c r="K36" s="137"/>
+      <c r="L36" s="137"/>
+      <c r="M36" s="137"/>
+      <c r="N36" s="137"/>
     </row>
     <row r="37" spans="3:14" ht="18">
-      <c r="C37" s="115" t="s">
+      <c r="C37" s="114" t="s">
         <v>835</v>
       </c>
-      <c r="D37" s="141"/>
-      <c r="E37" s="141"/>
-      <c r="F37" s="141" t="s">
+      <c r="D37" s="137"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G37" s="141"/>
-      <c r="H37" s="141"/>
-      <c r="I37" s="141" t="s">
+      <c r="G37" s="137"/>
+      <c r="H37" s="137"/>
+      <c r="I37" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J37" s="141"/>
-      <c r="K37" s="141"/>
-      <c r="L37" s="141"/>
-      <c r="M37" s="141"/>
-      <c r="N37" s="141"/>
+      <c r="J37" s="137"/>
+      <c r="K37" s="137"/>
+      <c r="L37" s="137"/>
+      <c r="M37" s="137"/>
+      <c r="N37" s="137"/>
     </row>
     <row r="38" spans="3:14" ht="18">
-      <c r="C38" s="115" t="s">
+      <c r="C38" s="114" t="s">
         <v>821</v>
       </c>
-      <c r="D38" s="141"/>
-      <c r="E38" s="141"/>
-      <c r="F38" s="141" t="s">
+      <c r="D38" s="137"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G38" s="141" t="s">
+      <c r="G38" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="H38" s="141"/>
-      <c r="I38" s="141" t="s">
+      <c r="H38" s="137"/>
+      <c r="I38" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J38" s="141"/>
-      <c r="K38" s="141"/>
-      <c r="L38" s="141"/>
-      <c r="M38" s="141"/>
-      <c r="N38" s="141"/>
+      <c r="J38" s="137"/>
+      <c r="K38" s="137"/>
+      <c r="L38" s="137"/>
+      <c r="M38" s="137"/>
+      <c r="N38" s="137"/>
     </row>
     <row r="39" spans="3:14" ht="18">
-      <c r="C39" s="115" t="s">
+      <c r="C39" s="114" t="s">
         <v>842</v>
       </c>
-      <c r="D39" s="141"/>
-      <c r="E39" s="141"/>
-      <c r="F39" s="141"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="141" t="s">
+      <c r="D39" s="137"/>
+      <c r="E39" s="137"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="137"/>
+      <c r="H39" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="I39" s="141" t="s">
+      <c r="I39" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J39" s="141"/>
-      <c r="K39" s="141"/>
-      <c r="L39" s="141"/>
-      <c r="M39" s="141"/>
-      <c r="N39" s="141"/>
+      <c r="J39" s="137"/>
+      <c r="K39" s="137"/>
+      <c r="L39" s="137"/>
+      <c r="M39" s="137"/>
+      <c r="N39" s="137"/>
     </row>
     <row r="40" spans="3:14" ht="18">
-      <c r="C40" s="115" t="s">
+      <c r="C40" s="114" t="s">
         <v>837</v>
       </c>
-      <c r="D40" s="141"/>
-      <c r="E40" s="141"/>
-      <c r="F40" s="141" t="s">
+      <c r="D40" s="137"/>
+      <c r="E40" s="137"/>
+      <c r="F40" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G40" s="141"/>
-      <c r="H40" s="141"/>
-      <c r="I40" s="141" t="s">
+      <c r="G40" s="137"/>
+      <c r="H40" s="137"/>
+      <c r="I40" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J40" s="141"/>
-      <c r="K40" s="141"/>
-      <c r="L40" s="141"/>
-      <c r="M40" s="141"/>
-      <c r="N40" s="141"/>
+      <c r="J40" s="137"/>
+      <c r="K40" s="137"/>
+      <c r="L40" s="137"/>
+      <c r="M40" s="137"/>
+      <c r="N40" s="137"/>
     </row>
     <row r="41" spans="3:14" ht="18">
-      <c r="C41" s="115" t="s">
+      <c r="C41" s="114" t="s">
         <v>838</v>
       </c>
-      <c r="D41" s="141"/>
-      <c r="E41" s="141"/>
-      <c r="F41" s="141" t="s">
+      <c r="D41" s="137"/>
+      <c r="E41" s="137"/>
+      <c r="F41" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="G41" s="141"/>
-      <c r="H41" s="141"/>
-      <c r="I41" s="141" t="s">
+      <c r="G41" s="137"/>
+      <c r="H41" s="137"/>
+      <c r="I41" s="137" t="s">
         <v>787</v>
       </c>
-      <c r="J41" s="141"/>
-      <c r="K41" s="141"/>
-      <c r="L41" s="141"/>
-      <c r="M41" s="141"/>
-      <c r="N41" s="141"/>
-    </row>
-    <row r="42" spans="3:14" ht="18">
-      <c r="C42" s="115"/>
-      <c r="D42" s="141"/>
-      <c r="E42" s="141"/>
-      <c r="F42" s="141"/>
-      <c r="G42" s="141"/>
-      <c r="H42" s="141"/>
-      <c r="I42" s="141"/>
-      <c r="J42" s="141"/>
-      <c r="K42" s="141"/>
-      <c r="L42" s="141"/>
-      <c r="M42" s="141"/>
-      <c r="N42" s="141"/>
-    </row>
-    <row r="43" spans="3:14">
-      <c r="C43" s="116"/>
-      <c r="D43" s="142"/>
-      <c r="E43" s="142"/>
-      <c r="F43" s="142"/>
-      <c r="G43" s="142"/>
-      <c r="H43" s="142"/>
-      <c r="I43" s="142"/>
-      <c r="J43" s="142"/>
-      <c r="K43" s="142"/>
-      <c r="L43" s="142"/>
-      <c r="M43" s="142"/>
-      <c r="N43" s="142"/>
+      <c r="J41" s="137"/>
+      <c r="K41" s="137"/>
+      <c r="L41" s="137"/>
+      <c r="M41" s="137"/>
+      <c r="N41" s="137"/>
+    </row>
+    <row r="42" spans="3:14" ht="19">
+      <c r="C42" s="114" t="s">
+        <v>861</v>
+      </c>
+      <c r="D42" s="137"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="137"/>
+      <c r="G42" s="137"/>
+      <c r="H42" s="137"/>
+      <c r="I42" s="137"/>
+      <c r="J42" s="137"/>
+      <c r="K42" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="L42" s="137"/>
+      <c r="M42" s="137"/>
+      <c r="N42" s="137"/>
+    </row>
+    <row r="43" spans="3:14" ht="18">
+      <c r="C43" s="114" t="s">
+        <v>862</v>
+      </c>
+      <c r="D43" s="138"/>
+      <c r="E43" s="138"/>
+      <c r="F43" s="138"/>
+      <c r="G43" s="138"/>
+      <c r="H43" s="138"/>
+      <c r="I43" s="138"/>
+      <c r="J43" s="138"/>
+      <c r="K43" s="137" t="s">
+        <v>787</v>
+      </c>
+      <c r="L43" s="138"/>
+      <c r="M43" s="138"/>
+      <c r="N43" s="138"/>
     </row>
     <row r="44" spans="3:14" ht="19" thickBot="1">
-      <c r="C44" s="115"/>
-      <c r="D44" s="141"/>
-      <c r="E44" s="141"/>
-      <c r="F44" s="141"/>
-      <c r="G44" s="141"/>
-      <c r="H44" s="141"/>
-      <c r="I44" s="141"/>
-      <c r="J44" s="182"/>
-      <c r="K44" s="143"/>
-      <c r="L44" s="143"/>
-      <c r="M44" s="143"/>
-      <c r="N44" s="143"/>
+      <c r="C44" s="211"/>
+      <c r="D44" s="201"/>
+      <c r="E44" s="201"/>
+      <c r="F44" s="201"/>
+      <c r="G44" s="201"/>
+      <c r="H44" s="201"/>
+      <c r="I44" s="201"/>
+      <c r="J44" s="201"/>
+      <c r="K44" s="139"/>
+      <c r="L44" s="139"/>
+      <c r="M44" s="139"/>
+      <c r="N44" s="139"/>
     </row>
     <row r="45" spans="3:14" ht="17" thickBot="1">
-      <c r="C45" s="122"/>
-      <c r="D45" s="110"/>
-      <c r="E45" s="110"/>
-      <c r="F45" s="110"/>
-      <c r="G45" s="110"/>
-      <c r="H45" s="110"/>
-      <c r="I45" s="110"/>
-      <c r="J45" s="110"/>
-      <c r="K45" s="110"/>
-      <c r="L45" s="110"/>
-      <c r="M45" s="110"/>
-      <c r="N45" s="125"/>
+      <c r="C45" s="204"/>
+      <c r="D45" s="205"/>
+      <c r="E45" s="205"/>
+      <c r="F45" s="205"/>
+      <c r="G45" s="205"/>
+      <c r="H45" s="205"/>
+      <c r="I45" s="205"/>
+      <c r="J45" s="205"/>
+      <c r="K45" s="205"/>
+      <c r="L45" s="205"/>
+      <c r="M45" s="205"/>
+      <c r="N45" s="206"/>
     </row>
     <row r="46" spans="3:14" ht="18">
-      <c r="C46" s="126" t="s">
+      <c r="C46" s="124" t="s">
         <v>803</v>
       </c>
-      <c r="D46" s="144"/>
-      <c r="E46" s="144"/>
-      <c r="F46" s="144"/>
-      <c r="G46" s="144"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="144"/>
-      <c r="J46" s="144"/>
-      <c r="K46" s="144"/>
-      <c r="L46" s="144"/>
-      <c r="M46" s="144"/>
-      <c r="N46" s="144"/>
+      <c r="D46" s="190"/>
+      <c r="E46" s="190"/>
+      <c r="F46" s="190"/>
+      <c r="G46" s="190"/>
+      <c r="H46" s="190"/>
+      <c r="I46" s="190"/>
+      <c r="J46" s="190"/>
+      <c r="K46" s="195"/>
+      <c r="L46" s="190"/>
+      <c r="M46" s="195"/>
+      <c r="N46" s="190"/>
     </row>
     <row r="47" spans="3:14" ht="18">
-      <c r="C47" s="127" t="s">
+      <c r="C47" s="125" t="s">
         <v>797</v>
       </c>
-      <c r="D47" s="145"/>
-      <c r="E47" s="145" t="s">
+      <c r="D47" s="191"/>
+      <c r="E47" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="F47" s="145" t="s">
+      <c r="F47" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G47" s="145"/>
-      <c r="H47" s="145"/>
-      <c r="I47" s="145"/>
-      <c r="J47" s="145"/>
-      <c r="K47" s="145"/>
-      <c r="L47" s="145"/>
-      <c r="M47" s="145"/>
-      <c r="N47" s="145"/>
+      <c r="G47" s="191"/>
+      <c r="H47" s="191"/>
+      <c r="I47" s="191"/>
+      <c r="J47" s="191"/>
+      <c r="K47" s="196"/>
+      <c r="L47" s="191"/>
+      <c r="M47" s="196"/>
+      <c r="N47" s="191"/>
     </row>
     <row r="48" spans="3:14" ht="18">
-      <c r="C48" s="127" t="s">
+      <c r="C48" s="125" t="s">
         <v>804</v>
       </c>
-      <c r="D48" s="145"/>
-      <c r="E48" s="145" t="s">
+      <c r="D48" s="191"/>
+      <c r="E48" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="F48" s="145" t="s">
+      <c r="F48" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G48" s="145"/>
-      <c r="H48" s="145"/>
-      <c r="I48" s="145" t="s">
+      <c r="G48" s="191"/>
+      <c r="H48" s="191"/>
+      <c r="I48" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J48" s="145" t="s">
+      <c r="J48" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="K48" s="145"/>
-      <c r="L48" s="145"/>
-      <c r="M48" s="145"/>
-      <c r="N48" s="145"/>
+      <c r="K48" s="196"/>
+      <c r="L48" s="191"/>
+      <c r="M48" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="N48" s="191"/>
     </row>
     <row r="49" spans="3:14" ht="18">
-      <c r="C49" s="127" t="s">
+      <c r="C49" s="125" t="s">
         <v>805</v>
       </c>
-      <c r="D49" s="145"/>
-      <c r="E49" s="145" t="s">
+      <c r="D49" s="191"/>
+      <c r="E49" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="F49" s="145" t="s">
+      <c r="F49" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G49" s="145"/>
-      <c r="H49" s="145"/>
-      <c r="I49" s="145"/>
-      <c r="J49" s="145"/>
-      <c r="K49" s="145"/>
-      <c r="L49" s="145"/>
-      <c r="M49" s="145"/>
-      <c r="N49" s="145"/>
+      <c r="G49" s="191"/>
+      <c r="H49" s="191"/>
+      <c r="I49" s="191"/>
+      <c r="J49" s="191"/>
+      <c r="K49" s="196"/>
+      <c r="L49" s="191"/>
+      <c r="M49" s="196"/>
+      <c r="N49" s="191"/>
     </row>
     <row r="50" spans="3:14" ht="18">
-      <c r="C50" s="127" t="s">
+      <c r="C50" s="125" t="s">
         <v>806</v>
       </c>
-      <c r="D50" s="145"/>
-      <c r="E50" s="145" t="s">
+      <c r="D50" s="191"/>
+      <c r="E50" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="F50" s="145"/>
-      <c r="G50" s="145"/>
-      <c r="H50" s="145"/>
-      <c r="I50" s="145" t="s">
+      <c r="F50" s="191"/>
+      <c r="G50" s="191"/>
+      <c r="H50" s="191"/>
+      <c r="I50" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J50" s="145"/>
-      <c r="K50" s="145"/>
-      <c r="L50" s="145"/>
-      <c r="M50" s="145"/>
-      <c r="N50" s="145"/>
+      <c r="J50" s="191"/>
+      <c r="K50" s="196"/>
+      <c r="L50" s="191"/>
+      <c r="M50" s="196"/>
+      <c r="N50" s="191"/>
     </row>
     <row r="51" spans="3:14" ht="19">
-      <c r="C51" s="127" t="s">
+      <c r="C51" s="125" t="s">
         <v>810</v>
       </c>
-      <c r="D51" s="145"/>
-      <c r="E51" s="145" t="s">
+      <c r="D51" s="191"/>
+      <c r="E51" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="F51" s="145"/>
-      <c r="G51" s="145"/>
-      <c r="H51" s="145"/>
-      <c r="I51" s="145"/>
-      <c r="J51" s="145"/>
-      <c r="K51" s="145"/>
-      <c r="L51" s="145"/>
-      <c r="M51" s="145"/>
-      <c r="N51" s="145"/>
+      <c r="F51" s="191"/>
+      <c r="G51" s="191"/>
+      <c r="H51" s="191"/>
+      <c r="I51" s="191"/>
+      <c r="J51" s="191"/>
+      <c r="K51" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L51" s="191"/>
+      <c r="M51" s="196"/>
+      <c r="N51" s="191"/>
     </row>
     <row r="52" spans="3:14" ht="18">
-      <c r="C52" s="127" t="s">
+      <c r="C52" s="125" t="s">
         <v>825</v>
       </c>
-      <c r="D52" s="145"/>
-      <c r="E52" s="145"/>
-      <c r="F52" s="145" t="s">
+      <c r="D52" s="191"/>
+      <c r="E52" s="191"/>
+      <c r="F52" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G52" s="145"/>
-      <c r="H52" s="145"/>
-      <c r="I52" s="145" t="s">
+      <c r="G52" s="191"/>
+      <c r="H52" s="191"/>
+      <c r="I52" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J52" s="145"/>
-      <c r="K52" s="145"/>
-      <c r="L52" s="145"/>
-      <c r="M52" s="145"/>
-      <c r="N52" s="145"/>
+      <c r="J52" s="191"/>
+      <c r="K52" s="196"/>
+      <c r="L52" s="191"/>
+      <c r="M52" s="196"/>
+      <c r="N52" s="191"/>
     </row>
     <row r="53" spans="3:14" ht="18">
-      <c r="C53" s="127" t="s">
+      <c r="C53" s="125" t="s">
         <v>826</v>
       </c>
-      <c r="D53" s="145"/>
-      <c r="E53" s="145"/>
-      <c r="F53" s="145" t="s">
+      <c r="D53" s="191"/>
+      <c r="E53" s="191"/>
+      <c r="F53" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G53" s="145"/>
-      <c r="H53" s="145"/>
-      <c r="I53" s="145" t="s">
+      <c r="G53" s="191"/>
+      <c r="H53" s="191"/>
+      <c r="I53" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J53" s="145"/>
-      <c r="K53" s="145"/>
-      <c r="L53" s="145"/>
-      <c r="M53" s="145"/>
-      <c r="N53" s="145"/>
+      <c r="J53" s="191"/>
+      <c r="K53" s="196"/>
+      <c r="L53" s="191"/>
+      <c r="M53" s="196"/>
+      <c r="N53" s="191"/>
     </row>
     <row r="54" spans="3:14" ht="18">
-      <c r="C54" s="127" t="s">
+      <c r="C54" s="125" t="s">
         <v>830</v>
       </c>
-      <c r="D54" s="127"/>
-      <c r="E54" s="127"/>
-      <c r="F54" s="145" t="s">
+      <c r="D54" s="194"/>
+      <c r="E54" s="194"/>
+      <c r="F54" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G54" s="145" t="s">
+      <c r="G54" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="H54" s="145" t="s">
+      <c r="H54" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="I54" s="145" t="s">
+      <c r="I54" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J54" s="145" t="s">
+      <c r="J54" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="K54" s="145"/>
-      <c r="L54" s="145"/>
-      <c r="M54" s="145"/>
-      <c r="N54" s="145"/>
+      <c r="K54" s="196"/>
+      <c r="L54" s="191"/>
+      <c r="M54" s="196"/>
+      <c r="N54" s="191"/>
     </row>
     <row r="55" spans="3:14" ht="18">
-      <c r="C55" s="127" t="s">
+      <c r="C55" s="125" t="s">
         <v>831</v>
       </c>
-      <c r="D55" s="127"/>
-      <c r="E55" s="127"/>
-      <c r="F55" s="145" t="s">
+      <c r="D55" s="194"/>
+      <c r="E55" s="194"/>
+      <c r="F55" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G55" s="145"/>
-      <c r="H55" s="145"/>
-      <c r="I55" s="145" t="s">
+      <c r="G55" s="191"/>
+      <c r="H55" s="191"/>
+      <c r="I55" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J55" s="145"/>
-      <c r="K55" s="145"/>
-      <c r="L55" s="145"/>
-      <c r="M55" s="145"/>
-      <c r="N55" s="145"/>
+      <c r="J55" s="191"/>
+      <c r="K55" s="196"/>
+      <c r="L55" s="191"/>
+      <c r="M55" s="196"/>
+      <c r="N55" s="191"/>
     </row>
     <row r="56" spans="3:14" ht="18">
-      <c r="C56" s="127" t="s">
+      <c r="C56" s="125" t="s">
         <v>832</v>
       </c>
-      <c r="D56" s="127"/>
-      <c r="E56" s="127"/>
-      <c r="F56" s="145" t="s">
+      <c r="D56" s="194"/>
+      <c r="E56" s="194"/>
+      <c r="F56" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="G56" s="145"/>
-      <c r="H56" s="145"/>
-      <c r="I56" s="145" t="s">
+      <c r="G56" s="191"/>
+      <c r="H56" s="191"/>
+      <c r="I56" s="191" t="s">
         <v>787</v>
       </c>
-      <c r="J56" s="145"/>
-      <c r="K56" s="145"/>
-      <c r="L56" s="145"/>
-      <c r="M56" s="145"/>
-      <c r="N56" s="145"/>
+      <c r="J56" s="191"/>
+      <c r="K56" s="196"/>
+      <c r="L56" s="191"/>
+      <c r="M56" s="196"/>
+      <c r="N56" s="191"/>
     </row>
     <row r="57" spans="3:14" ht="18">
-      <c r="C57" s="127"/>
-      <c r="D57" s="145"/>
-      <c r="E57" s="145"/>
-      <c r="F57" s="145"/>
-      <c r="G57" s="145"/>
-      <c r="H57" s="145"/>
-      <c r="I57" s="145"/>
-      <c r="J57" s="145"/>
-      <c r="K57" s="145"/>
-      <c r="L57" s="145"/>
-      <c r="M57" s="145"/>
-      <c r="N57" s="145"/>
+      <c r="C57" s="125" t="s">
+        <v>863</v>
+      </c>
+      <c r="D57" s="194"/>
+      <c r="E57" s="194"/>
+      <c r="F57" s="191"/>
+      <c r="G57" s="191"/>
+      <c r="H57" s="191"/>
+      <c r="I57" s="191"/>
+      <c r="J57" s="191"/>
+      <c r="K57" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L57" s="191"/>
+      <c r="M57" s="196"/>
+      <c r="N57" s="191"/>
     </row>
     <row r="58" spans="3:14" ht="18">
-      <c r="C58" s="127"/>
-      <c r="D58" s="145"/>
-      <c r="E58" s="145"/>
-      <c r="F58" s="145"/>
-      <c r="G58" s="145"/>
-      <c r="H58" s="145"/>
-      <c r="I58" s="145"/>
-      <c r="J58" s="145"/>
-      <c r="K58" s="145"/>
-      <c r="L58" s="145"/>
-      <c r="M58" s="145"/>
-      <c r="N58" s="145"/>
+      <c r="C58" s="125" t="s">
+        <v>854</v>
+      </c>
+      <c r="D58" s="194"/>
+      <c r="E58" s="194"/>
+      <c r="F58" s="191"/>
+      <c r="G58" s="191"/>
+      <c r="H58" s="191"/>
+      <c r="I58" s="191"/>
+      <c r="J58" s="191"/>
+      <c r="K58" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L58" s="191"/>
+      <c r="M58" s="196"/>
+      <c r="N58" s="191"/>
     </row>
     <row r="59" spans="3:14" ht="18">
-      <c r="C59" s="127"/>
-      <c r="D59" s="145"/>
-      <c r="E59" s="145"/>
-      <c r="F59" s="145"/>
-      <c r="G59" s="145"/>
-      <c r="H59" s="145"/>
-      <c r="I59" s="145"/>
-      <c r="J59" s="145"/>
-      <c r="K59" s="145"/>
-      <c r="L59" s="145"/>
-      <c r="M59" s="145"/>
-      <c r="N59" s="145"/>
-    </row>
-    <row r="60" spans="3:14">
-      <c r="C60" s="128"/>
-      <c r="D60" s="146"/>
-      <c r="E60" s="146"/>
-      <c r="F60" s="146"/>
-      <c r="G60" s="146"/>
-      <c r="H60" s="146"/>
-      <c r="I60" s="146"/>
-      <c r="J60" s="146"/>
-      <c r="K60" s="146"/>
-      <c r="L60" s="146"/>
-      <c r="M60" s="146"/>
-      <c r="N60" s="146"/>
-    </row>
-    <row r="61" spans="3:14" ht="19" thickBot="1">
-      <c r="C61" s="127"/>
-      <c r="D61" s="145"/>
-      <c r="E61" s="145"/>
-      <c r="F61" s="145"/>
-      <c r="G61" s="145"/>
-      <c r="H61" s="145"/>
-      <c r="I61" s="145"/>
-      <c r="J61" s="183"/>
-      <c r="K61" s="147"/>
-      <c r="L61" s="147"/>
-      <c r="M61" s="147"/>
-      <c r="N61" s="147"/>
-    </row>
-    <row r="62" spans="3:14" ht="17" thickBot="1">
-      <c r="C62" s="122"/>
-      <c r="D62" s="110"/>
-      <c r="E62" s="110"/>
-      <c r="F62" s="110"/>
-      <c r="G62" s="110"/>
-      <c r="H62" s="110"/>
-      <c r="I62" s="110"/>
-      <c r="J62" s="110"/>
-      <c r="K62" s="110"/>
-      <c r="L62" s="110"/>
-      <c r="M62" s="110"/>
-      <c r="N62" s="125"/>
+      <c r="C59" s="125" t="s">
+        <v>855</v>
+      </c>
+      <c r="D59" s="194"/>
+      <c r="E59" s="194"/>
+      <c r="F59" s="191"/>
+      <c r="G59" s="191"/>
+      <c r="H59" s="191"/>
+      <c r="I59" s="191"/>
+      <c r="J59" s="191"/>
+      <c r="K59" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L59" s="191"/>
+      <c r="M59" s="196"/>
+      <c r="N59" s="191"/>
+    </row>
+    <row r="60" spans="3:14" ht="19">
+      <c r="C60" s="125" t="s">
+        <v>856</v>
+      </c>
+      <c r="D60" s="194"/>
+      <c r="E60" s="194"/>
+      <c r="F60" s="191"/>
+      <c r="G60" s="191"/>
+      <c r="H60" s="191"/>
+      <c r="I60" s="191"/>
+      <c r="J60" s="191"/>
+      <c r="K60" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L60" s="191"/>
+      <c r="M60" s="196"/>
+      <c r="N60" s="191"/>
+    </row>
+    <row r="61" spans="3:14" ht="19">
+      <c r="C61" s="125" t="s">
+        <v>857</v>
+      </c>
+      <c r="D61" s="194"/>
+      <c r="E61" s="194"/>
+      <c r="F61" s="191"/>
+      <c r="G61" s="191"/>
+      <c r="H61" s="191"/>
+      <c r="I61" s="191"/>
+      <c r="J61" s="191"/>
+      <c r="K61" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L61" s="199"/>
+      <c r="M61" s="200"/>
+      <c r="N61" s="199"/>
+    </row>
+    <row r="62" spans="3:14" ht="19">
+      <c r="C62" s="125" t="s">
+        <v>857</v>
+      </c>
+      <c r="D62" s="194"/>
+      <c r="E62" s="194"/>
+      <c r="F62" s="191"/>
+      <c r="G62" s="191"/>
+      <c r="H62" s="191"/>
+      <c r="I62" s="191"/>
+      <c r="J62" s="191"/>
+      <c r="K62" s="196" t="s">
+        <v>787</v>
+      </c>
+      <c r="L62" s="216"/>
+      <c r="M62" s="217"/>
+      <c r="N62" s="216"/>
     </row>
     <row r="63" spans="3:14" ht="18">
-      <c r="C63" s="117" t="s">
+      <c r="C63" s="212"/>
+      <c r="D63" s="213"/>
+      <c r="E63" s="213"/>
+      <c r="F63" s="214"/>
+      <c r="G63" s="214"/>
+      <c r="H63" s="214"/>
+      <c r="I63" s="214"/>
+      <c r="J63" s="214"/>
+      <c r="K63" s="215"/>
+      <c r="L63" s="216"/>
+      <c r="M63" s="217"/>
+      <c r="N63" s="216"/>
+    </row>
+    <row r="64" spans="3:14" ht="18">
+      <c r="C64" s="212"/>
+      <c r="D64" s="213"/>
+      <c r="E64" s="213"/>
+      <c r="F64" s="214"/>
+      <c r="G64" s="214"/>
+      <c r="H64" s="214"/>
+      <c r="I64" s="214"/>
+      <c r="J64" s="214"/>
+      <c r="K64" s="215"/>
+      <c r="L64" s="216"/>
+      <c r="M64" s="217"/>
+      <c r="N64" s="216"/>
+    </row>
+    <row r="65" spans="3:14" ht="18">
+      <c r="C65" s="212"/>
+      <c r="D65" s="213"/>
+      <c r="E65" s="213"/>
+      <c r="F65" s="214"/>
+      <c r="G65" s="214"/>
+      <c r="H65" s="214"/>
+      <c r="I65" s="214"/>
+      <c r="J65" s="214"/>
+      <c r="K65" s="215"/>
+      <c r="L65" s="216"/>
+      <c r="M65" s="217"/>
+      <c r="N65" s="216"/>
+    </row>
+    <row r="66" spans="3:14" ht="19" thickBot="1">
+      <c r="C66" s="192"/>
+      <c r="D66" s="197"/>
+      <c r="E66" s="197"/>
+      <c r="F66" s="197"/>
+      <c r="G66" s="197"/>
+      <c r="H66" s="197"/>
+      <c r="I66" s="197"/>
+      <c r="J66" s="197"/>
+      <c r="K66" s="198"/>
+      <c r="L66" s="193"/>
+      <c r="M66" s="198"/>
+      <c r="N66" s="193"/>
+    </row>
+    <row r="67" spans="3:14" ht="17" thickBot="1">
+      <c r="C67" s="120"/>
+      <c r="D67" s="110"/>
+      <c r="E67" s="110"/>
+      <c r="F67" s="110"/>
+      <c r="G67" s="110"/>
+      <c r="H67" s="110"/>
+      <c r="I67" s="110"/>
+      <c r="J67" s="110"/>
+      <c r="K67" s="110"/>
+      <c r="L67" s="110"/>
+      <c r="M67" s="110"/>
+      <c r="N67" s="123"/>
+    </row>
+    <row r="68" spans="3:14" ht="18">
+      <c r="C68" s="115" t="s">
         <v>808</v>
       </c>
-      <c r="D63" s="148"/>
-      <c r="E63" s="148"/>
-      <c r="F63" s="148"/>
-      <c r="G63" s="148"/>
-      <c r="H63" s="148"/>
-      <c r="I63" s="148"/>
-      <c r="J63" s="148"/>
-      <c r="K63" s="148"/>
-      <c r="L63" s="148"/>
-      <c r="M63" s="148"/>
-      <c r="N63" s="148"/>
-    </row>
-    <row r="64" spans="3:14" ht="19">
-      <c r="C64" s="118" t="s">
+      <c r="D68" s="140"/>
+      <c r="E68" s="140"/>
+      <c r="F68" s="140"/>
+      <c r="G68" s="140"/>
+      <c r="H68" s="140"/>
+      <c r="I68" s="140"/>
+      <c r="J68" s="140"/>
+      <c r="K68" s="140"/>
+      <c r="L68" s="140"/>
+      <c r="M68" s="140"/>
+      <c r="N68" s="140"/>
+    </row>
+    <row r="69" spans="3:14" ht="19">
+      <c r="C69" s="116" t="s">
         <v>811</v>
       </c>
-      <c r="D64" s="149"/>
-      <c r="E64" s="149" t="s">
+      <c r="D69" s="141"/>
+      <c r="E69" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="F64" s="149" t="s">
+      <c r="F69" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="G64" s="149"/>
-      <c r="H64" s="149"/>
-      <c r="I64" s="149"/>
-      <c r="J64" s="149"/>
-      <c r="K64" s="149"/>
-      <c r="L64" s="149"/>
-      <c r="M64" s="149"/>
-      <c r="N64" s="149"/>
-    </row>
-    <row r="65" spans="3:14" ht="19">
-      <c r="C65" s="118" t="s">
+      <c r="G69" s="141"/>
+      <c r="H69" s="141"/>
+      <c r="I69" s="141"/>
+      <c r="J69" s="141"/>
+      <c r="K69" s="141"/>
+      <c r="L69" s="141"/>
+      <c r="M69" s="141"/>
+      <c r="N69" s="141"/>
+    </row>
+    <row r="70" spans="3:14" ht="19">
+      <c r="C70" s="116" t="s">
         <v>812</v>
       </c>
-      <c r="D65" s="149"/>
-      <c r="E65" s="149" t="s">
+      <c r="D70" s="141"/>
+      <c r="E70" s="141" t="s">
         <v>787</v>
       </c>
-      <c r="F65" s="149"/>
-      <c r="G65" s="149"/>
-      <c r="H65" s="149"/>
-      <c r="I65" s="149"/>
-      <c r="J65" s="149"/>
-      <c r="K65" s="149"/>
-      <c r="L65" s="149"/>
-      <c r="M65" s="149"/>
-      <c r="N65" s="149"/>
-    </row>
-    <row r="66" spans="3:14" ht="18">
-      <c r="C66" s="118"/>
-      <c r="D66" s="149"/>
-      <c r="E66" s="149"/>
-      <c r="F66" s="149"/>
-      <c r="G66" s="149"/>
-      <c r="H66" s="149"/>
-      <c r="I66" s="149"/>
-      <c r="J66" s="149"/>
-      <c r="K66" s="149"/>
-      <c r="L66" s="149"/>
-      <c r="M66" s="149"/>
-      <c r="N66" s="149"/>
-    </row>
-    <row r="67" spans="3:14" ht="18">
-      <c r="C67" s="118"/>
-      <c r="D67" s="149"/>
-      <c r="E67" s="149"/>
-      <c r="F67" s="149"/>
-      <c r="G67" s="149"/>
-      <c r="H67" s="149"/>
-      <c r="I67" s="149"/>
-      <c r="J67" s="149"/>
-      <c r="K67" s="149"/>
-      <c r="L67" s="149"/>
-      <c r="M67" s="149"/>
-      <c r="N67" s="149"/>
-    </row>
-    <row r="68" spans="3:14" ht="18">
-      <c r="C68" s="118"/>
-      <c r="D68" s="149"/>
-      <c r="E68" s="149"/>
-      <c r="F68" s="149"/>
-      <c r="G68" s="149"/>
-      <c r="H68" s="149"/>
-      <c r="I68" s="149"/>
-      <c r="J68" s="149"/>
-      <c r="K68" s="149"/>
-      <c r="L68" s="149"/>
-      <c r="M68" s="149"/>
-      <c r="N68" s="149"/>
-    </row>
-    <row r="69" spans="3:14" ht="18">
-      <c r="C69" s="118"/>
-      <c r="D69" s="149"/>
-      <c r="E69" s="149"/>
-      <c r="F69" s="149"/>
-      <c r="G69" s="149"/>
-      <c r="H69" s="149"/>
-      <c r="I69" s="149"/>
-      <c r="J69" s="149"/>
-      <c r="K69" s="149"/>
-      <c r="L69" s="149"/>
-      <c r="M69" s="149"/>
-      <c r="N69" s="149"/>
-    </row>
-    <row r="70" spans="3:14" ht="18">
-      <c r="C70" s="118"/>
-      <c r="D70" s="149"/>
-      <c r="E70" s="149"/>
-      <c r="F70" s="149"/>
-      <c r="G70" s="149"/>
-      <c r="H70" s="149"/>
-      <c r="I70" s="149"/>
-      <c r="J70" s="149"/>
-      <c r="K70" s="149"/>
-      <c r="L70" s="149"/>
-      <c r="M70" s="149"/>
-      <c r="N70" s="149"/>
-    </row>
-    <row r="71" spans="3:14" ht="18">
-      <c r="C71" s="118"/>
-      <c r="D71" s="149"/>
-      <c r="E71" s="149"/>
-      <c r="F71" s="149"/>
-      <c r="G71" s="149"/>
-      <c r="H71" s="149"/>
-      <c r="I71" s="149"/>
-      <c r="J71" s="149"/>
-      <c r="K71" s="149"/>
-      <c r="L71" s="149"/>
-      <c r="M71" s="149"/>
-      <c r="N71" s="149"/>
+      <c r="F70" s="141"/>
+      <c r="G70" s="141"/>
+      <c r="H70" s="141"/>
+      <c r="I70" s="141"/>
+      <c r="J70" s="141"/>
+      <c r="K70" s="141"/>
+      <c r="L70" s="141"/>
+      <c r="M70" s="141"/>
+      <c r="N70" s="141"/>
+    </row>
+    <row r="71" spans="3:14" ht="19">
+      <c r="C71" s="116" t="s">
+        <v>858</v>
+      </c>
+      <c r="D71" s="141"/>
+      <c r="E71" s="141"/>
+      <c r="F71" s="141"/>
+      <c r="G71" s="141"/>
+      <c r="H71" s="141"/>
+      <c r="I71" s="141"/>
+      <c r="J71" s="141"/>
+      <c r="K71" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="L71" s="141"/>
+      <c r="M71" s="141"/>
+      <c r="N71" s="141"/>
     </row>
     <row r="72" spans="3:14" ht="18">
-      <c r="C72" s="118"/>
-      <c r="D72" s="149"/>
-      <c r="E72" s="149"/>
-      <c r="F72" s="149"/>
-      <c r="G72" s="149"/>
-      <c r="H72" s="149"/>
-      <c r="I72" s="149"/>
-      <c r="J72" s="149"/>
-      <c r="K72" s="149"/>
-      <c r="L72" s="149"/>
-      <c r="M72" s="149"/>
-      <c r="N72" s="149"/>
-    </row>
-    <row r="73" spans="3:14">
-      <c r="C73" s="119"/>
-      <c r="D73" s="150"/>
-      <c r="E73" s="150"/>
-      <c r="F73" s="150"/>
-      <c r="G73" s="150"/>
-      <c r="H73" s="150"/>
-      <c r="I73" s="150"/>
-      <c r="J73" s="150"/>
-      <c r="K73" s="150"/>
-      <c r="L73" s="150"/>
-      <c r="M73" s="150"/>
-      <c r="N73" s="150"/>
-    </row>
-    <row r="74" spans="3:14" ht="17" thickBot="1">
-      <c r="C74" s="120"/>
-      <c r="D74" s="151"/>
-      <c r="E74" s="151"/>
-      <c r="F74" s="151"/>
-      <c r="G74" s="151"/>
-      <c r="H74" s="151"/>
-      <c r="I74" s="151"/>
-      <c r="J74" s="151"/>
-      <c r="K74" s="151"/>
-      <c r="L74" s="151"/>
-      <c r="M74" s="151"/>
-      <c r="N74" s="151"/>
-    </row>
-    <row r="75" spans="3:14" ht="17" thickBot="1">
-      <c r="C75" s="122"/>
-      <c r="D75" s="110"/>
-      <c r="E75" s="110"/>
-      <c r="F75" s="110"/>
-      <c r="G75" s="110"/>
-      <c r="H75" s="110"/>
-      <c r="I75" s="110"/>
-      <c r="J75" s="110"/>
-      <c r="K75" s="110"/>
-      <c r="L75" s="110"/>
-      <c r="M75" s="110"/>
-      <c r="N75" s="125"/>
-    </row>
-    <row r="76" spans="3:14" ht="19">
-      <c r="C76" s="132" t="s">
+      <c r="C72" s="116" t="s">
+        <v>859</v>
+      </c>
+      <c r="D72" s="141"/>
+      <c r="E72" s="141"/>
+      <c r="F72" s="141"/>
+      <c r="G72" s="141"/>
+      <c r="H72" s="141"/>
+      <c r="I72" s="141"/>
+      <c r="J72" s="141"/>
+      <c r="K72" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="L72" s="141"/>
+      <c r="M72" s="141"/>
+      <c r="N72" s="141"/>
+    </row>
+    <row r="73" spans="3:14" ht="19">
+      <c r="C73" s="116" t="s">
+        <v>860</v>
+      </c>
+      <c r="D73" s="141"/>
+      <c r="E73" s="141"/>
+      <c r="F73" s="141"/>
+      <c r="G73" s="141"/>
+      <c r="H73" s="141"/>
+      <c r="I73" s="141"/>
+      <c r="J73" s="141"/>
+      <c r="K73" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="L73" s="141"/>
+      <c r="M73" s="141"/>
+      <c r="N73" s="141"/>
+    </row>
+    <row r="74" spans="3:14" ht="19">
+      <c r="C74" s="116" t="s">
+        <v>864</v>
+      </c>
+      <c r="D74" s="141"/>
+      <c r="E74" s="141"/>
+      <c r="F74" s="141"/>
+      <c r="G74" s="141"/>
+      <c r="H74" s="141"/>
+      <c r="I74" s="141"/>
+      <c r="J74" s="141"/>
+      <c r="K74" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="L74" s="141"/>
+      <c r="M74" s="141"/>
+      <c r="N74" s="141"/>
+    </row>
+    <row r="75" spans="3:14" ht="18">
+      <c r="C75" s="116" t="s">
+        <v>865</v>
+      </c>
+      <c r="D75" s="141"/>
+      <c r="E75" s="141"/>
+      <c r="F75" s="141"/>
+      <c r="G75" s="141"/>
+      <c r="H75" s="141"/>
+      <c r="I75" s="141"/>
+      <c r="J75" s="141"/>
+      <c r="K75" s="141" t="s">
+        <v>787</v>
+      </c>
+      <c r="L75" s="141"/>
+      <c r="M75" s="141"/>
+      <c r="N75" s="141"/>
+    </row>
+    <row r="76" spans="3:14" ht="18">
+      <c r="C76" s="116"/>
+      <c r="D76" s="141"/>
+      <c r="E76" s="141"/>
+      <c r="F76" s="141"/>
+      <c r="G76" s="141"/>
+      <c r="H76" s="141"/>
+      <c r="I76" s="141"/>
+      <c r="J76" s="141"/>
+      <c r="K76" s="141"/>
+      <c r="L76" s="141"/>
+      <c r="M76" s="141"/>
+      <c r="N76" s="141"/>
+    </row>
+    <row r="77" spans="3:14" ht="18">
+      <c r="C77" s="116"/>
+      <c r="D77" s="141"/>
+      <c r="E77" s="141"/>
+      <c r="F77" s="141"/>
+      <c r="G77" s="141"/>
+      <c r="H77" s="141"/>
+      <c r="I77" s="141"/>
+      <c r="J77" s="141"/>
+      <c r="K77" s="141"/>
+      <c r="L77" s="141"/>
+      <c r="M77" s="141"/>
+      <c r="N77" s="141"/>
+    </row>
+    <row r="78" spans="3:14">
+      <c r="C78" s="117"/>
+      <c r="D78" s="142"/>
+      <c r="E78" s="142"/>
+      <c r="F78" s="142"/>
+      <c r="G78" s="142"/>
+      <c r="H78" s="142"/>
+      <c r="I78" s="142"/>
+      <c r="J78" s="142"/>
+      <c r="K78" s="142"/>
+      <c r="L78" s="142"/>
+      <c r="M78" s="142"/>
+      <c r="N78" s="142"/>
+    </row>
+    <row r="79" spans="3:14" ht="17" thickBot="1">
+      <c r="C79" s="118"/>
+      <c r="D79" s="143"/>
+      <c r="E79" s="143"/>
+      <c r="F79" s="143"/>
+      <c r="G79" s="143"/>
+      <c r="H79" s="143"/>
+      <c r="I79" s="143"/>
+      <c r="J79" s="143"/>
+      <c r="K79" s="143"/>
+      <c r="L79" s="143"/>
+      <c r="M79" s="143"/>
+      <c r="N79" s="143"/>
+    </row>
+    <row r="80" spans="3:14" ht="17" thickBot="1">
+      <c r="C80" s="120"/>
+      <c r="D80" s="110"/>
+      <c r="E80" s="110"/>
+      <c r="F80" s="110"/>
+      <c r="G80" s="110"/>
+      <c r="H80" s="110"/>
+      <c r="I80" s="110"/>
+      <c r="J80" s="110"/>
+      <c r="K80" s="110"/>
+      <c r="L80" s="110"/>
+      <c r="M80" s="110"/>
+      <c r="N80" s="123"/>
+    </row>
+    <row r="81" spans="3:14" ht="19">
+      <c r="C81" s="129" t="s">
         <v>796</v>
       </c>
-      <c r="D76" s="152"/>
-      <c r="E76" s="152"/>
-      <c r="F76" s="152"/>
-      <c r="G76" s="152"/>
-      <c r="H76" s="152"/>
-      <c r="I76" s="152"/>
-      <c r="J76" s="152"/>
-      <c r="K76" s="152"/>
-      <c r="L76" s="152"/>
-      <c r="M76" s="152"/>
-      <c r="N76" s="152"/>
-    </row>
-    <row r="77" spans="3:14" ht="18">
-      <c r="C77" s="130" t="s">
+      <c r="D81" s="144"/>
+      <c r="E81" s="144"/>
+      <c r="F81" s="144"/>
+      <c r="G81" s="144"/>
+      <c r="H81" s="144"/>
+      <c r="I81" s="144"/>
+      <c r="J81" s="144"/>
+      <c r="K81" s="144"/>
+      <c r="L81" s="144"/>
+      <c r="M81" s="144"/>
+      <c r="N81" s="144"/>
+    </row>
+    <row r="82" spans="3:14" ht="18">
+      <c r="C82" s="127" t="s">
         <v>809</v>
       </c>
-      <c r="D77" s="153"/>
-      <c r="E77" s="153" t="s">
+      <c r="D82" s="145"/>
+      <c r="E82" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="F77" s="153" t="s">
+      <c r="F82" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="G77" s="153" t="s">
+      <c r="G82" s="145" t="s">
         <v>844</v>
       </c>
-      <c r="H77" s="153"/>
-      <c r="I77" s="153" t="s">
+      <c r="H82" s="145"/>
+      <c r="I82" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="J77" s="153" t="s">
+      <c r="J82" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="K77" s="153"/>
-      <c r="L77" s="153"/>
-      <c r="M77" s="153"/>
-      <c r="N77" s="153"/>
-    </row>
-    <row r="78" spans="3:14" ht="18">
-      <c r="C78" s="130" t="s">
+      <c r="K82" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="L82" s="145"/>
+      <c r="M82" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="N82" s="145"/>
+    </row>
+    <row r="83" spans="3:14" ht="18">
+      <c r="C83" s="127" t="s">
         <v>798</v>
       </c>
-      <c r="D78" s="153"/>
-      <c r="E78" s="153" t="s">
+      <c r="D83" s="145"/>
+      <c r="E83" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="F78" s="153" t="s">
+      <c r="F83" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="G78" s="153"/>
-      <c r="H78" s="153"/>
-      <c r="I78" s="153" t="s">
+      <c r="G83" s="145"/>
+      <c r="H83" s="145"/>
+      <c r="I83" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="J78" s="153"/>
-      <c r="K78" s="153"/>
-      <c r="L78" s="153"/>
-      <c r="M78" s="153"/>
-      <c r="N78" s="153"/>
-    </row>
-    <row r="79" spans="3:14" ht="19">
-      <c r="C79" s="130" t="s">
+      <c r="J83" s="145"/>
+      <c r="K83" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="L83" s="145"/>
+      <c r="M83" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="N83" s="145"/>
+    </row>
+    <row r="84" spans="3:14" ht="19">
+      <c r="C84" s="127" t="s">
         <v>813</v>
       </c>
-      <c r="D79" s="153"/>
-      <c r="E79" s="153" t="s">
+      <c r="D84" s="145"/>
+      <c r="E84" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="F79" s="153" t="s">
+      <c r="F84" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="G79" s="153"/>
-      <c r="H79" s="153"/>
-      <c r="I79" s="153" t="s">
+      <c r="G84" s="145"/>
+      <c r="H84" s="145"/>
+      <c r="I84" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="J79" s="153" t="s">
+      <c r="J84" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="K79" s="153"/>
-      <c r="L79" s="153"/>
-      <c r="M79" s="153"/>
-      <c r="N79" s="153"/>
-    </row>
-    <row r="80" spans="3:14" ht="19">
-      <c r="C80" s="130" t="s">
+      <c r="K84" s="145"/>
+      <c r="L84" s="145"/>
+      <c r="M84" s="145" t="s">
+        <v>787</v>
+      </c>
+      <c r="N84" s="145"/>
+    </row>
+    <row r="85" spans="3:14" ht="19">
+      <c r="C85" s="127" t="s">
         <v>814</v>
       </c>
-      <c r="D80" s="153"/>
-      <c r="E80" s="153" t="s">
+      <c r="D85" s="145"/>
+      <c r="E85" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="F80" s="153" t="s">
+      <c r="F85" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="G80" s="153"/>
-      <c r="H80" s="153"/>
-      <c r="I80" s="153"/>
-      <c r="J80" s="153"/>
-      <c r="K80" s="153"/>
-      <c r="L80" s="153"/>
-      <c r="M80" s="153"/>
-      <c r="N80" s="153"/>
-    </row>
-    <row r="81" spans="3:14" ht="18">
-      <c r="C81" s="130" t="s">
+      <c r="G85" s="145"/>
+      <c r="H85" s="145"/>
+      <c r="I85" s="145"/>
+      <c r="J85" s="145"/>
+      <c r="K85" s="145"/>
+      <c r="L85" s="145"/>
+      <c r="M85" s="145"/>
+      <c r="N85" s="145"/>
+    </row>
+    <row r="86" spans="3:14" ht="18">
+      <c r="C86" s="127" t="s">
         <v>815</v>
       </c>
-      <c r="D81" s="153"/>
-      <c r="E81" s="153" t="s">
+      <c r="D86" s="145"/>
+      <c r="E86" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="F81" s="153" t="s">
+      <c r="F86" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="G81" s="153"/>
-      <c r="H81" s="153"/>
-      <c r="I81" s="153"/>
-      <c r="J81" s="153"/>
-      <c r="K81" s="153"/>
-      <c r="L81" s="153"/>
-      <c r="M81" s="153"/>
-      <c r="N81" s="153"/>
-    </row>
-    <row r="82" spans="3:14" ht="18">
-      <c r="C82" s="130" t="s">
+      <c r="G86" s="145"/>
+      <c r="H86" s="145"/>
+      <c r="I86" s="145"/>
+      <c r="J86" s="145"/>
+      <c r="K86" s="145"/>
+      <c r="L86" s="145"/>
+      <c r="M86" s="145"/>
+      <c r="N86" s="145"/>
+    </row>
+    <row r="87" spans="3:14" ht="18">
+      <c r="C87" s="127" t="s">
         <v>807</v>
       </c>
-      <c r="D82" s="153"/>
-      <c r="E82" s="153" t="s">
+      <c r="D87" s="145"/>
+      <c r="E87" s="145" t="s">
         <v>787</v>
       </c>
-      <c r="F82" s="153"/>
-      <c r="G82" s="153"/>
-      <c r="H82" s="153"/>
-      <c r="I82" s="153"/>
-      <c r="J82" s="153"/>
-      <c r="K82" s="153"/>
-      <c r="L82" s="153"/>
-      <c r="M82" s="153"/>
-      <c r="N82" s="153"/>
-    </row>
-    <row r="83" spans="3:14" ht="18">
-      <c r="C83" s="131" t="s">
+      <c r="F87" s="145"/>
+      <c r="G87" s="145"/>
+      <c r="H87" s="145"/>
+      <c r="I87" s="145"/>
+      <c r="J87" s="145"/>
+      <c r="K87" s="145"/>
+      <c r="L87" s="145"/>
+      <c r="M87" s="145"/>
+      <c r="N87" s="145"/>
+    </row>
+    <row r="88" spans="3:14" ht="18">
+      <c r="C88" s="128" t="s">
         <v>802</v>
       </c>
-      <c r="D83" s="154"/>
-      <c r="E83" s="154" t="s">
+      <c r="D88" s="146"/>
+      <c r="E88" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="F83" s="154" t="s">
+      <c r="F88" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="G83" s="154"/>
-      <c r="H83" s="154"/>
-      <c r="I83" s="154"/>
-      <c r="J83" s="154"/>
-      <c r="K83" s="154"/>
-      <c r="L83" s="154"/>
-      <c r="M83" s="154"/>
-      <c r="N83" s="154"/>
-    </row>
-    <row r="84" spans="3:14" ht="18">
-      <c r="C84" s="131" t="s">
+      <c r="G88" s="146"/>
+      <c r="H88" s="146"/>
+      <c r="I88" s="146"/>
+      <c r="J88" s="146"/>
+      <c r="K88" s="146"/>
+      <c r="L88" s="146"/>
+      <c r="M88" s="146"/>
+      <c r="N88" s="146"/>
+    </row>
+    <row r="89" spans="3:14" ht="18">
+      <c r="C89" s="128" t="s">
         <v>820</v>
       </c>
-      <c r="D84" s="154"/>
-      <c r="E84" s="154"/>
-      <c r="F84" s="154"/>
-      <c r="G84" s="154" t="s">
+      <c r="D89" s="146"/>
+      <c r="E89" s="146"/>
+      <c r="F89" s="146"/>
+      <c r="G89" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="H84" s="154"/>
-      <c r="I84" s="154"/>
-      <c r="J84" s="154"/>
-      <c r="K84" s="154"/>
-      <c r="L84" s="154"/>
-      <c r="M84" s="154"/>
-      <c r="N84" s="154"/>
-    </row>
-    <row r="85" spans="3:14" ht="18">
-      <c r="C85" s="131" t="s">
+      <c r="H89" s="146"/>
+      <c r="I89" s="146"/>
+      <c r="J89" s="146"/>
+      <c r="K89" s="146"/>
+      <c r="L89" s="146"/>
+      <c r="M89" s="146"/>
+      <c r="N89" s="146"/>
+    </row>
+    <row r="90" spans="3:14" ht="18">
+      <c r="C90" s="128" t="s">
         <v>822</v>
       </c>
-      <c r="D85" s="154"/>
-      <c r="E85" s="154"/>
-      <c r="F85" s="154"/>
-      <c r="G85" s="154" t="s">
+      <c r="D90" s="146"/>
+      <c r="E90" s="146"/>
+      <c r="F90" s="146"/>
+      <c r="G90" s="146" t="s">
         <v>787</v>
       </c>
-      <c r="H85" s="154"/>
-      <c r="I85" s="154"/>
-      <c r="J85" s="154"/>
-      <c r="K85" s="154"/>
-      <c r="L85" s="154"/>
-      <c r="M85" s="154"/>
-      <c r="N85" s="154"/>
-    </row>
-    <row r="86" spans="3:14" ht="18">
-      <c r="C86" s="131"/>
-      <c r="D86" s="154"/>
-      <c r="E86" s="154"/>
-      <c r="F86" s="154"/>
-      <c r="G86" s="154"/>
-      <c r="H86" s="154"/>
-      <c r="I86" s="154"/>
-      <c r="J86" s="154"/>
-      <c r="K86" s="154"/>
-      <c r="L86" s="154"/>
-      <c r="M86" s="154"/>
-      <c r="N86" s="154"/>
-    </row>
-    <row r="87" spans="3:14" ht="18">
-      <c r="C87" s="131"/>
-      <c r="D87" s="154"/>
-      <c r="E87" s="154"/>
-      <c r="F87" s="154"/>
-      <c r="G87" s="154"/>
-      <c r="H87" s="154"/>
-      <c r="I87" s="154"/>
-      <c r="J87" s="154"/>
-      <c r="K87" s="154"/>
-      <c r="L87" s="154"/>
-      <c r="M87" s="154"/>
-      <c r="N87" s="154"/>
-    </row>
-    <row r="88" spans="3:14" ht="18">
-      <c r="C88" s="131"/>
-      <c r="D88" s="154"/>
-      <c r="E88" s="154"/>
-      <c r="F88" s="154"/>
-      <c r="G88" s="154"/>
-      <c r="H88" s="154"/>
-      <c r="I88" s="154"/>
-      <c r="J88" s="154"/>
-      <c r="K88" s="154"/>
-      <c r="L88" s="154"/>
-      <c r="M88" s="154"/>
-      <c r="N88" s="154"/>
-    </row>
-    <row r="89" spans="3:14" ht="18">
-      <c r="C89" s="131"/>
-      <c r="D89" s="154"/>
-      <c r="E89" s="154"/>
-      <c r="F89" s="154"/>
-      <c r="G89" s="154"/>
-      <c r="H89" s="154"/>
-      <c r="I89" s="154"/>
-      <c r="J89" s="154"/>
-      <c r="K89" s="154"/>
-      <c r="L89" s="154"/>
-      <c r="M89" s="154"/>
-      <c r="N89" s="154"/>
-    </row>
-    <row r="90" spans="3:14" ht="18">
-      <c r="C90" s="131"/>
-      <c r="D90" s="154"/>
-      <c r="E90" s="154"/>
-      <c r="F90" s="154"/>
-      <c r="G90" s="154"/>
-      <c r="H90" s="154"/>
-      <c r="I90" s="154"/>
-      <c r="J90" s="154"/>
-      <c r="K90" s="154"/>
-      <c r="L90" s="154"/>
-      <c r="M90" s="154"/>
-      <c r="N90" s="154"/>
-    </row>
-    <row r="91" spans="3:14" ht="18">
-      <c r="C91" s="131"/>
-      <c r="D91" s="154"/>
-      <c r="E91" s="154"/>
-      <c r="F91" s="154"/>
-      <c r="G91" s="154"/>
-      <c r="H91" s="154"/>
-      <c r="I91" s="154"/>
-      <c r="J91" s="154"/>
-      <c r="K91" s="154"/>
-      <c r="L91" s="154"/>
-      <c r="M91" s="154"/>
-      <c r="N91" s="154"/>
-    </row>
-    <row r="92" spans="3:14" ht="18">
-      <c r="C92" s="131"/>
-      <c r="D92" s="154"/>
-      <c r="E92" s="154"/>
-      <c r="F92" s="154"/>
-      <c r="G92" s="154"/>
-      <c r="H92" s="154"/>
-      <c r="I92" s="154"/>
-      <c r="J92" s="154"/>
-      <c r="K92" s="154"/>
-      <c r="L92" s="154"/>
-      <c r="M92" s="154"/>
-      <c r="N92" s="154"/>
-    </row>
-    <row r="93" spans="3:14" ht="19" thickBot="1">
-      <c r="C93" s="131"/>
-      <c r="D93" s="154"/>
-      <c r="E93" s="154"/>
-      <c r="F93" s="154"/>
-      <c r="G93" s="154"/>
-      <c r="H93" s="154"/>
-      <c r="I93" s="154"/>
-      <c r="J93" s="154"/>
-      <c r="K93" s="154"/>
-      <c r="L93" s="154"/>
-      <c r="M93" s="154"/>
-      <c r="N93" s="154"/>
-    </row>
-    <row r="94" spans="3:14" ht="17" thickBot="1">
-      <c r="C94" s="121"/>
-      <c r="D94" s="123"/>
-      <c r="E94" s="123"/>
-      <c r="F94" s="123"/>
-      <c r="G94" s="123"/>
-      <c r="H94" s="123"/>
-      <c r="I94" s="123"/>
-      <c r="J94" s="123"/>
-      <c r="K94" s="123"/>
-      <c r="L94" s="123"/>
-      <c r="M94" s="123"/>
-      <c r="N94" s="124"/>
+      <c r="H90" s="146"/>
+      <c r="I90" s="146"/>
+      <c r="J90" s="146"/>
+      <c r="K90" s="146"/>
+      <c r="L90" s="146"/>
+      <c r="M90" s="146"/>
+      <c r="N90" s="146"/>
+    </row>
+    <row r="91" spans="3:14" ht="19">
+      <c r="C91" s="128" t="s">
+        <v>866</v>
+      </c>
+      <c r="D91" s="146"/>
+      <c r="E91" s="146"/>
+      <c r="F91" s="146"/>
+      <c r="G91" s="146"/>
+      <c r="H91" s="146"/>
+      <c r="I91" s="146"/>
+      <c r="J91" s="146"/>
+      <c r="K91" s="146" t="s">
+        <v>787</v>
+      </c>
+      <c r="L91" s="146"/>
+      <c r="M91" s="146"/>
+      <c r="N91" s="146"/>
+    </row>
+    <row r="92" spans="3:14" ht="19">
+      <c r="C92" s="128" t="s">
+        <v>867</v>
+      </c>
+      <c r="D92" s="146"/>
+      <c r="E92" s="146"/>
+      <c r="F92" s="146"/>
+      <c r="G92" s="146"/>
+      <c r="H92" s="146"/>
+      <c r="I92" s="146"/>
+      <c r="J92" s="146"/>
+      <c r="K92" s="146" t="s">
+        <v>787</v>
+      </c>
+      <c r="L92" s="146"/>
+      <c r="M92" s="146"/>
+      <c r="N92" s="146"/>
+    </row>
+    <row r="93" spans="3:14" ht="18">
+      <c r="C93" s="128"/>
+      <c r="D93" s="146"/>
+      <c r="E93" s="146"/>
+      <c r="F93" s="146"/>
+      <c r="G93" s="146"/>
+      <c r="H93" s="146"/>
+      <c r="I93" s="146"/>
+      <c r="J93" s="146"/>
+      <c r="K93" s="146"/>
+      <c r="L93" s="146"/>
+      <c r="M93" s="146"/>
+      <c r="N93" s="146"/>
+    </row>
+    <row r="94" spans="3:14" ht="18">
+      <c r="C94" s="128"/>
+      <c r="D94" s="146"/>
+      <c r="E94" s="146"/>
+      <c r="F94" s="146"/>
+      <c r="G94" s="146"/>
+      <c r="H94" s="146"/>
+      <c r="I94" s="146"/>
+      <c r="J94" s="146"/>
+      <c r="K94" s="146"/>
+      <c r="L94" s="146"/>
+      <c r="M94" s="146"/>
+      <c r="N94" s="146"/>
     </row>
     <row r="95" spans="3:14" ht="18">
-      <c r="C95" s="136" t="s">
+      <c r="C95" s="128"/>
+      <c r="D95" s="146"/>
+      <c r="E95" s="146"/>
+      <c r="F95" s="146"/>
+      <c r="G95" s="146"/>
+      <c r="H95" s="146"/>
+      <c r="I95" s="146"/>
+      <c r="J95" s="146"/>
+      <c r="K95" s="146"/>
+      <c r="L95" s="146"/>
+      <c r="M95" s="146"/>
+      <c r="N95" s="146"/>
+    </row>
+    <row r="96" spans="3:14" ht="18">
+      <c r="C96" s="128"/>
+      <c r="D96" s="146"/>
+      <c r="E96" s="146"/>
+      <c r="F96" s="146"/>
+      <c r="G96" s="146"/>
+      <c r="H96" s="146"/>
+      <c r="I96" s="146"/>
+      <c r="J96" s="146"/>
+      <c r="K96" s="146"/>
+      <c r="L96" s="146"/>
+      <c r="M96" s="146"/>
+      <c r="N96" s="146"/>
+    </row>
+    <row r="97" spans="3:14" ht="18">
+      <c r="C97" s="128"/>
+      <c r="D97" s="146"/>
+      <c r="E97" s="146"/>
+      <c r="F97" s="146"/>
+      <c r="G97" s="146"/>
+      <c r="H97" s="146"/>
+      <c r="I97" s="146"/>
+      <c r="J97" s="146"/>
+      <c r="K97" s="146"/>
+      <c r="L97" s="146"/>
+      <c r="M97" s="146"/>
+      <c r="N97" s="146"/>
+    </row>
+    <row r="98" spans="3:14" ht="19" thickBot="1">
+      <c r="C98" s="128"/>
+      <c r="D98" s="146"/>
+      <c r="E98" s="146"/>
+      <c r="F98" s="146"/>
+      <c r="G98" s="146"/>
+      <c r="H98" s="146"/>
+      <c r="I98" s="146"/>
+      <c r="J98" s="146"/>
+      <c r="K98" s="146"/>
+      <c r="L98" s="146"/>
+      <c r="M98" s="146"/>
+      <c r="N98" s="146"/>
+    </row>
+    <row r="99" spans="3:14" ht="17" thickBot="1">
+      <c r="C99" s="119"/>
+      <c r="D99" s="121"/>
+      <c r="E99" s="121"/>
+      <c r="F99" s="121"/>
+      <c r="G99" s="121"/>
+      <c r="H99" s="121"/>
+      <c r="I99" s="121"/>
+      <c r="J99" s="121"/>
+      <c r="K99" s="121"/>
+      <c r="L99" s="121"/>
+      <c r="M99" s="121"/>
+      <c r="N99" s="122"/>
+    </row>
+    <row r="100" spans="3:14" ht="18">
+      <c r="C100" s="133" t="s">
         <v>816</v>
       </c>
-      <c r="D95" s="155"/>
-      <c r="E95" s="155"/>
-      <c r="F95" s="155"/>
-      <c r="G95" s="155"/>
-      <c r="H95" s="155"/>
-      <c r="I95" s="155"/>
-      <c r="J95" s="155"/>
-      <c r="K95" s="155"/>
-      <c r="L95" s="155"/>
-      <c r="M95" s="155"/>
-      <c r="N95" s="155"/>
-    </row>
-    <row r="96" spans="3:14" ht="19">
-      <c r="C96" s="133" t="s">
+      <c r="D100" s="147"/>
+      <c r="E100" s="147"/>
+      <c r="F100" s="147"/>
+      <c r="G100" s="147"/>
+      <c r="H100" s="147"/>
+      <c r="I100" s="147"/>
+      <c r="J100" s="147"/>
+      <c r="K100" s="147"/>
+      <c r="L100" s="147"/>
+      <c r="M100" s="147"/>
+      <c r="N100" s="147"/>
+    </row>
+    <row r="101" spans="3:14" ht="19">
+      <c r="C101" s="130" t="s">
         <v>817</v>
       </c>
-      <c r="D96" s="156"/>
-      <c r="E96" s="156" t="s">
+      <c r="D101" s="148"/>
+      <c r="E101" s="148" t="s">
         <v>787</v>
       </c>
-      <c r="F96" s="156"/>
-      <c r="G96" s="156"/>
-      <c r="H96" s="156"/>
-      <c r="I96" s="156"/>
-      <c r="J96" s="156"/>
-      <c r="K96" s="156"/>
-      <c r="L96" s="156"/>
-      <c r="M96" s="156"/>
-      <c r="N96" s="156"/>
-    </row>
-    <row r="97" spans="3:14" ht="18">
-      <c r="C97" s="133"/>
-      <c r="D97" s="156"/>
-      <c r="E97" s="156"/>
-      <c r="F97" s="156"/>
-      <c r="G97" s="156"/>
-      <c r="H97" s="156"/>
-      <c r="I97" s="156"/>
-      <c r="J97" s="156"/>
-      <c r="K97" s="156"/>
-      <c r="L97" s="156"/>
-      <c r="M97" s="156"/>
-      <c r="N97" s="156"/>
-    </row>
-    <row r="98" spans="3:14" ht="18">
-      <c r="C98" s="133"/>
-      <c r="D98" s="156"/>
-      <c r="E98" s="156"/>
-      <c r="F98" s="156"/>
-      <c r="G98" s="156"/>
-      <c r="H98" s="156"/>
-      <c r="I98" s="156"/>
-      <c r="J98" s="156"/>
-      <c r="K98" s="156"/>
-      <c r="L98" s="156"/>
-      <c r="M98" s="156"/>
-      <c r="N98" s="156"/>
-    </row>
-    <row r="99" spans="3:14" ht="18">
-      <c r="C99" s="133"/>
-      <c r="D99" s="156"/>
-      <c r="E99" s="156"/>
-      <c r="F99" s="156"/>
-      <c r="G99" s="156"/>
-      <c r="H99" s="156"/>
-      <c r="I99" s="156"/>
-      <c r="J99" s="156"/>
-      <c r="K99" s="156"/>
-      <c r="L99" s="156"/>
-      <c r="M99" s="156"/>
-      <c r="N99" s="156"/>
-    </row>
-    <row r="100" spans="3:14">
-      <c r="C100" s="134"/>
-      <c r="D100" s="157"/>
-      <c r="E100" s="157"/>
-      <c r="F100" s="157"/>
-      <c r="G100" s="157"/>
-      <c r="H100" s="157"/>
-      <c r="I100" s="157"/>
-      <c r="J100" s="157"/>
-      <c r="K100" s="157"/>
-      <c r="L100" s="157"/>
-      <c r="M100" s="157"/>
-      <c r="N100" s="157"/>
-    </row>
-    <row r="101" spans="3:14" ht="17" thickBot="1">
-      <c r="C101" s="135"/>
-      <c r="D101" s="158"/>
-      <c r="E101" s="158"/>
-      <c r="F101" s="158"/>
-      <c r="G101" s="158"/>
-      <c r="H101" s="158"/>
-      <c r="I101" s="158"/>
-      <c r="J101" s="158"/>
-      <c r="K101" s="158"/>
-      <c r="L101" s="158"/>
-      <c r="M101" s="158"/>
-      <c r="N101" s="158"/>
-    </row>
-    <row r="102" spans="3:14" ht="17" thickBot="1">
-      <c r="C102" s="170"/>
-      <c r="D102" s="175"/>
-      <c r="E102" s="174"/>
-      <c r="F102" s="110"/>
-      <c r="G102" s="110"/>
-      <c r="H102" s="110"/>
-      <c r="I102" s="110"/>
-      <c r="J102" s="110"/>
-      <c r="K102" s="110"/>
-      <c r="L102" s="110"/>
-      <c r="M102" s="110"/>
-      <c r="N102" s="125"/>
+      <c r="F101" s="148"/>
+      <c r="G101" s="148"/>
+      <c r="H101" s="148"/>
+      <c r="I101" s="148"/>
+      <c r="J101" s="148"/>
+      <c r="K101" s="148"/>
+      <c r="L101" s="148"/>
+      <c r="M101" s="148"/>
+      <c r="N101" s="148"/>
+    </row>
+    <row r="102" spans="3:14" ht="18">
+      <c r="C102" s="130"/>
+      <c r="D102" s="148"/>
+      <c r="E102" s="148"/>
+      <c r="F102" s="148"/>
+      <c r="G102" s="148"/>
+      <c r="H102" s="148"/>
+      <c r="I102" s="148"/>
+      <c r="J102" s="148"/>
+      <c r="K102" s="148"/>
+      <c r="L102" s="148"/>
+      <c r="M102" s="148"/>
+      <c r="N102" s="148"/>
     </row>
     <row r="103" spans="3:14" ht="18">
-      <c r="C103" s="171" t="s">
+      <c r="C103" s="130"/>
+      <c r="D103" s="148"/>
+      <c r="E103" s="148"/>
+      <c r="F103" s="148"/>
+      <c r="G103" s="148"/>
+      <c r="H103" s="148"/>
+      <c r="I103" s="148"/>
+      <c r="J103" s="148"/>
+      <c r="K103" s="148"/>
+      <c r="L103" s="148"/>
+      <c r="M103" s="148"/>
+      <c r="N103" s="148"/>
+    </row>
+    <row r="104" spans="3:14" ht="18">
+      <c r="C104" s="130"/>
+      <c r="D104" s="148"/>
+      <c r="E104" s="148"/>
+      <c r="F104" s="148"/>
+      <c r="G104" s="148"/>
+      <c r="H104" s="148"/>
+      <c r="I104" s="148"/>
+      <c r="J104" s="148"/>
+      <c r="K104" s="148"/>
+      <c r="L104" s="148"/>
+      <c r="M104" s="148"/>
+      <c r="N104" s="148"/>
+    </row>
+    <row r="105" spans="3:14">
+      <c r="C105" s="131"/>
+      <c r="D105" s="149"/>
+      <c r="E105" s="149"/>
+      <c r="F105" s="149"/>
+      <c r="G105" s="149"/>
+      <c r="H105" s="149"/>
+      <c r="I105" s="149"/>
+      <c r="J105" s="149"/>
+      <c r="K105" s="149"/>
+      <c r="L105" s="149"/>
+      <c r="M105" s="149"/>
+      <c r="N105" s="149"/>
+    </row>
+    <row r="106" spans="3:14" ht="17" thickBot="1">
+      <c r="C106" s="132"/>
+      <c r="D106" s="150"/>
+      <c r="E106" s="150"/>
+      <c r="F106" s="150"/>
+      <c r="G106" s="150"/>
+      <c r="H106" s="150"/>
+      <c r="I106" s="150"/>
+      <c r="J106" s="150"/>
+      <c r="K106" s="150"/>
+      <c r="L106" s="150"/>
+      <c r="M106" s="150"/>
+      <c r="N106" s="150"/>
+    </row>
+    <row r="107" spans="3:14" ht="17" thickBot="1">
+      <c r="C107" s="162"/>
+      <c r="D107" s="167"/>
+      <c r="E107" s="166"/>
+      <c r="F107" s="110"/>
+      <c r="G107" s="110"/>
+      <c r="H107" s="110"/>
+      <c r="I107" s="110"/>
+      <c r="J107" s="110"/>
+      <c r="K107" s="110"/>
+      <c r="L107" s="110"/>
+      <c r="M107" s="110"/>
+      <c r="N107" s="123"/>
+    </row>
+    <row r="108" spans="3:14" ht="18">
+      <c r="C108" s="163" t="s">
         <v>818</v>
       </c>
-      <c r="D103" s="159"/>
-      <c r="E103" s="159"/>
-      <c r="F103" s="159"/>
-      <c r="G103" s="159"/>
-      <c r="H103" s="159"/>
-      <c r="I103" s="159"/>
-      <c r="J103" s="159"/>
-      <c r="K103" s="159"/>
-      <c r="L103" s="159"/>
-      <c r="M103" s="162"/>
-      <c r="N103" s="159"/>
-    </row>
-    <row r="104" spans="3:14" ht="18">
-      <c r="C104" s="172" t="s">
+      <c r="D108" s="151"/>
+      <c r="E108" s="151"/>
+      <c r="F108" s="151"/>
+      <c r="G108" s="151"/>
+      <c r="H108" s="151"/>
+      <c r="I108" s="151"/>
+      <c r="J108" s="151"/>
+      <c r="K108" s="151"/>
+      <c r="L108" s="151"/>
+      <c r="M108" s="154"/>
+      <c r="N108" s="151"/>
+    </row>
+    <row r="109" spans="3:14" ht="18">
+      <c r="C109" s="164" t="s">
         <v>839</v>
       </c>
-      <c r="D104" s="176"/>
-      <c r="E104" s="177" t="s">
+      <c r="D109" s="168"/>
+      <c r="E109" s="169" t="s">
         <v>787</v>
       </c>
-      <c r="F104" s="177" t="s">
+      <c r="F109" s="169" t="s">
         <v>787</v>
       </c>
-      <c r="G104" s="176"/>
-      <c r="H104" s="177"/>
-      <c r="I104" s="176"/>
-      <c r="J104" s="176"/>
-      <c r="K104" s="176"/>
-      <c r="L104" s="176"/>
-      <c r="M104" s="168"/>
-      <c r="N104" s="166"/>
-    </row>
-    <row r="105" spans="3:14" ht="18">
-      <c r="C105" s="172" t="s">
+      <c r="G109" s="168"/>
+      <c r="H109" s="169"/>
+      <c r="I109" s="168"/>
+      <c r="J109" s="168"/>
+      <c r="K109" s="168"/>
+      <c r="L109" s="168"/>
+      <c r="M109" s="160"/>
+      <c r="N109" s="158"/>
+    </row>
+    <row r="110" spans="3:14" ht="18">
+      <c r="C110" s="164" t="s">
         <v>819</v>
       </c>
-      <c r="D105" s="177"/>
-      <c r="E105" s="177" t="s">
+      <c r="D110" s="169"/>
+      <c r="E110" s="169" t="s">
         <v>787</v>
       </c>
-      <c r="F105" s="177" t="s">
+      <c r="F110" s="169" t="s">
         <v>787</v>
       </c>
-      <c r="G105" s="177"/>
-      <c r="H105" s="177"/>
-      <c r="I105" s="177"/>
-      <c r="J105" s="177"/>
-      <c r="K105" s="177"/>
-      <c r="L105" s="177"/>
-      <c r="M105" s="169"/>
-      <c r="N105" s="167"/>
-    </row>
-    <row r="106" spans="3:14" ht="18">
-      <c r="C106" s="165"/>
-      <c r="D106" s="177"/>
-      <c r="E106" s="177"/>
-      <c r="F106" s="177"/>
-      <c r="G106" s="177"/>
-      <c r="H106" s="177"/>
-      <c r="I106" s="177"/>
-      <c r="J106" s="177"/>
-      <c r="K106" s="177"/>
-      <c r="L106" s="177"/>
-      <c r="M106" s="169"/>
-      <c r="N106" s="167"/>
-    </row>
-    <row r="107" spans="3:14" ht="18">
-      <c r="C107" s="165"/>
-      <c r="D107" s="177"/>
-      <c r="E107" s="177"/>
-      <c r="F107" s="177"/>
-      <c r="G107" s="177"/>
-      <c r="H107" s="177"/>
-      <c r="I107" s="177"/>
-      <c r="J107" s="177"/>
-      <c r="K107" s="177"/>
-      <c r="L107" s="177"/>
-      <c r="M107" s="169"/>
-      <c r="N107" s="167"/>
-    </row>
-    <row r="108" spans="3:14" ht="18">
-      <c r="C108" s="165"/>
-      <c r="D108" s="177"/>
-      <c r="E108" s="177"/>
-      <c r="F108" s="177"/>
-      <c r="G108" s="177"/>
-      <c r="H108" s="177"/>
-      <c r="I108" s="177"/>
-      <c r="J108" s="177"/>
-      <c r="K108" s="177"/>
-      <c r="L108" s="177"/>
-      <c r="M108" s="169"/>
-      <c r="N108" s="167"/>
-    </row>
-    <row r="109" spans="3:14" ht="18">
-      <c r="C109" s="172"/>
-      <c r="D109" s="160"/>
-      <c r="E109" s="160"/>
-      <c r="F109" s="160"/>
-      <c r="G109" s="160"/>
-      <c r="H109" s="160"/>
-      <c r="I109" s="160"/>
-      <c r="J109" s="160"/>
-      <c r="K109" s="160"/>
-      <c r="L109" s="160"/>
-      <c r="M109" s="163"/>
-      <c r="N109" s="160"/>
-    </row>
-    <row r="110" spans="3:14" ht="19" thickBot="1">
-      <c r="C110" s="173"/>
-      <c r="D110" s="161"/>
-      <c r="E110" s="161"/>
-      <c r="F110" s="161"/>
-      <c r="G110" s="161"/>
-      <c r="H110" s="161"/>
-      <c r="I110" s="161"/>
-      <c r="J110" s="161"/>
-      <c r="K110" s="161"/>
-      <c r="L110" s="161"/>
-      <c r="M110" s="164"/>
-      <c r="N110" s="161"/>
+      <c r="G110" s="169"/>
+      <c r="H110" s="169"/>
+      <c r="I110" s="169"/>
+      <c r="J110" s="169"/>
+      <c r="K110" s="169"/>
+      <c r="L110" s="169"/>
+      <c r="M110" s="161"/>
+      <c r="N110" s="159"/>
+    </row>
+    <row r="111" spans="3:14" ht="18">
+      <c r="C111" s="157"/>
+      <c r="D111" s="169"/>
+      <c r="E111" s="169"/>
+      <c r="F111" s="169"/>
+      <c r="G111" s="169"/>
+      <c r="H111" s="169"/>
+      <c r="I111" s="169"/>
+      <c r="J111" s="169"/>
+      <c r="K111" s="169"/>
+      <c r="L111" s="169"/>
+      <c r="M111" s="161"/>
+      <c r="N111" s="159"/>
+    </row>
+    <row r="112" spans="3:14" ht="18">
+      <c r="C112" s="157"/>
+      <c r="D112" s="169"/>
+      <c r="E112" s="169"/>
+      <c r="F112" s="169"/>
+      <c r="G112" s="169"/>
+      <c r="H112" s="169"/>
+      <c r="I112" s="169"/>
+      <c r="J112" s="169"/>
+      <c r="K112" s="169"/>
+      <c r="L112" s="169"/>
+      <c r="M112" s="161"/>
+      <c r="N112" s="159"/>
+    </row>
+    <row r="113" spans="3:14" ht="18">
+      <c r="C113" s="157"/>
+      <c r="D113" s="169"/>
+      <c r="E113" s="169"/>
+      <c r="F113" s="169"/>
+      <c r="G113" s="169"/>
+      <c r="H113" s="169"/>
+      <c r="I113" s="169"/>
+      <c r="J113" s="169"/>
+      <c r="K113" s="169"/>
+      <c r="L113" s="169"/>
+      <c r="M113" s="161"/>
+      <c r="N113" s="159"/>
+    </row>
+    <row r="114" spans="3:14" ht="18">
+      <c r="C114" s="164"/>
+      <c r="D114" s="152"/>
+      <c r="E114" s="152"/>
+      <c r="F114" s="152"/>
+      <c r="G114" s="152"/>
+      <c r="H114" s="152"/>
+      <c r="I114" s="152"/>
+      <c r="J114" s="152"/>
+      <c r="K114" s="152"/>
+      <c r="L114" s="152"/>
+      <c r="M114" s="155"/>
+      <c r="N114" s="152"/>
+    </row>
+    <row r="115" spans="3:14" ht="19" thickBot="1">
+      <c r="C115" s="165"/>
+      <c r="D115" s="153"/>
+      <c r="E115" s="153"/>
+      <c r="F115" s="153"/>
+      <c r="G115" s="153"/>
+      <c r="H115" s="153"/>
+      <c r="I115" s="153"/>
+      <c r="J115" s="153"/>
+      <c r="K115" s="153"/>
+      <c r="L115" s="153"/>
+      <c r="M115" s="156"/>
+      <c r="N115" s="153"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C28" r:id="rId1" location="remove-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - remove-int-" xr:uid="{A3DFFAF1-3C93-B04D-A4B1-EA2A39FBEC91}"/>
-    <hyperlink ref="C78" r:id="rId2" location="isEmpty--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - isEmpty--" xr:uid="{F593362D-789B-7049-A3AA-7B6E2682E976}"/>
+    <hyperlink ref="C83" r:id="rId2" location="isEmpty--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - isEmpty--" xr:uid="{F593362D-789B-7049-A3AA-7B6E2682E976}"/>
     <hyperlink ref="C31" r:id="rId3" location="removeRange-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - removeRange-int-int-" xr:uid="{D0BFE38E-2B8B-CE41-967A-C3C9EA93BE4E}"/>
     <hyperlink ref="C34" r:id="rId4" location="clear--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - clear--" xr:uid="{2FFA909C-C109-B14D-8F33-325805174D8D}"/>
     <hyperlink ref="C47" r:id="rId5" location="get-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - get-int-" xr:uid="{FBBAAF6B-E143-864D-A6C3-F1E24E50E661}"/>
     <hyperlink ref="C48" r:id="rId6" location="iterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - iterator--" xr:uid="{A075F592-CC84-B840-8050-836C5620A000}"/>
     <hyperlink ref="C49" r:id="rId7" location="listIterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - listIterator--" xr:uid="{F4F1EE1C-1937-BB49-B4F9-158A67374360}"/>
     <hyperlink ref="C50" r:id="rId8" location="spliterator--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - spliterator--" xr:uid="{ECABA72C-AD77-1C4F-B3FC-B32A74B26EC8}"/>
-    <hyperlink ref="C82" r:id="rId9" location="subList-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - subList-int-int-" xr:uid="{1EB080CA-5D98-3844-A4A2-E79CA8CD8EBB}"/>
-    <hyperlink ref="C77" r:id="rId10" location="size--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - size--" xr:uid="{D71DFD34-DFF3-DA45-BA53-9457F025CBE6}"/>
-    <hyperlink ref="C104" r:id="rId11" tooltip="class in java.lang" display="https://docs.oracle.com/javase/8/docs/api/java/lang/Object.html" xr:uid="{80E00372-253A-5E46-B2A9-FAFBDA183C46}"/>
+    <hyperlink ref="C87" r:id="rId9" location="subList-int-int-" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - subList-int-int-" xr:uid="{1EB080CA-5D98-3844-A4A2-E79CA8CD8EBB}"/>
+    <hyperlink ref="C82" r:id="rId10" location="size--" display="https://docs.oracle.com/javase/8/docs/api/java/util/ArrayList.html - size--" xr:uid="{D71DFD34-DFF3-DA45-BA53-9457F025CBE6}"/>
+    <hyperlink ref="C109" r:id="rId11" tooltip="class in java.lang" display="https://docs.oracle.com/javase/8/docs/api/java/lang/Object.html" xr:uid="{80E00372-253A-5E46-B2A9-FAFBDA183C46}"/>
     <hyperlink ref="C52" r:id="rId12" location="getFirst()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - getFirst()" xr:uid="{8BDAB115-0121-3940-B451-BF302CE8770F}"/>
     <hyperlink ref="C53" r:id="rId13" location="getLast()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - getLast()" xr:uid="{8393D593-5133-A241-BE7A-9F172C52B66B}"/>
     <hyperlink ref="C54" r:id="rId14" location="peek()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - peek()" xr:uid="{0CEF2AF3-6D6C-9046-BE93-019C40035281}"/>
@@ -32150,8 +33097,10 @@
     <hyperlink ref="C35" r:id="rId17" location="poll()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - poll()" xr:uid="{8242EE68-D381-0941-87E8-C08B2EFCDCE1}"/>
     <hyperlink ref="C40" r:id="rId18" location="removeFirst()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - removeFirst()" xr:uid="{59C4D3D0-5891-744A-BA52-0FE35B2643B4}"/>
     <hyperlink ref="C41" r:id="rId19" location="removeLast()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - removeLast()" xr:uid="{DC2BE068-F09F-2443-B88D-91E77B963F1D}"/>
-    <hyperlink ref="C85" r:id="rId20" tooltip="class in java.lang" display="https://docs.oracle.com/javase/7/docs/api/java/lang/Object.html" xr:uid="{AFDBA6F5-E5D2-A442-8152-52E12532F525}"/>
+    <hyperlink ref="C90" r:id="rId20" tooltip="class in java.lang" display="https://docs.oracle.com/javase/7/docs/api/java/lang/Object.html" xr:uid="{AFDBA6F5-E5D2-A442-8152-52E12532F525}"/>
     <hyperlink ref="C38" r:id="rId21" location="pop()" display="https://docs.oracle.com/javase/7/docs/api/java/util/LinkedList.html - pop()" xr:uid="{ECBDC240-CEB4-A74E-8A39-3B4C3D4E658E}"/>
+    <hyperlink ref="C57" r:id="rId22" location="entrySet--" display="https://docs.oracle.com/javase/8/docs/api/java/util/HashMap.html - entrySet--" xr:uid="{F0217C40-A9C2-9F45-AB45-AB5F14305F82}"/>
+    <hyperlink ref="C58" r:id="rId23" location="entrySet--" display="https://docs.oracle.com/javase/8/docs/api/java/util/HashMap.html - entrySet--" xr:uid="{188ECD26-DD32-2946-892F-C58CD52C340F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>